<commit_message>
Updated the stats after last release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D59C8CF-281A-6B47-A552-AA696CB93015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0F62E4-3D73-8444-A61A-363B0C6ACF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24480" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -206,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R2" totalsRowShown="0">
-  <autoFilter ref="A1:R2" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R3" totalsRowShown="0">
+  <autoFilter ref="A1:R3" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="16"/>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,34 +621,34 @@
         <v>101</v>
       </c>
       <c r="C2" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D2" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E2" s="2">
-        <v>4344</v>
+        <v>4368</v>
       </c>
       <c r="F2" s="2">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="G2" s="2">
-        <v>3182</v>
+        <v>3195</v>
       </c>
       <c r="H2" s="2">
-        <v>57340</v>
+        <v>57442</v>
       </c>
       <c r="I2" s="2">
-        <v>40586</v>
+        <v>40634</v>
       </c>
       <c r="J2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
       </c>
       <c r="L2" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M2" s="2">
         <v>0</v>
@@ -660,14 +660,34 @@
         <v>125</v>
       </c>
       <c r="P2" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q2" s="2">
         <v>2</v>
       </c>
       <c r="R2" s="2">
-        <v>537</v>
-      </c>
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added the reason for a timeout to the error message
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC94EF9A-7A0F-124F-A07D-1CF93144E22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F5241-53F4-E24D-A02B-975C24F75ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24480" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24560" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -206,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R4" totalsRowShown="0">
-  <autoFilter ref="A1:R4" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R5" totalsRowShown="0">
+  <autoFilter ref="A1:R5" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="16"/>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,24 +726,116 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="A4" s="1">
+        <v>44580</v>
+      </c>
+      <c r="B4" s="2">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2">
+        <v>224</v>
+      </c>
+      <c r="D4" s="2">
+        <v>177</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4368</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1525</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3197</v>
+      </c>
+      <c r="H4" s="2">
+        <v>57422</v>
+      </c>
+      <c r="I4" s="2">
+        <v>40634</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>203</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>135</v>
+      </c>
+      <c r="O4" s="2">
+        <v>125</v>
+      </c>
+      <c r="P4" s="2">
+        <v>122</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44588</v>
+      </c>
+      <c r="B5" s="2">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2">
+        <v>224</v>
+      </c>
+      <c r="D5" s="2">
+        <v>177</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4368</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1531</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3207</v>
+      </c>
+      <c r="H5" s="2">
+        <v>57794</v>
+      </c>
+      <c r="I5" s="2">
+        <v>40652</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>203</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>135</v>
+      </c>
+      <c r="O5" s="2">
+        <v>125</v>
+      </c>
+      <c r="P5" s="2">
+        <v>122</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>3</v>
+      </c>
+      <c r="R5" s="2">
+        <v>550</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
do not set the default timeout if ${TIMEOUT} is already set
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F5241-53F4-E24D-A02B-975C24F75ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E51A684-6124-E74E-944B-6B37DF04E2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24560" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="12200" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -206,8 +206,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R5" totalsRowShown="0">
-  <autoFilter ref="A1:R5" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:R7" totalsRowShown="0">
+  <autoFilter ref="A1:R7" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="16"/>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,6 +837,82 @@
         <v>550</v>
       </c>
     </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B6" s="2">
+        <v>102</v>
+      </c>
+      <c r="C6" s="2">
+        <v>224</v>
+      </c>
+      <c r="D6" s="2">
+        <v>177</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4379</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1539</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3224</v>
+      </c>
+      <c r="H6" s="2">
+        <v>57859</v>
+      </c>
+      <c r="I6" s="2">
+        <v>40677</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>203</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>135</v>
+      </c>
+      <c r="O6" s="2">
+        <v>125</v>
+      </c>
+      <c r="P6" s="2">
+        <v>122</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>3</v>
+      </c>
+      <c r="R6" s="2">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed a bug in the host completio
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DD36D-6398-0C40-857C-6426DFF4E577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA972AF-28B9-5541-BD05-EA785D7E71B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31960" windowHeight="34240" activeTab="4" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="13520" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -270,10 +270,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -306,16 +306,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$12</c:f>
+              <c:f>Data!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -348,6 +351,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4434</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4454</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,10 +393,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -423,16 +429,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$12</c:f>
+              <c:f>Data!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -465,6 +474,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -504,10 +516,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -540,16 +552,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$12</c:f>
+              <c:f>Data!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -582,6 +597,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,10 +855,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -873,16 +891,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$K$2:$K$12</c:f>
+              <c:f>Data!$K$2:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -914,6 +935,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -954,10 +978,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -990,16 +1014,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$12</c:f>
+              <c:f>Data!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1031,6 +1058,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1071,10 +1101,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1107,16 +1137,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$J$2:$J$12</c:f>
+              <c:f>Data!$J$2:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1148,6 +1181,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1407,10 +1443,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1443,16 +1479,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$12</c:f>
+              <c:f>Data!$M$2:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -1484,6 +1523,9 @@
                   <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>215</c:v>
                 </c:pt>
               </c:numCache>
@@ -1524,10 +1566,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1560,16 +1602,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$12</c:f>
+              <c:f>Data!$P$2:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -1601,6 +1646,9 @@
                   <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>148</c:v>
                 </c:pt>
               </c:numCache>
@@ -1857,10 +1905,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1893,16 +1941,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$12</c:f>
+              <c:f>Data!$R$2:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -1934,6 +1985,9 @@
                   <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
@@ -4350,7 +4404,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B111F3D3-9A19-164A-A80F-5E41AF9CF1E4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="172" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4490,8 +4544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:T12" totalsRowShown="0">
-  <autoFilter ref="A1:T12" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:T13" totalsRowShown="0">
+  <autoFilter ref="A1:T13" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="18"/>
@@ -4819,10 +4873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5615,6 +5669,70 @@
         <v>669</v>
       </c>
     </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44664</v>
+      </c>
+      <c r="B13" s="2">
+        <v>102</v>
+      </c>
+      <c r="C13" s="2">
+        <v>230</v>
+      </c>
+      <c r="D13" s="2">
+        <v>183</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4454</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1637</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3406</v>
+      </c>
+      <c r="H13" s="2">
+        <v>60308</v>
+      </c>
+      <c r="I13" s="2">
+        <v>42743</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>214</v>
+      </c>
+      <c r="M13" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>215</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>148</v>
+      </c>
+      <c r="P13" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>148</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>128</v>
+      </c>
+      <c r="R13" s="2">
+        <v>131</v>
+      </c>
+      <c r="S13" s="2">
+        <v>3</v>
+      </c>
+      <c r="T13" s="2">
+        <v>677</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Statistics on the runs
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A321755-7072-864B-A212-0507E8EDC596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E02E4D-1A65-A045-97BA-E8A51EB40E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24540" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="13180" windowWidth="41120" windowHeight="12240" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -100,6 +100,18 @@
   <si>
     <t>Pull requests</t>
   </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +160,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -270,10 +294,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -339,16 +363,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$23</c:f>
+              <c:f>Data!$E$2:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -414,6 +441,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>4504</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,10 +483,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -522,16 +552,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$23</c:f>
+              <c:f>Data!$F$2:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -597,6 +630,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1724</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,10 +672,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -705,16 +741,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$23</c:f>
+              <c:f>Data!$G$2:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -780,6 +819,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3560</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1035,10 +1077,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1104,16 +1146,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$K$2:$K$23</c:f>
+              <c:f>Data!$K$2:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1178,6 +1223,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1218,10 +1266,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1287,16 +1335,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$23</c:f>
+              <c:f>Data!$N$2:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1361,6 +1412,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1401,10 +1455,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1470,16 +1524,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$J$2:$J$23</c:f>
+              <c:f>Data!$J$2:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1544,6 +1601,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1803,10 +1863,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1872,16 +1932,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$23</c:f>
+              <c:f>Data!$M$2:$M$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -1946,6 +2009,9 @@
                   <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>220</c:v>
                 </c:pt>
               </c:numCache>
@@ -1986,10 +2052,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2055,16 +2121,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$23</c:f>
+              <c:f>Data!$P$2:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2129,6 +2198,9 @@
                   <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
@@ -2385,10 +2457,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$23</c:f>
+              <c:f>Data!$A$2:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2454,16 +2526,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$23</c:f>
+              <c:f>Data!$R$2:$R$24</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -2528,6 +2603,9 @@
                   <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
@@ -5084,33 +5162,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:T23" totalsRowShown="0">
-  <autoFilter ref="A1:T23" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:X24" totalsRowShown="0">
+  <autoFilter ref="A1:X24" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="11">
       <calculatedColumnFormula>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="4">
+    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="8">
       <calculatedColumnFormula>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{67D9B221-0B31-4848-8615-FFAA31A553EC}" name="Running" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{EDC0224F-D9E5-6F46-A4AD-E4CCACBEC828}" name="Failed" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{10E4F180-ED15-E849-B5B3-B50AD4FD7CE9}" name="OK" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{41B7AB09-D6AC-6945-B9EC-BB3EC1357064}" name="Cancelled" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5413,10 +5495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5441,9 +5523,13 @@
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5502,10 +5588,22 @@
         <v>15</v>
       </c>
       <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44574</v>
       </c>
@@ -5565,11 +5663,15 @@
       <c r="S2" s="2">
         <v>2</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2">
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44578</v>
       </c>
@@ -5629,11 +5731,15 @@
       <c r="S3" s="2">
         <v>2</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2">
         <v>542</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44580</v>
       </c>
@@ -5693,11 +5799,15 @@
       <c r="S4" s="2">
         <v>2</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2">
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44588</v>
       </c>
@@ -5757,11 +5867,15 @@
       <c r="S5" s="2">
         <v>3</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2">
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44593</v>
       </c>
@@ -5821,11 +5935,15 @@
       <c r="S6" s="2">
         <v>3</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2">
         <v>561</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44602</v>
       </c>
@@ -5885,11 +6003,15 @@
       <c r="S7" s="2">
         <v>3</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2">
         <v>586</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44610</v>
       </c>
@@ -5949,11 +6071,15 @@
       <c r="S8" s="2">
         <v>3</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2">
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44613</v>
       </c>
@@ -6013,11 +6139,15 @@
       <c r="S9" s="2">
         <v>3</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2">
         <v>601</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44636</v>
       </c>
@@ -6077,11 +6207,15 @@
       <c r="S10" s="2">
         <v>3</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2">
         <v>632</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44645</v>
       </c>
@@ -6141,11 +6275,15 @@
       <c r="S11" s="2">
         <v>3</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2">
         <v>661</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44657</v>
       </c>
@@ -6205,11 +6343,15 @@
       <c r="S12" s="2">
         <v>3</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2">
         <v>669</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44664</v>
       </c>
@@ -6269,11 +6411,15 @@
       <c r="S13" s="2">
         <v>3</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2">
         <v>677</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44676</v>
       </c>
@@ -6333,11 +6479,15 @@
       <c r="S14" s="2">
         <v>3</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2">
         <v>685</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44678</v>
       </c>
@@ -6397,11 +6547,15 @@
       <c r="S15" s="2">
         <v>3</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2">
         <v>690</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44679</v>
       </c>
@@ -6461,11 +6615,15 @@
       <c r="S16" s="2">
         <v>3</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2">
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44686</v>
       </c>
@@ -6525,11 +6683,15 @@
       <c r="S17" s="2">
         <v>3</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2">
         <v>714</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44691</v>
       </c>
@@ -6589,11 +6751,15 @@
       <c r="S18" s="2">
         <v>3</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2">
         <v>721</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44705</v>
       </c>
@@ -6653,11 +6819,15 @@
       <c r="S19" s="2">
         <v>4</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2">
         <v>748</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44707</v>
       </c>
@@ -6717,11 +6887,15 @@
       <c r="S20" s="2">
         <v>4</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2">
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44710</v>
       </c>
@@ -6781,11 +6955,15 @@
       <c r="S21" s="2">
         <v>4</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2">
         <v>773</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44713</v>
       </c>
@@ -6845,11 +7023,15 @@
       <c r="S22" s="2">
         <v>4</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2">
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44714</v>
       </c>
@@ -6909,8 +7091,89 @@
       <c r="S23" s="2">
         <v>4</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2">
         <v>789</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B24" s="2">
+        <v>104</v>
+      </c>
+      <c r="C24" s="2">
+        <v>235</v>
+      </c>
+      <c r="D24" s="2">
+        <v>188</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4510</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1728</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3565</v>
+      </c>
+      <c r="H24" s="2">
+        <v>61091</v>
+      </c>
+      <c r="I24" s="2">
+        <v>43136</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>220</v>
+      </c>
+      <c r="M24" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>220</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2">
+        <v>157</v>
+      </c>
+      <c r="P24" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>157</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>131</v>
+      </c>
+      <c r="R24" s="2">
+        <v>132</v>
+      </c>
+      <c r="S24" s="2">
+        <v>4</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0</v>
+      </c>
+      <c r="U24" s="2">
+        <v>302</v>
+      </c>
+      <c r="V24" s="2">
+        <v>488</v>
+      </c>
+      <c r="W24" s="2">
+        <v>7</v>
+      </c>
+      <c r="X24" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[Cancelled]])</f>
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updted the stats after last release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBD39A1-69AB-B147-9EA9-07B3513E036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A344871A-65B1-B549-80FC-6C9C18F7DC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24520" activeTab="5" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12220" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -301,10 +301,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -382,16 +382,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$27</c:f>
+              <c:f>Data!$E$2:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -469,6 +472,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>4515</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,10 +514,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -589,16 +595,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$27</c:f>
+              <c:f>Data!$F$2:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -676,6 +685,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1758</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -715,10 +727,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -796,16 +808,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$27</c:f>
+              <c:f>Data!$G$2:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -883,6 +898,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>3610</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,10 +1156,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1219,16 +1237,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$K$2:$K$27</c:f>
+              <c:f>Data!$K$2:$K$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1305,6 +1326,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1345,10 +1369,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1426,16 +1450,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$27</c:f>
+              <c:f>Data!$N$2:$N$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1512,6 +1539,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1552,10 +1582,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1633,16 +1663,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$J$2:$J$27</c:f>
+              <c:f>Data!$J$2:$J$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1719,6 +1752,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1978,10 +2014,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2059,16 +2095,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$27</c:f>
+              <c:f>Data!$M$2:$M$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2146,6 +2185,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2185,10 +2227,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2266,16 +2308,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$27</c:f>
+              <c:f>Data!$P$2:$P$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2352,6 +2397,9 @@
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
@@ -2608,10 +2656,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2689,16 +2737,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$27</c:f>
+              <c:f>Data!$R$2:$R$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -2776,6 +2827,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2997,10 +3051,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3078,16 +3132,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$27</c:f>
+              <c:f>Data!$T$2:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3098,6 +3155,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3134,10 +3194,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3215,16 +3275,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$27</c:f>
+              <c:f>Data!$U$2:$U$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -3236,6 +3299,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3271,10 +3337,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3352,16 +3418,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$27</c:f>
+              <c:f>Data!$V$2:$V$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -3373,6 +3442,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>548</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3408,10 +3480,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3489,16 +3561,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$27</c:f>
+              <c:f>Data!$W$2:$W$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -3509,6 +3584,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3547,10 +3625,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$27</c:f>
+              <c:f>Data!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3628,16 +3706,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$27</c:f>
+              <c:f>Data!$X$2:$X$28</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -6703,7 +6784,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{5B2EC930-5C2E-4448-96C6-E1C9EC4CF674}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6876,8 +6957,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:Y27" totalsRowShown="0">
-  <autoFilter ref="A1:Y27" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:Y28" totalsRowShown="0">
+  <autoFilter ref="A1:Y28" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="23"/>
@@ -7212,10 +7293,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView topLeftCell="H20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9219,6 +9301,84 @@
         <v>857</v>
       </c>
     </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B28" s="2">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2">
+        <v>237</v>
+      </c>
+      <c r="D28" s="2">
+        <v>190</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4585</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1763</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3627</v>
+      </c>
+      <c r="H28" s="2">
+        <v>61547</v>
+      </c>
+      <c r="I28" s="2">
+        <v>43284</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>222</v>
+      </c>
+      <c r="M28" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>222</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2">
+        <v>159</v>
+      </c>
+      <c r="P28" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>159</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>133</v>
+      </c>
+      <c r="R28" s="2">
+        <v>135</v>
+      </c>
+      <c r="S28" s="2">
+        <v>4</v>
+      </c>
+      <c r="T28" s="2">
+        <v>0</v>
+      </c>
+      <c r="U28" s="2">
+        <v>316</v>
+      </c>
+      <c r="V28" s="2">
+        <v>548</v>
+      </c>
+      <c r="W28" s="2">
+        <v>7</v>
+      </c>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>871</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Using cloc for the statistics
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE2A3B6-A596-0247-8130-D7D0C8874496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DB2896-B9B3-BA45-B287-36C702C54626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -116,6 +116,27 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>YAML</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>Bash</t>
+  </si>
+  <si>
+    <t>Total2</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +185,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="32">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -301,10 +343,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -394,16 +436,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$31</c:f>
+              <c:f>Data!$E$2:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -492,6 +537,9 @@
                   <c:v>4712</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>4720</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>4720</c:v>
                 </c:pt>
               </c:numCache>
@@ -509,7 +557,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$F$1</c:f>
+              <c:f>Data!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -532,10 +580,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -625,16 +673,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$31</c:f>
+              <c:f>Data!$M$2:$M$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -723,6 +774,9 @@
                   <c:v>1776</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>1782</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>1782</c:v>
                 </c:pt>
               </c:numCache>
@@ -740,7 +794,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$G$1</c:f>
+              <c:f>Data!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -763,10 +817,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -856,16 +910,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$31</c:f>
+              <c:f>Data!$N$2:$N$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -954,6 +1011,9 @@
                   <c:v>3662</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>3684</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>3684</c:v>
                 </c:pt>
               </c:numCache>
@@ -1187,7 +1247,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$K$1</c:f>
+              <c:f>Data!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1210,10 +1270,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1303,16 +1363,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$K$2:$K$31</c:f>
+              <c:f>Data!$R$2:$R$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1401,6 +1464,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1418,7 +1484,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$N$1</c:f>
+              <c:f>Data!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1441,10 +1507,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1534,16 +1600,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$31</c:f>
+              <c:f>Data!$U$2:$U$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1632,6 +1701,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1649,7 +1721,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$J$1</c:f>
+              <c:f>Data!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1672,10 +1744,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1765,16 +1837,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$J$2:$J$31</c:f>
+              <c:f>Data!$Q$2:$Q$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1863,6 +1938,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2099,7 +2177,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$M$1</c:f>
+              <c:f>Data!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2122,10 +2200,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2215,16 +2293,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$31</c:f>
+              <c:f>Data!$T$2:$T$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2313,6 +2394,9 @@
                   <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>224</c:v>
                 </c:pt>
               </c:numCache>
@@ -2330,7 +2414,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$P$1</c:f>
+              <c:f>Data!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2353,10 +2437,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2446,16 +2530,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$31</c:f>
+              <c:f>Data!$W$2:$W$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2544,6 +2631,9 @@
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
@@ -2777,7 +2867,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$R$1</c:f>
+              <c:f>Data!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2800,10 +2890,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2893,16 +2983,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$31</c:f>
+              <c:f>Data!$Y$2:$Y$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -2991,6 +3084,9 @@
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
@@ -3193,7 +3289,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$T$1</c:f>
+              <c:f>Data!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3213,10 +3309,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3306,16 +3402,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$31</c:f>
+              <c:f>Data!$AA$2:$AA$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3338,6 +3437,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3354,7 +3456,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$U$1</c:f>
+              <c:f>Data!$AB$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3374,10 +3476,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3467,16 +3569,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$31</c:f>
+              <c:f>Data!$AB$2:$AB$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -3499,6 +3604,9 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>321</c:v>
                 </c:pt>
               </c:numCache>
@@ -3515,7 +3623,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$V$1</c:f>
+              <c:f>Data!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3535,10 +3643,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3628,16 +3736,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$31</c:f>
+              <c:f>Data!$AC$2:$AC$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -3661,6 +3772,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>593</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3676,7 +3790,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$W$1</c:f>
+              <c:f>Data!$AD$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3696,10 +3810,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3789,16 +3903,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$31</c:f>
+              <c:f>Data!$AD$2:$AD$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -3821,6 +3938,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3837,7 +3957,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$X$1</c:f>
+              <c:f>Data!$AE$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3859,10 +3979,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$31</c:f>
+              <c:f>Data!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3952,16 +4072,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$31</c:f>
+              <c:f>Data!$AE$2:$AE$32</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7200,38 +7323,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:Y31" totalsRowShown="0">
-  <autoFilter ref="A1:Y31" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF32" totalsRowShown="0">
+  <autoFilter ref="A1:AF32" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+  <tableColumns count="32">
+    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="27"/>
+    <tableColumn id="26" xr3:uid="{EA0BB0A1-B927-BA42-95D8-323FF0F98170}" name="Shell" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{044A9D24-EDBD-814E-8836-3A4FC1DAF6CD}" name="MD" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{7634D894-69D0-B844-B715-963F9BC2312D}" name="YAML" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{35076C74-15AC-EC42-A3FA-C7C55763EEA7}" name="Text" dataDxfId="3"/>
+    <tableColumn id="30" xr3:uid="{1A9EAD82-A8B4-184C-92DB-650EA2147810}" name="make" dataDxfId="2"/>
+    <tableColumn id="31" xr3:uid="{F5568E37-EB5F-0B40-B8FE-3BC68D2DEFB3}" name="Bash" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{74A04583-DF3F-244E-8F76-155696F8B4E4}" name="Total" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Data[[#This Row],[Shell]:[Bash]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="19">
       <calculatedColumnFormula>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="9">
+    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="16">
       <calculatedColumnFormula>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{67D9B221-0B31-4848-8615-FFAA31A553EC}" name="Running" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{EDC0224F-D9E5-6F46-A4AD-E4CCACBEC828}" name="Failed" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{10E4F180-ED15-E849-B5B3-B50AD4FD7CE9}" name="OK" dataDxfId="3"/>
-    <tableColumn id="24" xr3:uid="{41B7AB09-D6AC-6945-B9EC-BB3EC1357064}" name="Cancelled" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{B9A99AA7-42FD-D344-A29E-4499FB1F8CE3}" name="Total" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{67D9B221-0B31-4848-8615-FFAA31A553EC}" name="Running" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{EDC0224F-D9E5-6F46-A4AD-E4CCACBEC828}" name="Failed" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{10E4F180-ED15-E849-B5B3-B50AD4FD7CE9}" name="OK" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{41B7AB09-D6AC-6945-B9EC-BB3EC1357064}" name="Cancelled" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="8"/>
+    <tableColumn id="25" xr3:uid="{B9A99AA7-42FD-D344-A29E-4499FB1F8CE3}" name="Total2" dataDxfId="7">
       <calculatedColumnFormula>SUM(Data[[#This Row],[Running]:[GH runs]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7536,11 +7668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W31" sqref="W31"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7550,28 +7682,29 @@
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="6.5" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19" customWidth="1"/>
+    <col min="24" max="24" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7588,67 +7721,88 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="X1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Y1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Z1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" t="s">
-        <v>24</v>
+      <c r="AF1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44574</v>
       </c>
@@ -7664,63 +7818,70 @@
       <c r="E2" s="2">
         <v>4368</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
         <v>1523</v>
       </c>
-      <c r="G2" s="2">
+      <c r="N2" s="2">
         <v>3195</v>
       </c>
-      <c r="H2" s="2">
+      <c r="O2" s="2">
         <v>57442</v>
       </c>
-      <c r="I2" s="2">
+      <c r="P2" s="2">
         <v>40634</v>
       </c>
-      <c r="J2" s="2">
+      <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="2">
+      <c r="R2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="2">
+      <c r="S2" s="2">
         <v>203</v>
       </c>
-      <c r="M2" s="2">
+      <c r="T2" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N2" s="2">
+      <c r="U2" s="2">
         <v>0</v>
       </c>
-      <c r="O2" s="2">
+      <c r="V2" s="2">
         <v>135</v>
       </c>
-      <c r="P2" s="2">
+      <c r="W2" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="X2" s="2">
         <v>125</v>
       </c>
-      <c r="R2" s="2">
+      <c r="Y2" s="2">
         <v>122</v>
       </c>
-      <c r="S2" s="2">
+      <c r="Z2" s="2">
         <v>2</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2">
         <v>541</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AF2" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44578</v>
       </c>
@@ -7736,63 +7897,70 @@
       <c r="E3" s="2">
         <v>4368</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
         <v>1524</v>
       </c>
-      <c r="G3" s="2">
+      <c r="N3" s="2">
         <v>3196</v>
       </c>
-      <c r="H3" s="2">
+      <c r="O3" s="2">
         <v>57422</v>
       </c>
-      <c r="I3" s="2">
+      <c r="P3" s="2">
         <v>40034</v>
       </c>
-      <c r="J3" s="2">
+      <c r="Q3" s="2">
         <v>1</v>
       </c>
-      <c r="K3" s="2">
+      <c r="R3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="2">
+      <c r="S3" s="2">
         <v>203</v>
       </c>
-      <c r="M3" s="2">
+      <c r="T3" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N3" s="2">
+      <c r="U3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="2">
+      <c r="V3" s="2">
         <v>135</v>
       </c>
-      <c r="P3" s="2">
+      <c r="W3" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="X3" s="2">
         <v>125</v>
       </c>
-      <c r="R3" s="2">
+      <c r="Y3" s="2">
         <v>122</v>
       </c>
-      <c r="S3" s="2">
+      <c r="Z3" s="2">
         <v>2</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2">
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2">
         <v>542</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AF3" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>542</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44580</v>
       </c>
@@ -7808,63 +7976,70 @@
       <c r="E4" s="2">
         <v>4368</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
         <v>1525</v>
       </c>
-      <c r="G4" s="2">
+      <c r="N4" s="2">
         <v>3197</v>
       </c>
-      <c r="H4" s="2">
+      <c r="O4" s="2">
         <v>57422</v>
       </c>
-      <c r="I4" s="2">
+      <c r="P4" s="2">
         <v>40634</v>
       </c>
-      <c r="J4" s="2">
+      <c r="Q4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="2">
+      <c r="R4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="2">
+      <c r="S4" s="2">
         <v>203</v>
       </c>
-      <c r="M4" s="2">
+      <c r="T4" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N4" s="2">
+      <c r="U4" s="2">
         <v>0</v>
       </c>
-      <c r="O4" s="2">
+      <c r="V4" s="2">
         <v>135</v>
       </c>
-      <c r="P4" s="2">
+      <c r="W4" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="X4" s="2">
         <v>125</v>
       </c>
-      <c r="R4" s="2">
+      <c r="Y4" s="2">
         <v>122</v>
       </c>
-      <c r="S4" s="2">
+      <c r="Z4" s="2">
         <v>2</v>
       </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2">
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2">
         <v>543</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="AF4" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44588</v>
       </c>
@@ -7880,63 +8055,70 @@
       <c r="E5" s="2">
         <v>4368</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2">
         <v>1531</v>
       </c>
-      <c r="G5" s="2">
+      <c r="N5" s="2">
         <v>3207</v>
       </c>
-      <c r="H5" s="2">
+      <c r="O5" s="2">
         <v>57794</v>
       </c>
-      <c r="I5" s="2">
+      <c r="P5" s="2">
         <v>40652</v>
       </c>
-      <c r="J5" s="2">
+      <c r="Q5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="2">
+      <c r="R5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="2">
+      <c r="S5" s="2">
         <v>203</v>
       </c>
-      <c r="M5" s="2">
+      <c r="T5" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N5" s="2">
+      <c r="U5" s="2">
         <v>0</v>
       </c>
-      <c r="O5" s="2">
+      <c r="V5" s="2">
         <v>135</v>
       </c>
-      <c r="P5" s="2">
+      <c r="W5" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="X5" s="2">
         <v>125</v>
       </c>
-      <c r="R5" s="2">
+      <c r="Y5" s="2">
         <v>122</v>
       </c>
-      <c r="S5" s="2">
+      <c r="Z5" s="2">
         <v>3</v>
       </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2">
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2">
         <v>550</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="AF5" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44593</v>
       </c>
@@ -7952,63 +8134,70 @@
       <c r="E6" s="2">
         <v>4379</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
         <v>1539</v>
       </c>
-      <c r="G6" s="2">
+      <c r="N6" s="2">
         <v>3224</v>
       </c>
-      <c r="H6" s="2">
+      <c r="O6" s="2">
         <v>57859</v>
       </c>
-      <c r="I6" s="2">
+      <c r="P6" s="2">
         <v>40677</v>
       </c>
-      <c r="J6" s="2">
+      <c r="Q6" s="2">
         <v>1</v>
       </c>
-      <c r="K6" s="2">
+      <c r="R6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="2">
+      <c r="S6" s="2">
         <v>203</v>
       </c>
-      <c r="M6" s="2">
+      <c r="T6" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N6" s="2">
+      <c r="U6" s="2">
         <v>0</v>
       </c>
-      <c r="O6" s="2">
+      <c r="V6" s="2">
         <v>135</v>
       </c>
-      <c r="P6" s="2">
+      <c r="W6" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="X6" s="2">
         <v>125</v>
       </c>
-      <c r="R6" s="2">
+      <c r="Y6" s="2">
         <v>122</v>
       </c>
-      <c r="S6" s="2">
+      <c r="Z6" s="2">
         <v>3</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2">
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2">
         <v>561</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="AF6" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>561</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44602</v>
       </c>
@@ -8024,63 +8213,70 @@
       <c r="E7" s="2">
         <v>4381</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
         <v>1559</v>
       </c>
-      <c r="G7" s="2">
+      <c r="N7" s="2">
         <v>3265</v>
       </c>
-      <c r="H7" s="2">
+      <c r="O7" s="2">
         <v>58868</v>
       </c>
-      <c r="I7" s="2">
+      <c r="P7" s="2">
         <v>41555</v>
       </c>
-      <c r="J7" s="2">
+      <c r="Q7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="2">
+      <c r="R7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="2">
+      <c r="S7" s="2">
         <v>204</v>
       </c>
-      <c r="M7" s="2">
+      <c r="T7" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="N7" s="2">
+      <c r="U7" s="2">
         <v>0</v>
       </c>
-      <c r="O7" s="2">
+      <c r="V7" s="2">
         <v>135</v>
       </c>
-      <c r="P7" s="2">
+      <c r="W7" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="X7" s="2">
         <v>125</v>
       </c>
-      <c r="R7" s="2">
+      <c r="Y7" s="2">
         <v>122</v>
       </c>
-      <c r="S7" s="2">
+      <c r="Z7" s="2">
         <v>3</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2">
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2">
         <v>586</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="AF7" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>586</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44610</v>
       </c>
@@ -8096,63 +8292,70 @@
       <c r="E8" s="2">
         <v>4399</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2">
         <v>1568</v>
       </c>
-      <c r="G8" s="2">
+      <c r="N8" s="2">
         <v>3286</v>
       </c>
-      <c r="H8" s="2">
+      <c r="O8" s="2">
         <v>58985</v>
       </c>
-      <c r="I8" s="2">
+      <c r="P8" s="2">
         <v>41600</v>
       </c>
-      <c r="J8" s="2">
+      <c r="Q8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="R8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="2">
+      <c r="S8" s="2">
         <v>208</v>
       </c>
-      <c r="M8" s="2">
+      <c r="T8" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>208</v>
       </c>
-      <c r="N8" s="2">
+      <c r="U8" s="2">
         <v>0</v>
       </c>
-      <c r="O8" s="2">
+      <c r="V8" s="2">
         <v>135</v>
       </c>
-      <c r="P8" s="2">
+      <c r="W8" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="X8" s="2">
         <v>125</v>
       </c>
-      <c r="R8" s="2">
+      <c r="Y8" s="2">
         <v>122</v>
       </c>
-      <c r="S8" s="2">
+      <c r="Z8" s="2">
         <v>3</v>
       </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2">
         <v>595</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="AF8" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44613</v>
       </c>
@@ -8168,63 +8371,70 @@
       <c r="E9" s="2">
         <v>4413</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2">
         <v>1571</v>
       </c>
-      <c r="G9" s="2">
+      <c r="N9" s="2">
         <v>3298</v>
       </c>
-      <c r="H9" s="2">
+      <c r="O9" s="2">
         <v>59170</v>
       </c>
-      <c r="I9" s="2">
+      <c r="P9" s="2">
         <v>41754</v>
       </c>
-      <c r="J9" s="2">
+      <c r="Q9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="R9" s="2">
         <v>0</v>
       </c>
-      <c r="L9" s="2">
+      <c r="S9" s="2">
         <v>208</v>
       </c>
-      <c r="M9" s="2">
+      <c r="T9" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>208</v>
       </c>
-      <c r="N9" s="2">
+      <c r="U9" s="2">
         <v>0</v>
       </c>
-      <c r="O9" s="2">
+      <c r="V9" s="2">
         <v>135</v>
       </c>
-      <c r="P9" s="2">
+      <c r="W9" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="X9" s="2">
         <v>126</v>
       </c>
-      <c r="R9" s="2">
+      <c r="Y9" s="2">
         <v>122</v>
       </c>
-      <c r="S9" s="2">
+      <c r="Z9" s="2">
         <v>3</v>
       </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2">
         <v>601</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="AF9" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>601</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44636</v>
       </c>
@@ -8240,63 +8450,70 @@
       <c r="E10" s="2">
         <v>4430</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2">
         <v>1598</v>
       </c>
-      <c r="G10" s="2">
+      <c r="N10" s="2">
         <v>3339</v>
       </c>
-      <c r="H10" s="2">
+      <c r="O10" s="2">
         <v>59371</v>
       </c>
-      <c r="I10" s="2">
+      <c r="P10" s="2">
         <v>41908</v>
       </c>
-      <c r="J10" s="2">
+      <c r="Q10" s="2">
         <v>0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="R10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="2">
+      <c r="S10" s="2">
         <v>209</v>
       </c>
-      <c r="M10" s="2">
+      <c r="T10" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>209</v>
       </c>
-      <c r="N10" s="2">
+      <c r="U10" s="2">
         <v>0</v>
       </c>
-      <c r="O10" s="2">
+      <c r="V10" s="2">
         <v>141</v>
       </c>
-      <c r="P10" s="2">
+      <c r="W10" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>141</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="X10" s="2">
         <v>126</v>
       </c>
-      <c r="R10" s="2">
+      <c r="Y10" s="2">
         <v>122</v>
       </c>
-      <c r="S10" s="2">
+      <c r="Z10" s="2">
         <v>3</v>
       </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2">
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2">
         <v>632</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="AF10" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>632</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44645</v>
       </c>
@@ -8312,63 +8529,70 @@
       <c r="E11" s="2">
         <v>4432</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2">
         <v>1627</v>
       </c>
-      <c r="G11" s="2">
+      <c r="N11" s="2">
         <v>3375</v>
       </c>
-      <c r="H11" s="2">
+      <c r="O11" s="2">
         <v>59655</v>
       </c>
-      <c r="I11" s="2">
+      <c r="P11" s="2">
         <v>42123</v>
       </c>
-      <c r="J11" s="2">
+      <c r="Q11" s="2">
         <v>1</v>
       </c>
-      <c r="K11" s="2">
+      <c r="R11" s="2">
         <v>1</v>
       </c>
-      <c r="L11" s="2">
+      <c r="S11" s="2">
         <v>214</v>
       </c>
-      <c r="M11" s="2">
+      <c r="T11" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="N11" s="2">
+      <c r="U11" s="2">
         <v>0</v>
       </c>
-      <c r="O11" s="2">
+      <c r="V11" s="2">
         <v>148</v>
       </c>
-      <c r="P11" s="2">
+      <c r="W11" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="X11" s="2">
         <v>127</v>
       </c>
-      <c r="R11" s="2">
+      <c r="Y11" s="2">
         <v>128</v>
       </c>
-      <c r="S11" s="2">
+      <c r="Z11" s="2">
         <v>3</v>
       </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2">
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2">
         <v>661</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AF11" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>661</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44657</v>
       </c>
@@ -8384,63 +8608,70 @@
       <c r="E12" s="2">
         <v>4434</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2">
         <v>1632</v>
       </c>
-      <c r="G12" s="2">
+      <c r="N12" s="2">
         <v>3387</v>
       </c>
-      <c r="H12" s="2">
+      <c r="O12" s="2">
         <v>59702</v>
       </c>
-      <c r="I12" s="2">
+      <c r="P12" s="2">
         <v>42156</v>
       </c>
-      <c r="J12" s="2">
+      <c r="Q12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="2">
+      <c r="R12" s="2">
         <v>1</v>
       </c>
-      <c r="L12" s="2">
+      <c r="S12" s="2">
         <v>214</v>
       </c>
-      <c r="M12" s="2">
+      <c r="T12" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="N12" s="2">
+      <c r="U12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="2">
+      <c r="V12" s="2">
         <v>148</v>
       </c>
-      <c r="P12" s="2">
+      <c r="W12" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="X12" s="2">
         <v>127</v>
       </c>
-      <c r="R12" s="2">
+      <c r="Y12" s="2">
         <v>131</v>
       </c>
-      <c r="S12" s="2">
+      <c r="Z12" s="2">
         <v>3</v>
       </c>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2">
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2">
         <v>669</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="AF12" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>669</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44664</v>
       </c>
@@ -8456,63 +8687,70 @@
       <c r="E13" s="2">
         <v>4454</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2">
         <v>1637</v>
       </c>
-      <c r="G13" s="2">
+      <c r="N13" s="2">
         <v>3406</v>
       </c>
-      <c r="H13" s="2">
+      <c r="O13" s="2">
         <v>60308</v>
       </c>
-      <c r="I13" s="2">
+      <c r="P13" s="2">
         <v>42743</v>
       </c>
-      <c r="J13" s="2">
+      <c r="Q13" s="2">
         <v>1</v>
       </c>
-      <c r="K13" s="2">
+      <c r="R13" s="2">
         <v>1</v>
       </c>
-      <c r="L13" s="2">
+      <c r="S13" s="2">
         <v>214</v>
       </c>
-      <c r="M13" s="2">
+      <c r="T13" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="N13" s="2">
+      <c r="U13" s="2">
         <v>0</v>
       </c>
-      <c r="O13" s="2">
+      <c r="V13" s="2">
         <v>148</v>
       </c>
-      <c r="P13" s="2">
+      <c r="W13" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="X13" s="2">
         <v>128</v>
       </c>
-      <c r="R13" s="2">
+      <c r="Y13" s="2">
         <v>131</v>
       </c>
-      <c r="S13" s="2">
+      <c r="Z13" s="2">
         <v>3</v>
       </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2">
         <v>677</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="AF13" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>677</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44676</v>
       </c>
@@ -8528,63 +8766,70 @@
       <c r="E14" s="2">
         <v>4453</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2">
         <v>1647</v>
       </c>
-      <c r="G14" s="2">
+      <c r="N14" s="2">
         <v>3424</v>
       </c>
-      <c r="H14" s="2">
+      <c r="O14" s="2">
         <v>60352</v>
       </c>
-      <c r="I14" s="2">
+      <c r="P14" s="2">
         <v>42776</v>
       </c>
-      <c r="J14" s="2">
+      <c r="Q14" s="2">
         <v>2</v>
       </c>
-      <c r="K14" s="2">
+      <c r="R14" s="2">
         <v>2</v>
       </c>
-      <c r="L14" s="2">
+      <c r="S14" s="2">
         <v>215</v>
       </c>
-      <c r="M14" s="2">
+      <c r="T14" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>217</v>
       </c>
-      <c r="N14" s="2">
+      <c r="U14" s="2">
         <v>0</v>
       </c>
-      <c r="O14" s="2">
+      <c r="V14" s="2">
         <v>148</v>
       </c>
-      <c r="P14" s="2">
+      <c r="W14" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="X14" s="2">
         <v>128</v>
       </c>
-      <c r="R14" s="2">
+      <c r="Y14" s="2">
         <v>131</v>
       </c>
-      <c r="S14" s="2">
+      <c r="Z14" s="2">
         <v>3</v>
       </c>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2">
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2">
         <v>685</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="AF14" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>685</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44678</v>
       </c>
@@ -8600,63 +8845,70 @@
       <c r="E15" s="2">
         <v>4461</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2">
         <v>1652</v>
       </c>
-      <c r="G15" s="2">
+      <c r="N15" s="2">
         <v>3430</v>
       </c>
-      <c r="H15" s="2">
+      <c r="O15" s="2">
         <v>60372</v>
       </c>
-      <c r="I15" s="2">
+      <c r="P15" s="2">
         <v>42778</v>
       </c>
-      <c r="J15" s="2">
+      <c r="Q15" s="2">
         <v>1</v>
       </c>
-      <c r="K15" s="2">
+      <c r="R15" s="2">
         <v>1</v>
       </c>
-      <c r="L15" s="2">
+      <c r="S15" s="2">
         <v>216</v>
       </c>
-      <c r="M15" s="2">
+      <c r="T15" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>217</v>
       </c>
-      <c r="N15" s="2">
+      <c r="U15" s="2">
         <v>0</v>
       </c>
-      <c r="O15" s="2">
+      <c r="V15" s="2">
         <v>149</v>
       </c>
-      <c r="P15" s="2">
+      <c r="W15" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="X15" s="2">
         <v>128</v>
       </c>
-      <c r="R15" s="2">
+      <c r="Y15" s="2">
         <v>131</v>
       </c>
-      <c r="S15" s="2">
+      <c r="Z15" s="2">
         <v>3</v>
       </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2">
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2">
         <v>690</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="AF15" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>690</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44679</v>
       </c>
@@ -8672,63 +8924,70 @@
       <c r="E16" s="2">
         <v>4462</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2">
         <v>1660</v>
       </c>
-      <c r="G16" s="2">
+      <c r="N16" s="2">
         <v>3444</v>
       </c>
-      <c r="H16" s="2">
+      <c r="O16" s="2">
         <v>60431</v>
       </c>
-      <c r="I16" s="2">
+      <c r="P16" s="2">
         <v>42791</v>
       </c>
-      <c r="J16" s="2">
+      <c r="Q16" s="2">
         <v>1</v>
       </c>
-      <c r="K16" s="2">
+      <c r="R16" s="2">
         <v>1</v>
       </c>
-      <c r="L16" s="2">
+      <c r="S16" s="2">
         <v>217</v>
       </c>
-      <c r="M16" s="2">
+      <c r="T16" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>218</v>
       </c>
-      <c r="N16" s="2">
+      <c r="U16" s="2">
         <v>0</v>
       </c>
-      <c r="O16" s="2">
+      <c r="V16" s="2">
         <v>149</v>
       </c>
-      <c r="P16" s="2">
+      <c r="W16" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="X16" s="2">
         <v>128</v>
       </c>
-      <c r="R16" s="2">
+      <c r="Y16" s="2">
         <v>132</v>
       </c>
-      <c r="S16" s="2">
+      <c r="Z16" s="2">
         <v>3</v>
       </c>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2">
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2">
         <v>700</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="AF16" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44686</v>
       </c>
@@ -8744,63 +9003,70 @@
       <c r="E17" s="2">
         <v>4454</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2">
         <v>1670</v>
       </c>
-      <c r="G17" s="2">
+      <c r="N17" s="2">
         <v>3473</v>
       </c>
-      <c r="H17" s="2">
+      <c r="O17" s="2">
         <v>60537</v>
       </c>
-      <c r="I17" s="2">
+      <c r="P17" s="2">
         <v>42889</v>
       </c>
-      <c r="J17" s="2">
+      <c r="Q17" s="2">
         <v>1</v>
       </c>
-      <c r="K17" s="2">
+      <c r="R17" s="2">
         <v>1</v>
       </c>
-      <c r="L17" s="2">
+      <c r="S17" s="2">
         <v>218</v>
       </c>
-      <c r="M17" s="2">
+      <c r="T17" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="N17" s="2">
+      <c r="U17" s="2">
         <v>0</v>
       </c>
-      <c r="O17" s="2">
+      <c r="V17" s="2">
         <v>149</v>
       </c>
-      <c r="P17" s="2">
+      <c r="W17" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="X17" s="2">
         <v>128</v>
       </c>
-      <c r="R17" s="2">
+      <c r="Y17" s="2">
         <v>132</v>
       </c>
-      <c r="S17" s="2">
+      <c r="Z17" s="2">
         <v>3</v>
       </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2">
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2">
         <v>714</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="AF17" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>714</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44691</v>
       </c>
@@ -8816,63 +9082,70 @@
       <c r="E18" s="2">
         <v>4454</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2">
         <v>1676</v>
       </c>
-      <c r="G18" s="2">
+      <c r="N18" s="2">
         <v>3481</v>
       </c>
-      <c r="H18" s="2">
+      <c r="O18" s="2">
         <v>60564</v>
       </c>
-      <c r="I18" s="2">
+      <c r="P18" s="2">
         <v>42903</v>
       </c>
-      <c r="J18" s="2">
+      <c r="Q18" s="2">
         <v>1</v>
       </c>
-      <c r="K18" s="2">
+      <c r="R18" s="2">
         <v>1</v>
       </c>
-      <c r="L18" s="2">
+      <c r="S18" s="2">
         <v>218</v>
       </c>
-      <c r="M18" s="2">
+      <c r="T18" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="N18" s="2">
+      <c r="U18" s="2">
         <v>0</v>
       </c>
-      <c r="O18" s="2">
+      <c r="V18" s="2">
         <v>150</v>
       </c>
-      <c r="P18" s="2">
+      <c r="W18" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>150</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="X18" s="2">
         <v>128</v>
       </c>
-      <c r="R18" s="2">
+      <c r="Y18" s="2">
         <v>132</v>
       </c>
-      <c r="S18" s="2">
+      <c r="Z18" s="2">
         <v>3</v>
       </c>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2">
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2">
         <v>721</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="AF18" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>721</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44705</v>
       </c>
@@ -8888,63 +9161,70 @@
       <c r="E19" s="2">
         <v>4470</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2">
         <v>1695</v>
       </c>
-      <c r="G19" s="2">
+      <c r="N19" s="2">
         <v>3500</v>
       </c>
-      <c r="H19" s="2">
+      <c r="O19" s="2">
         <v>60613</v>
       </c>
-      <c r="I19" s="2">
+      <c r="P19" s="2">
         <v>42943</v>
       </c>
-      <c r="J19" s="2">
+      <c r="Q19" s="2">
         <v>1</v>
       </c>
-      <c r="K19" s="2">
+      <c r="R19" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="2">
+      <c r="S19" s="2">
         <v>218</v>
       </c>
-      <c r="M19" s="2">
+      <c r="T19" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="N19" s="2">
+      <c r="U19" s="2">
         <v>2</v>
       </c>
-      <c r="O19" s="2">
+      <c r="V19" s="2">
         <v>154</v>
       </c>
-      <c r="P19" s="2">
+      <c r="W19" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="X19" s="2">
         <v>128</v>
       </c>
-      <c r="R19" s="2">
+      <c r="Y19" s="2">
         <v>131</v>
       </c>
-      <c r="S19" s="2">
+      <c r="Z19" s="2">
         <v>4</v>
       </c>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2">
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2">
         <v>748</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="AF19" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>748</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44707</v>
       </c>
@@ -8960,63 +9240,70 @@
       <c r="E20" s="2">
         <v>4506</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2">
         <v>1699</v>
       </c>
-      <c r="G20" s="2">
+      <c r="N20" s="2">
         <v>3520</v>
       </c>
-      <c r="H20" s="2">
+      <c r="O20" s="2">
         <v>60719</v>
       </c>
-      <c r="I20" s="2">
+      <c r="P20" s="2">
         <v>42953</v>
       </c>
-      <c r="J20" s="2">
+      <c r="Q20" s="2">
         <v>1</v>
       </c>
-      <c r="K20" s="2">
+      <c r="R20" s="2">
         <v>1</v>
       </c>
-      <c r="L20" s="2">
+      <c r="S20" s="2">
         <v>219</v>
       </c>
-      <c r="M20" s="2">
+      <c r="T20" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="N20" s="2">
+      <c r="U20" s="2">
         <v>1</v>
       </c>
-      <c r="O20" s="2">
+      <c r="V20" s="2">
         <v>155</v>
       </c>
-      <c r="P20" s="2">
+      <c r="W20" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="X20" s="2">
         <v>131</v>
       </c>
-      <c r="R20" s="2">
+      <c r="Y20" s="2">
         <v>132</v>
       </c>
-      <c r="S20" s="2">
+      <c r="Z20" s="2">
         <v>4</v>
       </c>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2">
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2">
         <v>754</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="AF20" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44710</v>
       </c>
@@ -9032,63 +9319,70 @@
       <c r="E21" s="2">
         <v>4504</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2">
         <v>1718</v>
       </c>
-      <c r="G21" s="2">
+      <c r="N21" s="2">
         <v>3546</v>
       </c>
-      <c r="H21" s="2">
+      <c r="O21" s="2">
         <v>61044</v>
       </c>
-      <c r="I21" s="2">
+      <c r="P21" s="2">
         <v>43112</v>
       </c>
-      <c r="J21" s="2">
+      <c r="Q21" s="2">
         <v>1</v>
       </c>
-      <c r="K21" s="2">
+      <c r="R21" s="2">
         <v>1</v>
       </c>
-      <c r="L21" s="2">
+      <c r="S21" s="2">
         <v>219</v>
       </c>
-      <c r="M21" s="2">
+      <c r="T21" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="N21" s="2">
+      <c r="U21" s="2">
         <v>0</v>
       </c>
-      <c r="O21" s="2">
+      <c r="V21" s="2">
         <v>156</v>
       </c>
-      <c r="P21" s="2">
+      <c r="W21" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="X21" s="2">
         <v>131</v>
       </c>
-      <c r="R21" s="2">
+      <c r="Y21" s="2">
         <v>132</v>
       </c>
-      <c r="S21" s="2">
+      <c r="Z21" s="2">
         <v>4</v>
       </c>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2">
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2">
         <v>773</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="AF21" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>773</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44713</v>
       </c>
@@ -9104,63 +9398,70 @@
       <c r="E22" s="2">
         <v>4504</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2">
         <v>1723</v>
       </c>
-      <c r="G22" s="2">
+      <c r="N22" s="2">
         <v>3559</v>
       </c>
-      <c r="H22" s="2">
+      <c r="O22" s="2">
         <v>61077</v>
       </c>
-      <c r="I22" s="2">
+      <c r="P22" s="2">
         <v>43133</v>
       </c>
-      <c r="J22" s="2">
+      <c r="Q22" s="2">
         <v>1</v>
       </c>
-      <c r="K22" s="2">
+      <c r="R22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="2">
+      <c r="S22" s="2">
         <v>219</v>
       </c>
-      <c r="M22" s="2">
+      <c r="T22" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="N22" s="2">
+      <c r="U22" s="2">
         <v>0</v>
       </c>
-      <c r="O22" s="2">
+      <c r="V22" s="2">
         <v>157</v>
       </c>
-      <c r="P22" s="2">
+      <c r="W22" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="X22" s="2">
         <v>131</v>
       </c>
-      <c r="R22" s="2">
+      <c r="Y22" s="2">
         <v>132</v>
       </c>
-      <c r="S22" s="2">
+      <c r="Z22" s="2">
         <v>4</v>
       </c>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2">
         <v>787</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="AF22" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44714</v>
       </c>
@@ -9176,63 +9477,70 @@
       <c r="E23" s="2">
         <v>4504</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2">
         <v>1724</v>
       </c>
-      <c r="G23" s="2">
+      <c r="N23" s="2">
         <v>3560</v>
       </c>
-      <c r="H23" s="2">
+      <c r="O23" s="2">
         <v>61077</v>
       </c>
-      <c r="I23" s="2">
+      <c r="P23" s="2">
         <v>43133</v>
       </c>
-      <c r="J23" s="2">
+      <c r="Q23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="R23" s="2">
         <v>0</v>
       </c>
-      <c r="L23" s="2">
+      <c r="S23" s="2">
         <v>220</v>
       </c>
-      <c r="M23" s="2">
+      <c r="T23" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="N23" s="2">
+      <c r="U23" s="2">
         <v>0</v>
       </c>
-      <c r="O23" s="2">
+      <c r="V23" s="2">
         <v>157</v>
       </c>
-      <c r="P23" s="2">
+      <c r="W23" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="X23" s="2">
         <v>131</v>
       </c>
-      <c r="R23" s="2">
+      <c r="Y23" s="2">
         <v>132</v>
       </c>
-      <c r="S23" s="2">
+      <c r="Z23" s="2">
         <v>4</v>
       </c>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2">
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2">
         <v>789</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="AF23" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>789</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44715</v>
       </c>
@@ -9248,69 +9556,76 @@
       <c r="E24" s="2">
         <v>4510</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2">
         <v>1728</v>
       </c>
-      <c r="G24" s="2">
+      <c r="N24" s="2">
         <v>3565</v>
       </c>
-      <c r="H24" s="2">
+      <c r="O24" s="2">
         <v>61091</v>
       </c>
-      <c r="I24" s="2">
+      <c r="P24" s="2">
         <v>43136</v>
       </c>
-      <c r="J24" s="2">
+      <c r="Q24" s="2">
         <v>0</v>
       </c>
-      <c r="K24" s="2">
+      <c r="R24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="2">
+      <c r="S24" s="2">
         <v>220</v>
       </c>
-      <c r="M24" s="2">
+      <c r="T24" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="N24" s="2">
+      <c r="U24" s="2">
         <v>0</v>
       </c>
-      <c r="O24" s="2">
+      <c r="V24" s="2">
         <v>157</v>
       </c>
-      <c r="P24" s="2">
+      <c r="W24" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="X24" s="2">
         <v>131</v>
       </c>
-      <c r="R24" s="2">
+      <c r="Y24" s="2">
         <v>132</v>
       </c>
-      <c r="S24" s="2">
+      <c r="Z24" s="2">
         <v>4</v>
       </c>
-      <c r="T24" s="2">
+      <c r="AA24" s="2">
         <v>0</v>
       </c>
-      <c r="U24" s="2">
+      <c r="AB24" s="2">
         <v>302</v>
       </c>
-      <c r="V24" s="2">
+      <c r="AC24" s="2">
         <v>488</v>
       </c>
-      <c r="W24" s="2">
+      <c r="AD24" s="2">
         <v>7</v>
       </c>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2">
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>797</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44723</v>
       </c>
@@ -9326,69 +9641,76 @@
       <c r="E25" s="2">
         <v>4510</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2">
         <v>1733</v>
       </c>
-      <c r="G25" s="2">
+      <c r="N25" s="2">
         <v>3579</v>
       </c>
-      <c r="H25" s="2">
+      <c r="O25" s="2">
         <v>61141</v>
       </c>
-      <c r="I25" s="2">
+      <c r="P25" s="2">
         <v>43154</v>
       </c>
-      <c r="J25" s="2">
+      <c r="Q25" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="2">
+      <c r="R25" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="2">
+      <c r="S25" s="2">
         <v>221</v>
       </c>
-      <c r="M25" s="2">
+      <c r="T25" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="N25" s="2">
+      <c r="U25" s="2">
         <v>0</v>
       </c>
-      <c r="O25" s="2">
+      <c r="V25" s="2">
         <v>158</v>
       </c>
-      <c r="P25" s="2">
+      <c r="W25" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>158</v>
       </c>
-      <c r="Q25" s="2">
+      <c r="X25" s="2">
         <v>131</v>
       </c>
-      <c r="R25" s="2">
+      <c r="Y25" s="2">
         <v>132</v>
       </c>
-      <c r="S25" s="2">
+      <c r="Z25" s="2">
         <v>4</v>
       </c>
-      <c r="T25" s="2">
+      <c r="AA25" s="2">
         <v>0</v>
       </c>
-      <c r="U25" s="2">
+      <c r="AB25" s="2">
         <v>304</v>
       </c>
-      <c r="V25" s="2">
+      <c r="AC25" s="2">
         <v>501</v>
       </c>
-      <c r="W25" s="2">
+      <c r="AD25" s="2">
         <v>7</v>
       </c>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2">
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>812</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44725</v>
       </c>
@@ -9404,69 +9726,76 @@
       <c r="E26" s="2">
         <v>4510</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2">
         <v>1743</v>
       </c>
-      <c r="G26" s="2">
+      <c r="N26" s="2">
         <v>3590</v>
       </c>
-      <c r="H26" s="2">
+      <c r="O26" s="2">
         <v>61156</v>
       </c>
-      <c r="I26" s="2">
+      <c r="P26" s="2">
         <v>43168</v>
       </c>
-      <c r="J26" s="2">
+      <c r="Q26" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="2">
+      <c r="R26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="2">
+      <c r="S26" s="2">
         <v>221</v>
       </c>
-      <c r="M26" s="2">
+      <c r="T26" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="N26" s="2">
+      <c r="U26" s="2">
         <v>0</v>
       </c>
-      <c r="O26" s="2">
+      <c r="V26" s="2">
         <v>159</v>
       </c>
-      <c r="P26" s="2">
+      <c r="W26" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q26" s="2">
+      <c r="X26" s="2">
         <v>131</v>
       </c>
-      <c r="R26" s="2">
+      <c r="Y26" s="2">
         <v>132</v>
       </c>
-      <c r="S26" s="2">
+      <c r="Z26" s="2">
         <v>4</v>
       </c>
-      <c r="T26" s="2">
+      <c r="AA26" s="2">
         <v>0</v>
       </c>
-      <c r="U26" s="2">
+      <c r="AB26" s="2">
         <v>305</v>
       </c>
-      <c r="V26" s="2">
+      <c r="AC26" s="2">
         <v>517</v>
       </c>
-      <c r="W26" s="2">
+      <c r="AD26" s="2">
         <v>7</v>
       </c>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2">
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>829</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44727</v>
       </c>
@@ -9482,69 +9811,76 @@
       <c r="E27" s="2">
         <v>4515</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2">
         <v>1758</v>
       </c>
-      <c r="G27" s="2">
+      <c r="N27" s="2">
         <v>3610</v>
       </c>
-      <c r="H27" s="2">
+      <c r="O27" s="2">
         <v>61388</v>
       </c>
-      <c r="I27" s="2">
+      <c r="P27" s="2">
         <v>43266</v>
       </c>
-      <c r="J27" s="2">
+      <c r="Q27" s="2">
         <v>0</v>
       </c>
-      <c r="K27" s="2">
+      <c r="R27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="2">
+      <c r="S27" s="2">
         <v>221</v>
       </c>
-      <c r="M27" s="2">
+      <c r="T27" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="N27" s="2">
+      <c r="U27" s="2">
         <v>0</v>
       </c>
-      <c r="O27" s="2">
+      <c r="V27" s="2">
         <v>159</v>
       </c>
-      <c r="P27" s="2">
+      <c r="W27" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q27" s="2">
+      <c r="X27" s="2">
         <v>131</v>
       </c>
-      <c r="R27" s="2">
+      <c r="Y27" s="2">
         <v>132</v>
       </c>
-      <c r="S27" s="2">
+      <c r="Z27" s="2">
         <v>4</v>
       </c>
-      <c r="T27" s="2">
+      <c r="AA27" s="2">
         <v>0</v>
       </c>
-      <c r="U27" s="2">
+      <c r="AB27" s="2">
         <v>314</v>
       </c>
-      <c r="V27" s="2">
+      <c r="AC27" s="2">
         <v>536</v>
       </c>
-      <c r="W27" s="2">
+      <c r="AD27" s="2">
         <v>7</v>
       </c>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2">
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>857</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44729</v>
       </c>
@@ -9560,69 +9896,76 @@
       <c r="E28" s="2">
         <v>4585</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2">
         <v>1763</v>
       </c>
-      <c r="G28" s="2">
+      <c r="N28" s="2">
         <v>3627</v>
       </c>
-      <c r="H28" s="2">
+      <c r="O28" s="2">
         <v>61547</v>
       </c>
-      <c r="I28" s="2">
+      <c r="P28" s="2">
         <v>43284</v>
       </c>
-      <c r="J28" s="2">
+      <c r="Q28" s="2">
         <v>0</v>
       </c>
-      <c r="K28" s="2">
+      <c r="R28" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="2">
+      <c r="S28" s="2">
         <v>222</v>
       </c>
-      <c r="M28" s="2">
+      <c r="T28" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>222</v>
       </c>
-      <c r="N28" s="2">
+      <c r="U28" s="2">
         <v>0</v>
       </c>
-      <c r="O28" s="2">
+      <c r="V28" s="2">
         <v>159</v>
       </c>
-      <c r="P28" s="2">
+      <c r="W28" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q28" s="2">
+      <c r="X28" s="2">
         <v>133</v>
       </c>
-      <c r="R28" s="2">
+      <c r="Y28" s="2">
         <v>135</v>
       </c>
-      <c r="S28" s="2">
+      <c r="Z28" s="2">
         <v>4</v>
       </c>
-      <c r="T28" s="2">
+      <c r="AA28" s="2">
         <v>0</v>
       </c>
-      <c r="U28" s="2">
+      <c r="AB28" s="2">
         <v>316</v>
       </c>
-      <c r="V28" s="2">
+      <c r="AC28" s="2">
         <v>548</v>
       </c>
-      <c r="W28" s="2">
+      <c r="AD28" s="2">
         <v>7</v>
       </c>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2">
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>871</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44743</v>
       </c>
@@ -9638,69 +9981,76 @@
       <c r="E29" s="2">
         <v>4689</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2">
         <v>1773</v>
       </c>
-      <c r="G29" s="2">
+      <c r="N29" s="2">
         <v>3651</v>
       </c>
-      <c r="H29" s="2">
+      <c r="O29" s="2">
         <v>61778</v>
       </c>
-      <c r="I29" s="2">
+      <c r="P29" s="2">
         <v>43332</v>
       </c>
-      <c r="J29" s="2">
+      <c r="Q29" s="2">
         <v>0</v>
       </c>
-      <c r="K29" s="2">
+      <c r="R29" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="2">
+      <c r="S29" s="2">
         <v>222</v>
       </c>
-      <c r="M29" s="2">
+      <c r="T29" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>222</v>
       </c>
-      <c r="N29" s="2">
+      <c r="U29" s="2">
         <v>0</v>
       </c>
-      <c r="O29" s="2">
+      <c r="V29" s="2">
         <v>159</v>
       </c>
-      <c r="P29" s="2">
+      <c r="W29" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q29" s="2">
+      <c r="X29" s="2">
         <v>134</v>
       </c>
-      <c r="R29" s="2">
+      <c r="Y29" s="2">
         <v>137</v>
       </c>
-      <c r="S29" s="2">
+      <c r="Z29" s="2">
         <v>4</v>
       </c>
-      <c r="T29" s="2">
+      <c r="AA29" s="2">
         <v>0</v>
       </c>
-      <c r="U29" s="2">
+      <c r="AB29" s="2">
         <v>320</v>
       </c>
-      <c r="V29" s="2">
+      <c r="AC29" s="2">
         <v>568</v>
       </c>
-      <c r="W29" s="2">
+      <c r="AD29" s="2">
         <v>7</v>
       </c>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2">
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44748</v>
       </c>
@@ -9716,69 +10066,76 @@
       <c r="E30" s="2">
         <v>4712</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2">
         <v>1776</v>
       </c>
-      <c r="G30" s="2">
+      <c r="N30" s="2">
         <v>3662</v>
       </c>
-      <c r="H30" s="2">
+      <c r="O30" s="2">
         <v>61856</v>
       </c>
-      <c r="I30" s="2">
+      <c r="P30" s="2">
         <v>43366</v>
       </c>
-      <c r="J30" s="2">
+      <c r="Q30" s="2">
         <v>0</v>
       </c>
-      <c r="K30" s="2">
+      <c r="R30" s="2">
         <v>0</v>
       </c>
-      <c r="L30" s="2">
+      <c r="S30" s="2">
         <v>223</v>
       </c>
-      <c r="M30" s="2">
+      <c r="T30" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>223</v>
       </c>
-      <c r="N30" s="2">
+      <c r="U30" s="2">
         <v>0</v>
       </c>
-      <c r="O30" s="2">
+      <c r="V30" s="2">
         <v>159</v>
       </c>
-      <c r="P30" s="2">
+      <c r="W30" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q30" s="2">
+      <c r="X30" s="2">
         <v>134</v>
       </c>
-      <c r="R30" s="2">
+      <c r="Y30" s="2">
         <v>137</v>
       </c>
-      <c r="S30" s="2">
+      <c r="Z30" s="2">
         <v>4</v>
       </c>
-      <c r="T30" s="2">
+      <c r="AA30" s="2">
         <v>0</v>
       </c>
-      <c r="U30" s="2">
+      <c r="AB30" s="2">
         <v>320</v>
       </c>
-      <c r="V30" s="2">
+      <c r="AC30" s="2">
         <v>578</v>
       </c>
-      <c r="W30" s="2">
+      <c r="AD30" s="2">
         <v>7</v>
       </c>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2">
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>905</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44757</v>
       </c>
@@ -9794,66 +10151,173 @@
       <c r="E31" s="2">
         <v>4720</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2">
         <v>1782</v>
       </c>
-      <c r="G31" s="2">
+      <c r="N31" s="2">
         <v>3684</v>
       </c>
-      <c r="H31" s="2">
+      <c r="O31" s="2">
         <v>62189</v>
       </c>
-      <c r="I31" s="2">
+      <c r="P31" s="2">
         <v>43626</v>
       </c>
-      <c r="J31" s="2">
+      <c r="Q31" s="2">
         <v>0</v>
       </c>
-      <c r="K31" s="2">
+      <c r="R31" s="2">
         <v>0</v>
       </c>
-      <c r="L31" s="2">
+      <c r="S31" s="2">
         <v>224</v>
       </c>
-      <c r="M31" s="2">
+      <c r="T31" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>224</v>
       </c>
-      <c r="N31" s="2">
+      <c r="U31" s="2">
         <v>0</v>
       </c>
-      <c r="O31" s="2">
+      <c r="V31" s="2">
         <v>159</v>
       </c>
-      <c r="P31" s="2">
+      <c r="W31" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="Q31" s="2">
+      <c r="X31" s="2">
         <v>134</v>
       </c>
-      <c r="R31" s="2">
+      <c r="Y31" s="2">
         <v>138</v>
       </c>
-      <c r="S31" s="2">
+      <c r="Z31" s="2">
         <v>4</v>
       </c>
-      <c r="T31" s="2">
+      <c r="AA31" s="2">
         <v>0</v>
       </c>
-      <c r="U31" s="2">
+      <c r="AB31" s="2">
         <v>321</v>
       </c>
-      <c r="V31" s="2">
+      <c r="AC31" s="2">
         <v>593</v>
       </c>
-      <c r="W31" s="2">
+      <c r="AD31" s="2">
         <v>7</v>
       </c>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2">
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>921</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44761</v>
+      </c>
+      <c r="B32" s="2">
+        <v>105</v>
+      </c>
+      <c r="C32" s="2">
+        <v>240</v>
+      </c>
+      <c r="D32" s="2">
+        <v>193</v>
+      </c>
+      <c r="E32" s="2">
+        <v>4720</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5498</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1781</v>
+      </c>
+      <c r="H32" s="2">
+        <v>315</v>
+      </c>
+      <c r="I32" s="2">
+        <v>240</v>
+      </c>
+      <c r="J32" s="2">
+        <v>97</v>
+      </c>
+      <c r="K32" s="2">
+        <v>48</v>
+      </c>
+      <c r="L32" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>7979</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1782</v>
+      </c>
+      <c r="N32" s="2">
+        <v>3684</v>
+      </c>
+      <c r="O32" s="2">
+        <v>62189</v>
+      </c>
+      <c r="P32" s="2">
+        <v>43626</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>0</v>
+      </c>
+      <c r="R32" s="2">
+        <v>0</v>
+      </c>
+      <c r="S32" s="2">
+        <v>224</v>
+      </c>
+      <c r="T32" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>224</v>
+      </c>
+      <c r="U32" s="2">
+        <v>0</v>
+      </c>
+      <c r="V32" s="2">
+        <v>159</v>
+      </c>
+      <c r="W32" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>159</v>
+      </c>
+      <c r="X32" s="2">
+        <v>134</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>138</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>321</v>
+      </c>
+      <c r="AC32" s="2">
+        <v>595</v>
+      </c>
+      <c r="AD32" s="2">
+        <v>7</v>
+      </c>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the stats after release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD684C63-12B6-D94C-912D-EA52F816E83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B9348A-83D4-2447-9825-E8487F517EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -343,10 +343,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -442,16 +442,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$33</c:f>
+              <c:f>Data!$E$2:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -547,6 +550,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>4724</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,10 +592,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -685,16 +691,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$33</c:f>
+              <c:f>Data!$M$2:$M$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -790,6 +799,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>1785</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,10 +841,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -928,16 +940,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$33</c:f>
+              <c:f>Data!$N$2:$N$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1033,6 +1048,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>3689</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1288,10 +1306,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1387,16 +1405,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$33</c:f>
+              <c:f>Data!$R$2:$R$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1491,6 +1512,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1531,10 +1555,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1630,16 +1654,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$33</c:f>
+              <c:f>Data!$U$2:$U$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1734,6 +1761,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1774,10 +1804,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1873,16 +1903,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$33</c:f>
+              <c:f>Data!$Q$2:$Q$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1977,6 +2010,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2236,10 +2272,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2335,16 +2371,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$33</c:f>
+              <c:f>Data!$T$2:$T$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2440,6 +2479,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2479,10 +2521,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2578,16 +2620,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$33</c:f>
+              <c:f>Data!$W$2:$W$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2683,6 +2728,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2938,10 +2986,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3037,16 +3085,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$33</c:f>
+              <c:f>Data!$Y$2:$Y$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -3141,6 +3192,9 @@
                   <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
@@ -3363,10 +3417,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3462,16 +3516,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$33</c:f>
+              <c:f>Data!$AA$2:$AA$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3500,6 +3557,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3536,10 +3596,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3635,16 +3695,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$33</c:f>
+              <c:f>Data!$AB$2:$AB$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -3674,6 +3737,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3709,10 +3775,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3808,16 +3874,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$33</c:f>
+              <c:f>Data!$AC$2:$AC$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -3847,6 +3916,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>610</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3882,10 +3954,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3981,16 +4053,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$33</c:f>
+              <c:f>Data!$AD$2:$AD$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -4019,6 +4094,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4057,10 +4135,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$33</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4156,16 +4234,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$33</c:f>
+              <c:f>Data!$AE$2:$AE$34</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7404,8 +7485,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF33" totalsRowShown="0">
-  <autoFilter ref="A1:AF33" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF34" totalsRowShown="0">
+  <autoFilter ref="A1:AF34" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="30"/>
@@ -7749,11 +7830,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AF33"/>
+  <dimension ref="A1:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF33" sqref="AF33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10501,6 +10582,106 @@
         <v>927</v>
       </c>
     </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44768</v>
+      </c>
+      <c r="B34" s="2">
+        <v>106</v>
+      </c>
+      <c r="C34" s="2">
+        <v>241</v>
+      </c>
+      <c r="D34" s="2">
+        <v>194</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4731</v>
+      </c>
+      <c r="F34" s="2">
+        <v>5589</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1785</v>
+      </c>
+      <c r="H34" s="2">
+        <v>315</v>
+      </c>
+      <c r="I34" s="2">
+        <v>242</v>
+      </c>
+      <c r="J34" s="2">
+        <v>97</v>
+      </c>
+      <c r="K34" s="2">
+        <v>48</v>
+      </c>
+      <c r="L34" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8076</v>
+      </c>
+      <c r="M34" s="2">
+        <v>1789</v>
+      </c>
+      <c r="N34" s="2">
+        <v>3703</v>
+      </c>
+      <c r="O34" s="2">
+        <v>62262</v>
+      </c>
+      <c r="P34" s="2">
+        <v>43661</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>0</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0</v>
+      </c>
+      <c r="S34" s="2">
+        <v>225</v>
+      </c>
+      <c r="T34" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>225</v>
+      </c>
+      <c r="U34" s="2">
+        <v>0</v>
+      </c>
+      <c r="V34" s="2">
+        <v>160</v>
+      </c>
+      <c r="W34" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>160</v>
+      </c>
+      <c r="X34" s="2">
+        <v>136</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>138</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>322</v>
+      </c>
+      <c r="AC34" s="2">
+        <v>610</v>
+      </c>
+      <c r="AD34" s="2">
+        <v>7</v>
+      </c>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>939</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the statistics after publication of 2.37.0
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B9348A-83D4-2447-9825-E8487F517EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F29EAEB-E702-5C44-80C3-9F48A889F2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="31100" windowHeight="32860" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -343,10 +343,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -445,16 +445,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$34</c:f>
+              <c:f>Data!$E$2:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -553,6 +556,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>4731</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,10 +598,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -694,16 +700,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$34</c:f>
+              <c:f>Data!$M$2:$M$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -802,6 +811,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>1789</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,10 +853,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -943,16 +955,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$34</c:f>
+              <c:f>Data!$N$2:$N$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1051,6 +1066,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>3703</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,10 +1324,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1408,16 +1426,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$34</c:f>
+              <c:f>Data!$R$2:$R$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1515,6 +1536,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1555,10 +1579,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1657,16 +1681,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$34</c:f>
+              <c:f>Data!$U$2:$U$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1764,6 +1791,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1804,10 +1834,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1906,16 +1936,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$34</c:f>
+              <c:f>Data!$Q$2:$Q$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2013,6 +2046,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2272,10 +2308,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2374,16 +2410,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$34</c:f>
+              <c:f>Data!$T$2:$T$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2481,6 +2520,9 @@
                   <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
@@ -2521,10 +2563,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2623,16 +2665,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$34</c:f>
+              <c:f>Data!$W$2:$W$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2730,6 +2775,9 @@
                   <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
@@ -2986,10 +3034,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3088,16 +3136,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$34</c:f>
+              <c:f>Data!$Y$2:$Y$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -3196,6 +3247,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3417,10 +3471,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3519,16 +3573,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$34</c:f>
+              <c:f>Data!$AA$2:$AA$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3560,6 +3617,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3596,10 +3656,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3698,16 +3758,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$34</c:f>
+              <c:f>Data!$AB$2:$AB$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -3739,6 +3802,9 @@
                   <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>322</c:v>
                 </c:pt>
               </c:numCache>
@@ -3775,10 +3841,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3877,16 +3943,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$34</c:f>
+              <c:f>Data!$AC$2:$AC$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -3919,6 +3988,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3954,10 +4026,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4056,16 +4128,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$34</c:f>
+              <c:f>Data!$AD$2:$AD$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -4097,6 +4172,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4135,10 +4213,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4237,16 +4315,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$34</c:f>
+              <c:f>Data!$AE$2:$AE$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7268,7 +7349,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7279,7 +7360,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{24ACA0B5-B5F6-0649-9568-624D24B93699}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7290,7 +7371,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{50B1BB8B-A1E8-FB42-B88F-023CE9967AAB}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7301,7 +7382,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B111F3D3-9A19-164A-A80F-5E41AF9CF1E4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7312,7 +7393,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{5B2EC930-5C2E-4448-96C6-E1C9EC4CF674}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7323,7 +7404,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6077857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7356,7 +7437,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6077857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7389,7 +7470,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6077857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7422,7 +7503,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6077857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7455,7 +7536,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6077857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7485,8 +7566,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF34" totalsRowShown="0">
-  <autoFilter ref="A1:AF34" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF35" totalsRowShown="0">
+  <autoFilter ref="A1:AF35" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="31"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="30"/>
@@ -7830,11 +7911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AF34"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF34" sqref="AF34"/>
+      <selection pane="bottomLeft" activeCell="AE35" sqref="AE35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10656,7 +10737,7 @@
         <v>160</v>
       </c>
       <c r="X34" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Y34" s="2">
         <v>138</v>
@@ -10680,6 +10761,106 @@
       <c r="AF34" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>939</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44790</v>
+      </c>
+      <c r="B35" s="2">
+        <v>106</v>
+      </c>
+      <c r="C35" s="2">
+        <v>242</v>
+      </c>
+      <c r="D35" s="2">
+        <v>195</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4749</v>
+      </c>
+      <c r="F35" s="2">
+        <v>5535</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1788</v>
+      </c>
+      <c r="H35" s="2">
+        <v>315</v>
+      </c>
+      <c r="I35" s="2">
+        <v>243</v>
+      </c>
+      <c r="J35" s="2">
+        <v>97</v>
+      </c>
+      <c r="K35" s="2">
+        <v>48</v>
+      </c>
+      <c r="L35" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8026</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1791</v>
+      </c>
+      <c r="N35" s="2">
+        <v>3716</v>
+      </c>
+      <c r="O35" s="2">
+        <v>62325</v>
+      </c>
+      <c r="P35" s="2">
+        <v>43671</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>0</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0</v>
+      </c>
+      <c r="S35" s="2">
+        <v>225</v>
+      </c>
+      <c r="T35" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>225</v>
+      </c>
+      <c r="U35" s="2">
+        <v>0</v>
+      </c>
+      <c r="V35" s="2">
+        <v>160</v>
+      </c>
+      <c r="W35" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>160</v>
+      </c>
+      <c r="X35" s="2">
+        <v>136</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>140</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>322</v>
+      </c>
+      <c r="AC35" s="2">
+        <v>618</v>
+      </c>
+      <c r="AD35" s="2">
+        <v>7</v>
+      </c>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the statistics after the new release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F29EAEB-E702-5C44-80C3-9F48A889F2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1800265E-F5BC-7B4D-889F-095CCD619523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="31100" windowHeight="32860" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24540" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -137,11 +137,20 @@
   <si>
     <t>Total2</t>
   </si>
+  <si>
+    <t>∆LoC</t>
+  </si>
+  <si>
+    <t>∆Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\+#,##0;\-#,##0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -177,15 +186,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="\+#,##0;\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="\+#,##0;\-#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -343,10 +359,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -448,16 +464,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$35</c:f>
+              <c:f>Data!$E$2:$E$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -559,6 +578,9 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>4749</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4762</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,7 +597,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$M$1</c:f>
+              <c:f>Data!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -598,10 +620,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -703,16 +725,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$M$2:$M$35</c:f>
+              <c:f>Data!$O$2:$O$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -830,7 +855,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$N$1</c:f>
+              <c:f>Data!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -853,10 +878,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -958,16 +983,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$N$2:$N$35</c:f>
+              <c:f>Data!$P$2:$P$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1301,7 +1329,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$R$1</c:f>
+              <c:f>Data!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1324,10 +1352,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1429,16 +1457,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$35</c:f>
+              <c:f>Data!$T$2:$T$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1556,7 +1587,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$U$1</c:f>
+              <c:f>Data!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1579,10 +1610,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1684,16 +1715,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$35</c:f>
+              <c:f>Data!$W$2:$W$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1811,7 +1845,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$Q$1</c:f>
+              <c:f>Data!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1834,10 +1868,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1939,16 +1973,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$35</c:f>
+              <c:f>Data!$S$2:$S$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2285,7 +2322,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$T$1</c:f>
+              <c:f>Data!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2308,10 +2345,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2413,16 +2450,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$35</c:f>
+              <c:f>Data!$V$2:$V$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2524,6 +2564,9 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2540,7 +2583,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$W$1</c:f>
+              <c:f>Data!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2563,10 +2606,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2668,16 +2711,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$35</c:f>
+              <c:f>Data!$Y$2:$Y$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -2779,6 +2825,9 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3011,7 +3060,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$Y$1</c:f>
+              <c:f>Data!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3034,10 +3083,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3139,16 +3188,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$35</c:f>
+              <c:f>Data!$AA$2:$AA$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -3451,7 +3503,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AA$1</c:f>
+              <c:f>Data!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3471,10 +3523,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3576,16 +3628,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$35</c:f>
+              <c:f>Data!$AC$2:$AC$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3636,7 +3691,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AB$1</c:f>
+              <c:f>Data!$AD$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3656,10 +3711,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3761,16 +3816,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$35</c:f>
+              <c:f>Data!$AD$2:$AD$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -3821,7 +3879,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AC$1</c:f>
+              <c:f>Data!$AE$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3841,10 +3899,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3946,16 +4004,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$35</c:f>
+              <c:f>Data!$AE$2:$AE$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -4006,7 +4067,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AD$1</c:f>
+              <c:f>Data!$AF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4026,10 +4087,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4131,16 +4192,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$35</c:f>
+              <c:f>Data!$AF$2:$AF$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -4191,7 +4255,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AE$1</c:f>
+              <c:f>Data!$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4213,10 +4277,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$35</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4318,16 +4382,19 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$35</c:f>
+              <c:f>Data!$AG$2:$AG$36</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7566,47 +7633,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AF35" totalsRowShown="0">
-  <autoFilter ref="A1:AF35" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
-  <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="27"/>
-    <tableColumn id="26" xr3:uid="{EA0BB0A1-B927-BA42-95D8-323FF0F98170}" name="Shell" dataDxfId="26"/>
-    <tableColumn id="27" xr3:uid="{044A9D24-EDBD-814E-8836-3A4FC1DAF6CD}" name="MD" dataDxfId="25"/>
-    <tableColumn id="28" xr3:uid="{7634D894-69D0-B844-B715-963F9BC2312D}" name="YAML" dataDxfId="24"/>
-    <tableColumn id="29" xr3:uid="{35076C74-15AC-EC42-A3FA-C7C55763EEA7}" name="Text" dataDxfId="23"/>
-    <tableColumn id="30" xr3:uid="{1A9EAD82-A8B4-184C-92DB-650EA2147810}" name="make" dataDxfId="22"/>
-    <tableColumn id="31" xr3:uid="{F5568E37-EB5F-0B40-B8FE-3BC68D2DEFB3}" name="Bash" dataDxfId="21"/>
-    <tableColumn id="32" xr3:uid="{74A04583-DF3F-244E-8F76-155696F8B4E4}" name="Total" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH36" totalsRowShown="0">
+  <autoFilter ref="A1:AH36" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{9D977A2F-FBC7-9444-809F-55429A0A93FA}" name="Versions" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{50EF9E4F-56ED-AE43-9F2C-3273E23CA123}" name="GH Releases" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{7A031666-B40E-9C44-B04D-F85418485CE9}" name="LoC" dataDxfId="29"/>
+    <tableColumn id="33" xr3:uid="{314C5206-2A7B-F841-94C2-27E5FA3210D6}" name="∆LoC" dataDxfId="1">
+      <calculatedColumnFormula>Data[[#This Row],[LoC]]-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{EA0BB0A1-B927-BA42-95D8-323FF0F98170}" name="Shell" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{044A9D24-EDBD-814E-8836-3A4FC1DAF6CD}" name="MD" dataDxfId="27"/>
+    <tableColumn id="28" xr3:uid="{7634D894-69D0-B844-B715-963F9BC2312D}" name="YAML" dataDxfId="26"/>
+    <tableColumn id="29" xr3:uid="{35076C74-15AC-EC42-A3FA-C7C55763EEA7}" name="Text" dataDxfId="25"/>
+    <tableColumn id="30" xr3:uid="{1A9EAD82-A8B4-184C-92DB-650EA2147810}" name="make" dataDxfId="24"/>
+    <tableColumn id="31" xr3:uid="{F5568E37-EB5F-0B40-B8FE-3BC68D2DEFB3}" name="Bash" dataDxfId="23"/>
+    <tableColumn id="32" xr3:uid="{74A04583-DF3F-244E-8F76-155696F8B4E4}" name="Total" dataDxfId="22">
       <calculatedColumnFormula>SUM(Data[[#This Row],[Shell]:[Bash]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="12">
+    <tableColumn id="34" xr3:uid="{FD44257B-EFD4-EF46-B0EE-B5B6EBB0D9D7}" name="∆Total" dataDxfId="0">
+      <calculatedColumnFormula>Data[[#This Row],[Total]]-M1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{209B02FE-4C5E-A34D-8A40-FEEE65FDC588}" name="Commits" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{5F63508D-C840-F54A-8A71-C80EA9D4AD88}" name="File Changes" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{54572B04-73DF-B54E-8CA8-08B855E57298}" name="Insertions" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{5B41BC3F-409E-3E48-ACF0-FB5B2991C84B}" name="Deletions" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{1C05E18A-C711-644C-80DB-657BE50D2023}" name="Open issues" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{B8CD0192-45D4-214D-A61D-035F6343DBF3}" name="Open bugs" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{C647B025-84B9-2A4A-A39F-474FCCC1A725}" name="Closed issues" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{5358541A-D71D-924E-B96F-092E458438D7}" name="Issues" dataDxfId="14">
       <calculatedColumnFormula>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="9">
+    <tableColumn id="13" xr3:uid="{4328C74F-4512-BC47-A624-E12D52DA1C64}" name="Open pull requests" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{B0E7CD5E-8EFD-0845-8464-DDA5DB404F1A}" name="Closed pull requests" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{5AC2FAE8-07F8-0C4D-B5FE-D75B75751C52}" name="Pull requests" dataDxfId="11">
       <calculatedColumnFormula>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{67D9B221-0B31-4848-8615-FFAA31A553EC}" name="Running" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{EDC0224F-D9E5-6F46-A4AD-E4CCACBEC828}" name="Failed" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{10E4F180-ED15-E849-B5B3-B50AD4FD7CE9}" name="OK" dataDxfId="3"/>
-    <tableColumn id="24" xr3:uid="{41B7AB09-D6AC-6945-B9EC-BB3EC1357064}" name="Cancelled" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{B9A99AA7-42FD-D344-A29E-4499FB1F8CE3}" name="Total2" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{90523CC0-E84C-064F-9345-04A52C3C2A93}" name="Command line options" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{775D40B7-33AD-894D-A997-09D0BCFA826F}" name="Tests" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{0DCC1450-6CC4-E146-A105-3B45157DE09A}" name="GH workflows" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{67D9B221-0B31-4848-8615-FFAA31A553EC}" name="Running" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{EDC0224F-D9E5-6F46-A4AD-E4CCACBEC828}" name="Failed" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{10E4F180-ED15-E849-B5B3-B50AD4FD7CE9}" name="OK" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{41B7AB09-D6AC-6945-B9EC-BB3EC1357064}" name="Cancelled" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{45136596-751E-4E4D-93FD-EBC25B854FA5}" name="GH runs" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{B9A99AA7-42FD-D344-A29E-4499FB1F8CE3}" name="Total2" dataDxfId="2">
       <calculatedColumnFormula>SUM(Data[[#This Row],[Running]:[GH runs]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7911,11 +7984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE35" sqref="AE35"/>
+      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7925,29 +7998,31 @@
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="6.5" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5" customWidth="1"/>
-    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="6.5" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" customWidth="1"/>
+    <col min="26" max="26" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7964,88 +8039,94 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>16</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44574</v>
       </c>
@@ -8061,70 +8142,76 @@
       <c r="E2" s="2">
         <v>4368</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2">
+      <c r="M2" s="2"/>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
         <v>1523</v>
       </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>3195</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>57442</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <v>40634</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="S2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
         <v>203</v>
       </c>
-      <c r="T2" s="2">
+      <c r="V2" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
         <v>135</v>
       </c>
-      <c r="W2" s="2">
+      <c r="Y2" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Z2" s="2">
         <v>125</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="AA2" s="2">
         <v>122</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AB2" s="2">
         <v>2</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" s="2">
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2">
         <v>541</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AH2" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44578</v>
       </c>
@@ -8140,70 +8227,78 @@
       <c r="E3" s="2">
         <v>4368</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3">
+        <f>Data[[#This Row],[LoC]]-E2</f>
+        <v>0</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2">
+      <c r="M3" s="2"/>
+      <c r="N3" s="3">
+        <f>Data[[#This Row],[Total]]-M2</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
         <v>1524</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>3196</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>57422</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <v>40034</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="S3" s="2">
         <v>1</v>
       </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
         <v>203</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2">
         <v>135</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Z3" s="2">
         <v>125</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AA3" s="2">
         <v>122</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AB3" s="2">
         <v>2</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="2">
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2">
         <v>542</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AH3" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>542</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44580</v>
       </c>
@@ -8219,70 +8314,78 @@
       <c r="E4" s="2">
         <v>4368</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="3">
+        <f>Data[[#This Row],[LoC]]-E3</f>
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3">
+        <f>Data[[#This Row],[Total]]-M3</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
         <v>1525</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>3197</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <v>57422</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R4" s="2">
         <v>40634</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="S4" s="2">
         <v>1</v>
       </c>
-      <c r="R4" s="2">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
         <v>203</v>
       </c>
-      <c r="T4" s="2">
+      <c r="V4" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U4" s="2">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
         <v>135</v>
       </c>
-      <c r="W4" s="2">
+      <c r="Y4" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Z4" s="2">
         <v>125</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="AA4" s="2">
         <v>122</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AB4" s="2">
         <v>2</v>
       </c>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="2">
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2">
         <v>543</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AH4" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44588</v>
       </c>
@@ -8298,70 +8401,78 @@
       <c r="E5" s="2">
         <v>4368</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="3">
+        <f>Data[[#This Row],[LoC]]-E4</f>
+        <v>0</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2">
+      <c r="M5" s="2"/>
+      <c r="N5" s="3">
+        <f>Data[[#This Row],[Total]]-M4</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
         <v>1531</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>3207</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>57794</v>
       </c>
-      <c r="P5" s="2">
+      <c r="R5" s="2">
         <v>40652</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="S5" s="2">
         <v>1</v>
       </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
         <v>203</v>
       </c>
-      <c r="T5" s="2">
+      <c r="V5" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
         <v>135</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Z5" s="2">
         <v>125</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="AA5" s="2">
         <v>122</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AB5" s="2">
         <v>3</v>
       </c>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="2">
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2">
         <v>550</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AH5" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44593</v>
       </c>
@@ -8377,70 +8488,78 @@
       <c r="E6" s="2">
         <v>4379</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="3">
+        <f>Data[[#This Row],[LoC]]-E5</f>
+        <v>11</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2">
+      <c r="M6" s="2"/>
+      <c r="N6" s="3">
+        <f>Data[[#This Row],[Total]]-M5</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
         <v>1539</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>3224</v>
       </c>
-      <c r="O6" s="2">
+      <c r="Q6" s="2">
         <v>57859</v>
       </c>
-      <c r="P6" s="2">
+      <c r="R6" s="2">
         <v>40677</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="S6" s="2">
         <v>1</v>
       </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
         <v>203</v>
       </c>
-      <c r="T6" s="2">
+      <c r="V6" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
         <v>135</v>
       </c>
-      <c r="W6" s="2">
+      <c r="Y6" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Z6" s="2">
         <v>125</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="AA6" s="2">
         <v>122</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AB6" s="2">
         <v>3</v>
       </c>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="2">
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2">
         <v>561</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AH6" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>561</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44602</v>
       </c>
@@ -8456,70 +8575,78 @@
       <c r="E7" s="2">
         <v>4381</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="3">
+        <f>Data[[#This Row],[LoC]]-E6</f>
+        <v>2</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2">
+      <c r="M7" s="2"/>
+      <c r="N7" s="3">
+        <f>Data[[#This Row],[Total]]-M6</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
         <v>1559</v>
       </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2">
         <v>3265</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>58868</v>
       </c>
-      <c r="P7" s="2">
+      <c r="R7" s="2">
         <v>41555</v>
       </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0</v>
-      </c>
       <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
         <v>204</v>
       </c>
-      <c r="T7" s="2">
+      <c r="V7" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>204</v>
       </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
         <v>135</v>
       </c>
-      <c r="W7" s="2">
+      <c r="Y7" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Z7" s="2">
         <v>125</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="AA7" s="2">
         <v>122</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AB7" s="2">
         <v>3</v>
       </c>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="2">
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2">
         <v>586</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AH7" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>586</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44610</v>
       </c>
@@ -8535,70 +8662,78 @@
       <c r="E8" s="2">
         <v>4399</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="3">
+        <f>Data[[#This Row],[LoC]]-E7</f>
+        <v>18</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2">
+      <c r="M8" s="2"/>
+      <c r="N8" s="3">
+        <f>Data[[#This Row],[Total]]-M7</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
         <v>1568</v>
       </c>
-      <c r="N8" s="2">
+      <c r="P8" s="2">
         <v>3286</v>
       </c>
-      <c r="O8" s="2">
+      <c r="Q8" s="2">
         <v>58985</v>
       </c>
-      <c r="P8" s="2">
+      <c r="R8" s="2">
         <v>41600</v>
       </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
-        <v>0</v>
-      </c>
       <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
         <v>208</v>
       </c>
-      <c r="T8" s="2">
+      <c r="V8" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>208</v>
       </c>
-      <c r="U8" s="2">
-        <v>0</v>
-      </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
         <v>135</v>
       </c>
-      <c r="W8" s="2">
+      <c r="Y8" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Z8" s="2">
         <v>125</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="AA8" s="2">
         <v>122</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AB8" s="2">
         <v>3</v>
       </c>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="2">
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2">
         <v>595</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AH8" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44613</v>
       </c>
@@ -8614,70 +8749,78 @@
       <c r="E9" s="2">
         <v>4413</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3">
+        <f>Data[[#This Row],[LoC]]-E8</f>
+        <v>14</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2">
+      <c r="M9" s="2"/>
+      <c r="N9" s="3">
+        <f>Data[[#This Row],[Total]]-M8</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
         <v>1571</v>
       </c>
-      <c r="N9" s="2">
+      <c r="P9" s="2">
         <v>3298</v>
       </c>
-      <c r="O9" s="2">
+      <c r="Q9" s="2">
         <v>59170</v>
       </c>
-      <c r="P9" s="2">
+      <c r="R9" s="2">
         <v>41754</v>
       </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
-        <v>0</v>
-      </c>
       <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
         <v>208</v>
       </c>
-      <c r="T9" s="2">
+      <c r="V9" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>208</v>
       </c>
-      <c r="U9" s="2">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
         <v>135</v>
       </c>
-      <c r="W9" s="2">
+      <c r="Y9" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>135</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Z9" s="2">
         <v>126</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="AA9" s="2">
         <v>122</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AB9" s="2">
         <v>3</v>
       </c>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="2">
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2">
         <v>601</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AH9" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>601</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44636</v>
       </c>
@@ -8693,70 +8836,78 @@
       <c r="E10" s="2">
         <v>4430</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="3">
+        <f>Data[[#This Row],[LoC]]-E9</f>
+        <v>17</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2">
+      <c r="M10" s="2"/>
+      <c r="N10" s="3">
+        <f>Data[[#This Row],[Total]]-M9</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
         <v>1598</v>
       </c>
-      <c r="N10" s="2">
+      <c r="P10" s="2">
         <v>3339</v>
       </c>
-      <c r="O10" s="2">
+      <c r="Q10" s="2">
         <v>59371</v>
       </c>
-      <c r="P10" s="2">
+      <c r="R10" s="2">
         <v>41908</v>
       </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
       <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
         <v>209</v>
       </c>
-      <c r="T10" s="2">
+      <c r="V10" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>209</v>
       </c>
-      <c r="U10" s="2">
-        <v>0</v>
-      </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2">
         <v>141</v>
       </c>
-      <c r="W10" s="2">
+      <c r="Y10" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>141</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Z10" s="2">
         <v>126</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="AA10" s="2">
         <v>122</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AB10" s="2">
         <v>3</v>
       </c>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="2">
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2">
         <v>632</v>
       </c>
-      <c r="AF10" s="2">
+      <c r="AH10" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>632</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44645</v>
       </c>
@@ -8772,70 +8923,78 @@
       <c r="E11" s="2">
         <v>4432</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="3">
+        <f>Data[[#This Row],[LoC]]-E10</f>
+        <v>2</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2">
+      <c r="M11" s="2"/>
+      <c r="N11" s="3">
+        <f>Data[[#This Row],[Total]]-M10</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
         <v>1627</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>3375</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <v>59655</v>
       </c>
-      <c r="P11" s="2">
+      <c r="R11" s="2">
         <v>42123</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="S11" s="2">
         <v>1</v>
       </c>
-      <c r="R11" s="2">
+      <c r="T11" s="2">
         <v>1</v>
       </c>
-      <c r="S11" s="2">
+      <c r="U11" s="2">
         <v>214</v>
       </c>
-      <c r="T11" s="2">
+      <c r="V11" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="U11" s="2">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
         <v>148</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y11" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Z11" s="2">
         <v>127</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AA11" s="2">
         <v>128</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AB11" s="2">
         <v>3</v>
       </c>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="2">
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2">
         <v>661</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="AH11" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>661</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44657</v>
       </c>
@@ -8851,70 +9010,78 @@
       <c r="E12" s="2">
         <v>4434</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="3">
+        <f>Data[[#This Row],[LoC]]-E11</f>
+        <v>2</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2">
+      <c r="M12" s="2"/>
+      <c r="N12" s="3">
+        <f>Data[[#This Row],[Total]]-M11</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
         <v>1632</v>
       </c>
-      <c r="N12" s="2">
+      <c r="P12" s="2">
         <v>3387</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <v>59702</v>
       </c>
-      <c r="P12" s="2">
+      <c r="R12" s="2">
         <v>42156</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="S12" s="2">
         <v>1</v>
       </c>
-      <c r="R12" s="2">
+      <c r="T12" s="2">
         <v>1</v>
       </c>
-      <c r="S12" s="2">
+      <c r="U12" s="2">
         <v>214</v>
       </c>
-      <c r="T12" s="2">
+      <c r="V12" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="U12" s="2">
-        <v>0</v>
-      </c>
-      <c r="V12" s="2">
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
         <v>148</v>
       </c>
-      <c r="W12" s="2">
+      <c r="Y12" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="X12" s="2">
+      <c r="Z12" s="2">
         <v>127</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="AA12" s="2">
         <v>131</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AB12" s="2">
         <v>3</v>
       </c>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="2">
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2">
         <v>669</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="AH12" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>669</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44664</v>
       </c>
@@ -8930,70 +9097,78 @@
       <c r="E13" s="2">
         <v>4454</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="3">
+        <f>Data[[#This Row],[LoC]]-E12</f>
+        <v>20</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2">
+      <c r="M13" s="2"/>
+      <c r="N13" s="3">
+        <f>Data[[#This Row],[Total]]-M12</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
         <v>1637</v>
       </c>
-      <c r="N13" s="2">
+      <c r="P13" s="2">
         <v>3406</v>
       </c>
-      <c r="O13" s="2">
+      <c r="Q13" s="2">
         <v>60308</v>
       </c>
-      <c r="P13" s="2">
+      <c r="R13" s="2">
         <v>42743</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="S13" s="2">
         <v>1</v>
       </c>
-      <c r="R13" s="2">
+      <c r="T13" s="2">
         <v>1</v>
       </c>
-      <c r="S13" s="2">
+      <c r="U13" s="2">
         <v>214</v>
       </c>
-      <c r="T13" s="2">
+      <c r="V13" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>215</v>
       </c>
-      <c r="U13" s="2">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2">
+      <c r="W13" s="2">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
         <v>148</v>
       </c>
-      <c r="W13" s="2">
+      <c r="Y13" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Z13" s="2">
         <v>128</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="AA13" s="2">
         <v>131</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AB13" s="2">
         <v>3</v>
       </c>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
-      <c r="AE13" s="2">
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2">
         <v>677</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AH13" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>677</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44676</v>
       </c>
@@ -9009,70 +9184,78 @@
       <c r="E14" s="2">
         <v>4453</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="3">
+        <f>Data[[#This Row],[LoC]]-E13</f>
+        <v>-1</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="3">
+        <f>Data[[#This Row],[Total]]-M13</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
         <v>1647</v>
       </c>
-      <c r="N14" s="2">
+      <c r="P14" s="2">
         <v>3424</v>
       </c>
-      <c r="O14" s="2">
+      <c r="Q14" s="2">
         <v>60352</v>
       </c>
-      <c r="P14" s="2">
+      <c r="R14" s="2">
         <v>42776</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="S14" s="2">
         <v>2</v>
       </c>
-      <c r="R14" s="2">
+      <c r="T14" s="2">
         <v>2</v>
       </c>
-      <c r="S14" s="2">
+      <c r="U14" s="2">
         <v>215</v>
       </c>
-      <c r="T14" s="2">
+      <c r="V14" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>217</v>
       </c>
-      <c r="U14" s="2">
-        <v>0</v>
-      </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
+        <v>0</v>
+      </c>
+      <c r="X14" s="2">
         <v>148</v>
       </c>
-      <c r="W14" s="2">
+      <c r="Y14" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>148</v>
       </c>
-      <c r="X14" s="2">
+      <c r="Z14" s="2">
         <v>128</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="AA14" s="2">
         <v>131</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AB14" s="2">
         <v>3</v>
       </c>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
-      <c r="AE14" s="2">
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2">
         <v>685</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="AH14" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>685</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44678</v>
       </c>
@@ -9088,70 +9271,78 @@
       <c r="E15" s="2">
         <v>4461</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="3">
+        <f>Data[[#This Row],[LoC]]-E14</f>
+        <v>8</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2">
+      <c r="M15" s="2"/>
+      <c r="N15" s="3">
+        <f>Data[[#This Row],[Total]]-M14</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
         <v>1652</v>
       </c>
-      <c r="N15" s="2">
+      <c r="P15" s="2">
         <v>3430</v>
       </c>
-      <c r="O15" s="2">
+      <c r="Q15" s="2">
         <v>60372</v>
       </c>
-      <c r="P15" s="2">
+      <c r="R15" s="2">
         <v>42778</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="S15" s="2">
         <v>1</v>
       </c>
-      <c r="R15" s="2">
+      <c r="T15" s="2">
         <v>1</v>
       </c>
-      <c r="S15" s="2">
+      <c r="U15" s="2">
         <v>216</v>
       </c>
-      <c r="T15" s="2">
+      <c r="V15" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>217</v>
       </c>
-      <c r="U15" s="2">
-        <v>0</v>
-      </c>
-      <c r="V15" s="2">
+      <c r="W15" s="2">
+        <v>0</v>
+      </c>
+      <c r="X15" s="2">
         <v>149</v>
       </c>
-      <c r="W15" s="2">
+      <c r="Y15" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="X15" s="2">
+      <c r="Z15" s="2">
         <v>128</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="AA15" s="2">
         <v>131</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AB15" s="2">
         <v>3</v>
       </c>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="2">
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2">
         <v>690</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AH15" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>690</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44679</v>
       </c>
@@ -9167,70 +9358,78 @@
       <c r="E16" s="2">
         <v>4462</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="3">
+        <f>Data[[#This Row],[LoC]]-E15</f>
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="2">
+      <c r="M16" s="2"/>
+      <c r="N16" s="3">
+        <f>Data[[#This Row],[Total]]-M15</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
         <v>1660</v>
       </c>
-      <c r="N16" s="2">
+      <c r="P16" s="2">
         <v>3444</v>
       </c>
-      <c r="O16" s="2">
+      <c r="Q16" s="2">
         <v>60431</v>
       </c>
-      <c r="P16" s="2">
+      <c r="R16" s="2">
         <v>42791</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="S16" s="2">
         <v>1</v>
       </c>
-      <c r="R16" s="2">
+      <c r="T16" s="2">
         <v>1</v>
       </c>
-      <c r="S16" s="2">
+      <c r="U16" s="2">
         <v>217</v>
       </c>
-      <c r="T16" s="2">
+      <c r="V16" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>218</v>
       </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2">
         <v>149</v>
       </c>
-      <c r="W16" s="2">
+      <c r="Y16" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="X16" s="2">
+      <c r="Z16" s="2">
         <v>128</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="AA16" s="2">
         <v>132</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AB16" s="2">
         <v>3</v>
       </c>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="2">
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2">
         <v>700</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AH16" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>700</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44686</v>
       </c>
@@ -9246,70 +9445,78 @@
       <c r="E17" s="2">
         <v>4454</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="3">
+        <f>Data[[#This Row],[LoC]]-E16</f>
+        <v>-8</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2">
+      <c r="M17" s="2"/>
+      <c r="N17" s="3">
+        <f>Data[[#This Row],[Total]]-M16</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
         <v>1670</v>
       </c>
-      <c r="N17" s="2">
+      <c r="P17" s="2">
         <v>3473</v>
       </c>
-      <c r="O17" s="2">
+      <c r="Q17" s="2">
         <v>60537</v>
       </c>
-      <c r="P17" s="2">
+      <c r="R17" s="2">
         <v>42889</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="S17" s="2">
         <v>1</v>
       </c>
-      <c r="R17" s="2">
+      <c r="T17" s="2">
         <v>1</v>
       </c>
-      <c r="S17" s="2">
+      <c r="U17" s="2">
         <v>218</v>
       </c>
-      <c r="T17" s="2">
+      <c r="V17" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="U17" s="2">
-        <v>0</v>
-      </c>
-      <c r="V17" s="2">
+      <c r="W17" s="2">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2">
         <v>149</v>
       </c>
-      <c r="W17" s="2">
+      <c r="Y17" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>149</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Z17" s="2">
         <v>128</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="AA17" s="2">
         <v>132</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AB17" s="2">
         <v>3</v>
       </c>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="2">
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2">
         <v>714</v>
       </c>
-      <c r="AF17" s="2">
+      <c r="AH17" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>714</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44691</v>
       </c>
@@ -9325,70 +9532,78 @@
       <c r="E18" s="2">
         <v>4454</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="3">
+        <f>Data[[#This Row],[LoC]]-E17</f>
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2">
+      <c r="M18" s="2"/>
+      <c r="N18" s="3">
+        <f>Data[[#This Row],[Total]]-M17</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
         <v>1676</v>
       </c>
-      <c r="N18" s="2">
+      <c r="P18" s="2">
         <v>3481</v>
       </c>
-      <c r="O18" s="2">
+      <c r="Q18" s="2">
         <v>60564</v>
       </c>
-      <c r="P18" s="2">
+      <c r="R18" s="2">
         <v>42903</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="S18" s="2">
         <v>1</v>
       </c>
-      <c r="R18" s="2">
+      <c r="T18" s="2">
         <v>1</v>
       </c>
-      <c r="S18" s="2">
+      <c r="U18" s="2">
         <v>218</v>
       </c>
-      <c r="T18" s="2">
+      <c r="V18" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="U18" s="2">
-        <v>0</v>
-      </c>
-      <c r="V18" s="2">
+      <c r="W18" s="2">
+        <v>0</v>
+      </c>
+      <c r="X18" s="2">
         <v>150</v>
       </c>
-      <c r="W18" s="2">
+      <c r="Y18" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>150</v>
       </c>
-      <c r="X18" s="2">
+      <c r="Z18" s="2">
         <v>128</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="AA18" s="2">
         <v>132</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="AB18" s="2">
         <v>3</v>
       </c>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
-      <c r="AE18" s="2">
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2">
         <v>721</v>
       </c>
-      <c r="AF18" s="2">
+      <c r="AH18" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>721</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44705</v>
       </c>
@@ -9404,70 +9619,78 @@
       <c r="E19" s="2">
         <v>4470</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="3">
+        <f>Data[[#This Row],[LoC]]-E18</f>
+        <v>16</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2">
+      <c r="M19" s="2"/>
+      <c r="N19" s="3">
+        <f>Data[[#This Row],[Total]]-M18</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
         <v>1695</v>
       </c>
-      <c r="N19" s="2">
+      <c r="P19" s="2">
         <v>3500</v>
       </c>
-      <c r="O19" s="2">
+      <c r="Q19" s="2">
         <v>60613</v>
       </c>
-      <c r="P19" s="2">
+      <c r="R19" s="2">
         <v>42943</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="S19" s="2">
         <v>1</v>
       </c>
-      <c r="R19" s="2">
+      <c r="T19" s="2">
         <v>1</v>
       </c>
-      <c r="S19" s="2">
+      <c r="U19" s="2">
         <v>218</v>
       </c>
-      <c r="T19" s="2">
+      <c r="V19" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>219</v>
       </c>
-      <c r="U19" s="2">
+      <c r="W19" s="2">
         <v>2</v>
       </c>
-      <c r="V19" s="2">
+      <c r="X19" s="2">
         <v>154</v>
       </c>
-      <c r="W19" s="2">
+      <c r="Y19" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="X19" s="2">
+      <c r="Z19" s="2">
         <v>128</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="AA19" s="2">
         <v>131</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AB19" s="2">
         <v>4</v>
       </c>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="2">
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2">
         <v>748</v>
       </c>
-      <c r="AF19" s="2">
+      <c r="AH19" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>748</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44707</v>
       </c>
@@ -9483,70 +9706,78 @@
       <c r="E20" s="2">
         <v>4506</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="3">
+        <f>Data[[#This Row],[LoC]]-E19</f>
+        <v>36</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2">
+      <c r="M20" s="2"/>
+      <c r="N20" s="3">
+        <f>Data[[#This Row],[Total]]-M19</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
         <v>1699</v>
       </c>
-      <c r="N20" s="2">
+      <c r="P20" s="2">
         <v>3520</v>
       </c>
-      <c r="O20" s="2">
+      <c r="Q20" s="2">
         <v>60719</v>
       </c>
-      <c r="P20" s="2">
+      <c r="R20" s="2">
         <v>42953</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="S20" s="2">
         <v>1</v>
       </c>
-      <c r="R20" s="2">
+      <c r="T20" s="2">
         <v>1</v>
       </c>
-      <c r="S20" s="2">
+      <c r="U20" s="2">
         <v>219</v>
       </c>
-      <c r="T20" s="2">
+      <c r="V20" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="U20" s="2">
+      <c r="W20" s="2">
         <v>1</v>
       </c>
-      <c r="V20" s="2">
+      <c r="X20" s="2">
         <v>155</v>
       </c>
-      <c r="W20" s="2">
+      <c r="Y20" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="X20" s="2">
+      <c r="Z20" s="2">
         <v>131</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="AA20" s="2">
         <v>132</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AB20" s="2">
         <v>4</v>
       </c>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
-      <c r="AE20" s="2">
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2">
         <v>754</v>
       </c>
-      <c r="AF20" s="2">
+      <c r="AH20" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44710</v>
       </c>
@@ -9562,70 +9793,78 @@
       <c r="E21" s="2">
         <v>4504</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="3">
+        <f>Data[[#This Row],[LoC]]-E20</f>
+        <v>-2</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2">
+      <c r="M21" s="2"/>
+      <c r="N21" s="3">
+        <f>Data[[#This Row],[Total]]-M20</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
         <v>1718</v>
       </c>
-      <c r="N21" s="2">
+      <c r="P21" s="2">
         <v>3546</v>
       </c>
-      <c r="O21" s="2">
+      <c r="Q21" s="2">
         <v>61044</v>
       </c>
-      <c r="P21" s="2">
+      <c r="R21" s="2">
         <v>43112</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="S21" s="2">
         <v>1</v>
       </c>
-      <c r="R21" s="2">
+      <c r="T21" s="2">
         <v>1</v>
       </c>
-      <c r="S21" s="2">
+      <c r="U21" s="2">
         <v>219</v>
       </c>
-      <c r="T21" s="2">
+      <c r="V21" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="U21" s="2">
-        <v>0</v>
-      </c>
-      <c r="V21" s="2">
+      <c r="W21" s="2">
+        <v>0</v>
+      </c>
+      <c r="X21" s="2">
         <v>156</v>
       </c>
-      <c r="W21" s="2">
+      <c r="Y21" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>156</v>
       </c>
-      <c r="X21" s="2">
+      <c r="Z21" s="2">
         <v>131</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="AA21" s="2">
         <v>132</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AB21" s="2">
         <v>4</v>
       </c>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
-      <c r="AE21" s="2">
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2">
         <v>773</v>
       </c>
-      <c r="AF21" s="2">
+      <c r="AH21" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>773</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44713</v>
       </c>
@@ -9641,70 +9880,78 @@
       <c r="E22" s="2">
         <v>4504</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="3">
+        <f>Data[[#This Row],[LoC]]-E21</f>
+        <v>0</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2">
+      <c r="M22" s="2"/>
+      <c r="N22" s="3">
+        <f>Data[[#This Row],[Total]]-M21</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
         <v>1723</v>
       </c>
-      <c r="N22" s="2">
+      <c r="P22" s="2">
         <v>3559</v>
       </c>
-      <c r="O22" s="2">
+      <c r="Q22" s="2">
         <v>61077</v>
       </c>
-      <c r="P22" s="2">
+      <c r="R22" s="2">
         <v>43133</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="S22" s="2">
         <v>1</v>
       </c>
-      <c r="R22" s="2">
+      <c r="T22" s="2">
         <v>1</v>
       </c>
-      <c r="S22" s="2">
+      <c r="U22" s="2">
         <v>219</v>
       </c>
-      <c r="T22" s="2">
+      <c r="V22" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="U22" s="2">
-        <v>0</v>
-      </c>
-      <c r="V22" s="2">
+      <c r="W22" s="2">
+        <v>0</v>
+      </c>
+      <c r="X22" s="2">
         <v>157</v>
       </c>
-      <c r="W22" s="2">
+      <c r="Y22" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="X22" s="2">
+      <c r="Z22" s="2">
         <v>131</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="AA22" s="2">
         <v>132</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="AB22" s="2">
         <v>4</v>
       </c>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
-      <c r="AE22" s="2">
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2">
         <v>787</v>
       </c>
-      <c r="AF22" s="2">
+      <c r="AH22" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>787</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44714</v>
       </c>
@@ -9720,70 +9967,78 @@
       <c r="E23" s="2">
         <v>4504</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="3">
+        <f>Data[[#This Row],[LoC]]-E22</f>
+        <v>0</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2">
+      <c r="M23" s="2"/>
+      <c r="N23" s="3">
+        <f>Data[[#This Row],[Total]]-M22</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
         <v>1724</v>
       </c>
-      <c r="N23" s="2">
+      <c r="P23" s="2">
         <v>3560</v>
       </c>
-      <c r="O23" s="2">
+      <c r="Q23" s="2">
         <v>61077</v>
       </c>
-      <c r="P23" s="2">
+      <c r="R23" s="2">
         <v>43133</v>
       </c>
-      <c r="Q23" s="2">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0</v>
-      </c>
       <c r="S23" s="2">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0</v>
+      </c>
+      <c r="U23" s="2">
         <v>220</v>
       </c>
-      <c r="T23" s="2">
+      <c r="V23" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="U23" s="2">
-        <v>0</v>
-      </c>
-      <c r="V23" s="2">
+      <c r="W23" s="2">
+        <v>0</v>
+      </c>
+      <c r="X23" s="2">
         <v>157</v>
       </c>
-      <c r="W23" s="2">
+      <c r="Y23" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Z23" s="2">
         <v>131</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="AA23" s="2">
         <v>132</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AB23" s="2">
         <v>4</v>
       </c>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
-      <c r="AE23" s="2">
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2">
         <v>789</v>
       </c>
-      <c r="AF23" s="2">
+      <c r="AH23" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>789</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44715</v>
       </c>
@@ -9799,76 +10054,84 @@
       <c r="E24" s="2">
         <v>4510</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="3">
+        <f>Data[[#This Row],[LoC]]-E23</f>
+        <v>6</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2">
+      <c r="M24" s="2"/>
+      <c r="N24" s="3">
+        <f>Data[[#This Row],[Total]]-M23</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="2">
         <v>1728</v>
       </c>
-      <c r="N24" s="2">
+      <c r="P24" s="2">
         <v>3565</v>
       </c>
-      <c r="O24" s="2">
+      <c r="Q24" s="2">
         <v>61091</v>
       </c>
-      <c r="P24" s="2">
+      <c r="R24" s="2">
         <v>43136</v>
       </c>
-      <c r="Q24" s="2">
-        <v>0</v>
-      </c>
-      <c r="R24" s="2">
-        <v>0</v>
-      </c>
       <c r="S24" s="2">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0</v>
+      </c>
+      <c r="U24" s="2">
         <v>220</v>
       </c>
-      <c r="T24" s="2">
+      <c r="V24" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>220</v>
       </c>
-      <c r="U24" s="2">
-        <v>0</v>
-      </c>
-      <c r="V24" s="2">
+      <c r="W24" s="2">
+        <v>0</v>
+      </c>
+      <c r="X24" s="2">
         <v>157</v>
       </c>
-      <c r="W24" s="2">
+      <c r="Y24" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>157</v>
       </c>
-      <c r="X24" s="2">
+      <c r="Z24" s="2">
         <v>131</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="AA24" s="2">
         <v>132</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="AB24" s="2">
         <v>4</v>
       </c>
-      <c r="AA24" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="2">
+      <c r="AC24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2">
         <v>302</v>
       </c>
-      <c r="AC24" s="2">
+      <c r="AE24" s="2">
         <v>488</v>
       </c>
-      <c r="AD24" s="2">
+      <c r="AF24" s="2">
         <v>7</v>
       </c>
-      <c r="AE24" s="2"/>
-      <c r="AF24" s="2">
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>797</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44723</v>
       </c>
@@ -9884,76 +10147,84 @@
       <c r="E25" s="2">
         <v>4510</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="3">
+        <f>Data[[#This Row],[LoC]]-E24</f>
+        <v>0</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2">
+      <c r="M25" s="2"/>
+      <c r="N25" s="3">
+        <f>Data[[#This Row],[Total]]-M24</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="2">
         <v>1733</v>
       </c>
-      <c r="N25" s="2">
+      <c r="P25" s="2">
         <v>3579</v>
       </c>
-      <c r="O25" s="2">
+      <c r="Q25" s="2">
         <v>61141</v>
       </c>
-      <c r="P25" s="2">
+      <c r="R25" s="2">
         <v>43154</v>
       </c>
-      <c r="Q25" s="2">
-        <v>0</v>
-      </c>
-      <c r="R25" s="2">
-        <v>0</v>
-      </c>
       <c r="S25" s="2">
+        <v>0</v>
+      </c>
+      <c r="T25" s="2">
+        <v>0</v>
+      </c>
+      <c r="U25" s="2">
         <v>221</v>
       </c>
-      <c r="T25" s="2">
+      <c r="V25" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="U25" s="2">
-        <v>0</v>
-      </c>
-      <c r="V25" s="2">
+      <c r="W25" s="2">
+        <v>0</v>
+      </c>
+      <c r="X25" s="2">
         <v>158</v>
       </c>
-      <c r="W25" s="2">
+      <c r="Y25" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>158</v>
       </c>
-      <c r="X25" s="2">
+      <c r="Z25" s="2">
         <v>131</v>
       </c>
-      <c r="Y25" s="2">
+      <c r="AA25" s="2">
         <v>132</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AB25" s="2">
         <v>4</v>
       </c>
-      <c r="AA25" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="2">
+      <c r="AC25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2">
         <v>304</v>
       </c>
-      <c r="AC25" s="2">
+      <c r="AE25" s="2">
         <v>501</v>
       </c>
-      <c r="AD25" s="2">
+      <c r="AF25" s="2">
         <v>7</v>
       </c>
-      <c r="AE25" s="2"/>
-      <c r="AF25" s="2">
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>812</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44725</v>
       </c>
@@ -9969,76 +10240,84 @@
       <c r="E26" s="2">
         <v>4510</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="3">
+        <f>Data[[#This Row],[LoC]]-E25</f>
+        <v>0</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2">
+      <c r="M26" s="2"/>
+      <c r="N26" s="3">
+        <f>Data[[#This Row],[Total]]-M25</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
         <v>1743</v>
       </c>
-      <c r="N26" s="2">
+      <c r="P26" s="2">
         <v>3590</v>
       </c>
-      <c r="O26" s="2">
+      <c r="Q26" s="2">
         <v>61156</v>
       </c>
-      <c r="P26" s="2">
+      <c r="R26" s="2">
         <v>43168</v>
       </c>
-      <c r="Q26" s="2">
-        <v>0</v>
-      </c>
-      <c r="R26" s="2">
-        <v>0</v>
-      </c>
       <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
+      <c r="U26" s="2">
         <v>221</v>
       </c>
-      <c r="T26" s="2">
+      <c r="V26" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="U26" s="2">
-        <v>0</v>
-      </c>
-      <c r="V26" s="2">
+      <c r="W26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="2">
         <v>159</v>
       </c>
-      <c r="W26" s="2">
+      <c r="Y26" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X26" s="2">
+      <c r="Z26" s="2">
         <v>131</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="AA26" s="2">
         <v>132</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="AB26" s="2">
         <v>4</v>
       </c>
-      <c r="AA26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="2">
+      <c r="AC26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2">
         <v>305</v>
       </c>
-      <c r="AC26" s="2">
+      <c r="AE26" s="2">
         <v>517</v>
       </c>
-      <c r="AD26" s="2">
+      <c r="AF26" s="2">
         <v>7</v>
       </c>
-      <c r="AE26" s="2"/>
-      <c r="AF26" s="2">
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>829</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44727</v>
       </c>
@@ -10054,76 +10333,84 @@
       <c r="E27" s="2">
         <v>4515</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="3">
+        <f>Data[[#This Row],[LoC]]-E26</f>
+        <v>5</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2">
+      <c r="M27" s="2"/>
+      <c r="N27" s="3">
+        <f>Data[[#This Row],[Total]]-M26</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
         <v>1758</v>
       </c>
-      <c r="N27" s="2">
+      <c r="P27" s="2">
         <v>3610</v>
       </c>
-      <c r="O27" s="2">
+      <c r="Q27" s="2">
         <v>61388</v>
       </c>
-      <c r="P27" s="2">
+      <c r="R27" s="2">
         <v>43266</v>
       </c>
-      <c r="Q27" s="2">
-        <v>0</v>
-      </c>
-      <c r="R27" s="2">
-        <v>0</v>
-      </c>
       <c r="S27" s="2">
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <v>0</v>
+      </c>
+      <c r="U27" s="2">
         <v>221</v>
       </c>
-      <c r="T27" s="2">
+      <c r="V27" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>221</v>
       </c>
-      <c r="U27" s="2">
-        <v>0</v>
-      </c>
-      <c r="V27" s="2">
+      <c r="W27" s="2">
+        <v>0</v>
+      </c>
+      <c r="X27" s="2">
         <v>159</v>
       </c>
-      <c r="W27" s="2">
+      <c r="Y27" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X27" s="2">
+      <c r="Z27" s="2">
         <v>131</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="AA27" s="2">
         <v>132</v>
       </c>
-      <c r="Z27" s="2">
+      <c r="AB27" s="2">
         <v>4</v>
       </c>
-      <c r="AA27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="2">
+      <c r="AC27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="2">
         <v>314</v>
       </c>
-      <c r="AC27" s="2">
+      <c r="AE27" s="2">
         <v>536</v>
       </c>
-      <c r="AD27" s="2">
+      <c r="AF27" s="2">
         <v>7</v>
       </c>
-      <c r="AE27" s="2"/>
-      <c r="AF27" s="2">
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>857</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44729</v>
       </c>
@@ -10139,76 +10426,84 @@
       <c r="E28" s="2">
         <v>4585</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="3">
+        <f>Data[[#This Row],[LoC]]-E27</f>
+        <v>70</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2">
+      <c r="M28" s="2"/>
+      <c r="N28" s="3">
+        <f>Data[[#This Row],[Total]]-M27</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="2">
         <v>1763</v>
       </c>
-      <c r="N28" s="2">
+      <c r="P28" s="2">
         <v>3627</v>
       </c>
-      <c r="O28" s="2">
+      <c r="Q28" s="2">
         <v>61547</v>
       </c>
-      <c r="P28" s="2">
+      <c r="R28" s="2">
         <v>43284</v>
       </c>
-      <c r="Q28" s="2">
-        <v>0</v>
-      </c>
-      <c r="R28" s="2">
-        <v>0</v>
-      </c>
       <c r="S28" s="2">
+        <v>0</v>
+      </c>
+      <c r="T28" s="2">
+        <v>0</v>
+      </c>
+      <c r="U28" s="2">
         <v>222</v>
       </c>
-      <c r="T28" s="2">
+      <c r="V28" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>222</v>
       </c>
-      <c r="U28" s="2">
-        <v>0</v>
-      </c>
-      <c r="V28" s="2">
+      <c r="W28" s="2">
+        <v>0</v>
+      </c>
+      <c r="X28" s="2">
         <v>159</v>
       </c>
-      <c r="W28" s="2">
+      <c r="Y28" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X28" s="2">
+      <c r="Z28" s="2">
         <v>133</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="AA28" s="2">
         <v>135</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="AB28" s="2">
         <v>4</v>
       </c>
-      <c r="AA28" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="2">
+      <c r="AC28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="2">
         <v>316</v>
       </c>
-      <c r="AC28" s="2">
+      <c r="AE28" s="2">
         <v>548</v>
       </c>
-      <c r="AD28" s="2">
+      <c r="AF28" s="2">
         <v>7</v>
       </c>
-      <c r="AE28" s="2"/>
-      <c r="AF28" s="2">
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>871</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44743</v>
       </c>
@@ -10224,76 +10519,84 @@
       <c r="E29" s="2">
         <v>4689</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="3">
+        <f>Data[[#This Row],[LoC]]-E28</f>
+        <v>104</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2">
+      <c r="M29" s="2"/>
+      <c r="N29" s="3">
+        <f>Data[[#This Row],[Total]]-M28</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="2">
         <v>1773</v>
       </c>
-      <c r="N29" s="2">
+      <c r="P29" s="2">
         <v>3651</v>
       </c>
-      <c r="O29" s="2">
+      <c r="Q29" s="2">
         <v>61778</v>
       </c>
-      <c r="P29" s="2">
+      <c r="R29" s="2">
         <v>43332</v>
       </c>
-      <c r="Q29" s="2">
-        <v>0</v>
-      </c>
-      <c r="R29" s="2">
-        <v>0</v>
-      </c>
       <c r="S29" s="2">
+        <v>0</v>
+      </c>
+      <c r="T29" s="2">
+        <v>0</v>
+      </c>
+      <c r="U29" s="2">
         <v>222</v>
       </c>
-      <c r="T29" s="2">
+      <c r="V29" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>222</v>
       </c>
-      <c r="U29" s="2">
-        <v>0</v>
-      </c>
-      <c r="V29" s="2">
+      <c r="W29" s="2">
+        <v>0</v>
+      </c>
+      <c r="X29" s="2">
         <v>159</v>
       </c>
-      <c r="W29" s="2">
+      <c r="Y29" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X29" s="2">
+      <c r="Z29" s="2">
         <v>134</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="AA29" s="2">
         <v>137</v>
       </c>
-      <c r="Z29" s="2">
+      <c r="AB29" s="2">
         <v>4</v>
       </c>
-      <c r="AA29" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="2">
+      <c r="AC29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="2">
         <v>320</v>
       </c>
-      <c r="AC29" s="2">
+      <c r="AE29" s="2">
         <v>568</v>
       </c>
-      <c r="AD29" s="2">
+      <c r="AF29" s="2">
         <v>7</v>
       </c>
-      <c r="AE29" s="2"/>
-      <c r="AF29" s="2">
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>895</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44748</v>
       </c>
@@ -10309,76 +10612,84 @@
       <c r="E30" s="2">
         <v>4712</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="3">
+        <f>Data[[#This Row],[LoC]]-E29</f>
+        <v>23</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2">
+      <c r="M30" s="2"/>
+      <c r="N30" s="3">
+        <f>Data[[#This Row],[Total]]-M29</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="2">
         <v>1776</v>
       </c>
-      <c r="N30" s="2">
+      <c r="P30" s="2">
         <v>3662</v>
       </c>
-      <c r="O30" s="2">
+      <c r="Q30" s="2">
         <v>61856</v>
       </c>
-      <c r="P30" s="2">
+      <c r="R30" s="2">
         <v>43366</v>
       </c>
-      <c r="Q30" s="2">
-        <v>0</v>
-      </c>
-      <c r="R30" s="2">
-        <v>0</v>
-      </c>
       <c r="S30" s="2">
+        <v>0</v>
+      </c>
+      <c r="T30" s="2">
+        <v>0</v>
+      </c>
+      <c r="U30" s="2">
         <v>223</v>
       </c>
-      <c r="T30" s="2">
+      <c r="V30" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>223</v>
       </c>
-      <c r="U30" s="2">
-        <v>0</v>
-      </c>
-      <c r="V30" s="2">
+      <c r="W30" s="2">
+        <v>0</v>
+      </c>
+      <c r="X30" s="2">
         <v>159</v>
       </c>
-      <c r="W30" s="2">
+      <c r="Y30" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X30" s="2">
+      <c r="Z30" s="2">
         <v>134</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="AA30" s="2">
         <v>137</v>
       </c>
-      <c r="Z30" s="2">
+      <c r="AB30" s="2">
         <v>4</v>
       </c>
-      <c r="AA30" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="2">
+      <c r="AC30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="2">
         <v>320</v>
       </c>
-      <c r="AC30" s="2">
+      <c r="AE30" s="2">
         <v>578</v>
       </c>
-      <c r="AD30" s="2">
+      <c r="AF30" s="2">
         <v>7</v>
       </c>
-      <c r="AE30" s="2"/>
-      <c r="AF30" s="2">
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>905</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44757</v>
       </c>
@@ -10394,76 +10705,84 @@
       <c r="E31" s="2">
         <v>4720</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="3">
+        <f>Data[[#This Row],[LoC]]-E30</f>
+        <v>8</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2">
+      <c r="M31" s="2"/>
+      <c r="N31" s="3">
+        <f>Data[[#This Row],[Total]]-M30</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="2">
         <v>1782</v>
       </c>
-      <c r="N31" s="2">
+      <c r="P31" s="2">
         <v>3684</v>
       </c>
-      <c r="O31" s="2">
+      <c r="Q31" s="2">
         <v>62189</v>
       </c>
-      <c r="P31" s="2">
+      <c r="R31" s="2">
         <v>43626</v>
       </c>
-      <c r="Q31" s="2">
-        <v>0</v>
-      </c>
-      <c r="R31" s="2">
-        <v>0</v>
-      </c>
       <c r="S31" s="2">
+        <v>0</v>
+      </c>
+      <c r="T31" s="2">
+        <v>0</v>
+      </c>
+      <c r="U31" s="2">
         <v>224</v>
       </c>
-      <c r="T31" s="2">
+      <c r="V31" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>224</v>
       </c>
-      <c r="U31" s="2">
-        <v>0</v>
-      </c>
-      <c r="V31" s="2">
+      <c r="W31" s="2">
+        <v>0</v>
+      </c>
+      <c r="X31" s="2">
         <v>159</v>
       </c>
-      <c r="W31" s="2">
+      <c r="Y31" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X31" s="2">
+      <c r="Z31" s="2">
         <v>134</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="AA31" s="2">
         <v>138</v>
       </c>
-      <c r="Z31" s="2">
+      <c r="AB31" s="2">
         <v>4</v>
       </c>
-      <c r="AA31" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="2">
+      <c r="AC31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="2">
         <v>321</v>
       </c>
-      <c r="AC31" s="2">
+      <c r="AE31" s="2">
         <v>593</v>
       </c>
-      <c r="AD31" s="2">
+      <c r="AF31" s="2">
         <v>7</v>
       </c>
-      <c r="AE31" s="2"/>
-      <c r="AF31" s="2">
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>921</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44761</v>
       </c>
@@ -10479,91 +10798,98 @@
       <c r="E32" s="2">
         <v>4720</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
+        <f>Data[[#This Row],[LoC]]-E31</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
         <v>5498</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>1781</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>315</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>240</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>97</v>
       </c>
-      <c r="K32" s="2">
+      <c r="L32" s="2">
         <v>48</v>
       </c>
-      <c r="L32" s="2">
+      <c r="M32" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
         <v>7979</v>
       </c>
-      <c r="M32" s="2">
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="2">
         <v>1782</v>
       </c>
-      <c r="N32" s="2">
+      <c r="P32" s="2">
         <v>3684</v>
       </c>
-      <c r="O32" s="2">
+      <c r="Q32" s="2">
         <v>62189</v>
       </c>
-      <c r="P32" s="2">
+      <c r="R32" s="2">
         <v>43626</v>
       </c>
-      <c r="Q32" s="2">
-        <v>0</v>
-      </c>
-      <c r="R32" s="2">
-        <v>0</v>
-      </c>
       <c r="S32" s="2">
+        <v>0</v>
+      </c>
+      <c r="T32" s="2">
+        <v>0</v>
+      </c>
+      <c r="U32" s="2">
         <v>224</v>
       </c>
-      <c r="T32" s="2">
+      <c r="V32" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>224</v>
       </c>
-      <c r="U32" s="2">
-        <v>0</v>
-      </c>
-      <c r="V32" s="2">
+      <c r="W32" s="2">
+        <v>0</v>
+      </c>
+      <c r="X32" s="2">
         <v>159</v>
       </c>
-      <c r="W32" s="2">
+      <c r="Y32" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X32" s="2">
+      <c r="Z32" s="2">
         <v>134</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="AA32" s="2">
         <v>138</v>
       </c>
-      <c r="Z32" s="2">
+      <c r="AB32" s="2">
         <v>4</v>
       </c>
-      <c r="AA32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="2">
+      <c r="AC32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="2">
         <v>321</v>
       </c>
-      <c r="AC32" s="2">
+      <c r="AE32" s="2">
         <v>595</v>
       </c>
-      <c r="AD32" s="2">
+      <c r="AF32" s="2">
         <v>7</v>
       </c>
-      <c r="AE32" s="2"/>
-      <c r="AF32" s="2">
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>923</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44764</v>
       </c>
@@ -10579,91 +10905,99 @@
       <c r="E33" s="2">
         <v>4724</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
+        <f>Data[[#This Row],[LoC]]-E32</f>
+        <v>4</v>
+      </c>
+      <c r="G33" s="2">
         <v>5502</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>1781</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>315</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>240</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>97</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L33" s="2">
         <v>48</v>
       </c>
-      <c r="L33" s="2">
+      <c r="M33" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
         <v>7983</v>
       </c>
-      <c r="M33" s="2">
+      <c r="N33" s="3">
+        <f>Data[[#This Row],[Total]]-M32</f>
+        <v>4</v>
+      </c>
+      <c r="O33" s="2">
         <v>1785</v>
       </c>
-      <c r="N33" s="2">
+      <c r="P33" s="2">
         <v>3689</v>
       </c>
-      <c r="O33" s="2">
+      <c r="Q33" s="2">
         <v>62207</v>
       </c>
-      <c r="P33" s="2">
+      <c r="R33" s="2">
         <v>43630</v>
       </c>
-      <c r="Q33" s="2">
-        <v>0</v>
-      </c>
-      <c r="R33" s="2">
-        <v>0</v>
-      </c>
       <c r="S33" s="2">
+        <v>0</v>
+      </c>
+      <c r="T33" s="2">
+        <v>0</v>
+      </c>
+      <c r="U33" s="2">
         <v>224</v>
       </c>
-      <c r="T33" s="2">
+      <c r="V33" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>224</v>
       </c>
-      <c r="U33" s="2">
-        <v>0</v>
-      </c>
-      <c r="V33" s="2">
+      <c r="W33" s="2">
+        <v>0</v>
+      </c>
+      <c r="X33" s="2">
         <v>159</v>
       </c>
-      <c r="W33" s="2">
+      <c r="Y33" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>159</v>
       </c>
-      <c r="X33" s="2">
+      <c r="Z33" s="2">
         <v>134</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="AA33" s="2">
         <v>138</v>
       </c>
-      <c r="Z33" s="2">
+      <c r="AB33" s="2">
         <v>4</v>
       </c>
-      <c r="AA33" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="2">
+      <c r="AC33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="2">
         <v>321</v>
       </c>
-      <c r="AC33" s="2">
+      <c r="AE33" s="2">
         <v>599</v>
       </c>
-      <c r="AD33" s="2">
+      <c r="AF33" s="2">
         <v>7</v>
       </c>
-      <c r="AE33" s="2"/>
-      <c r="AF33" s="2">
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>927</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44768</v>
       </c>
@@ -10679,91 +11013,99 @@
       <c r="E34" s="2">
         <v>4731</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
+        <f>Data[[#This Row],[LoC]]-E33</f>
+        <v>7</v>
+      </c>
+      <c r="G34" s="2">
         <v>5589</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>1785</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>315</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>242</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>97</v>
       </c>
-      <c r="K34" s="2">
+      <c r="L34" s="2">
         <v>48</v>
       </c>
-      <c r="L34" s="2">
+      <c r="M34" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
         <v>8076</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="3">
+        <f>Data[[#This Row],[Total]]-M33</f>
+        <v>93</v>
+      </c>
+      <c r="O34" s="2">
         <v>1789</v>
       </c>
-      <c r="N34" s="2">
+      <c r="P34" s="2">
         <v>3703</v>
       </c>
-      <c r="O34" s="2">
+      <c r="Q34" s="2">
         <v>62262</v>
       </c>
-      <c r="P34" s="2">
+      <c r="R34" s="2">
         <v>43661</v>
       </c>
-      <c r="Q34" s="2">
-        <v>0</v>
-      </c>
-      <c r="R34" s="2">
-        <v>0</v>
-      </c>
       <c r="S34" s="2">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>0</v>
+      </c>
+      <c r="U34" s="2">
         <v>225</v>
       </c>
-      <c r="T34" s="2">
+      <c r="V34" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>225</v>
       </c>
-      <c r="U34" s="2">
-        <v>0</v>
-      </c>
-      <c r="V34" s="2">
+      <c r="W34" s="2">
+        <v>0</v>
+      </c>
+      <c r="X34" s="2">
         <v>160</v>
       </c>
-      <c r="W34" s="2">
+      <c r="Y34" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>160</v>
       </c>
-      <c r="X34" s="2">
+      <c r="Z34" s="2">
         <v>135</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="AA34" s="2">
         <v>138</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="AB34" s="2">
         <v>4</v>
       </c>
-      <c r="AA34" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="2">
+      <c r="AC34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="2">
         <v>322</v>
       </c>
-      <c r="AC34" s="2">
+      <c r="AE34" s="2">
         <v>610</v>
       </c>
-      <c r="AD34" s="2">
+      <c r="AF34" s="2">
         <v>7</v>
       </c>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2">
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>939</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44790</v>
       </c>
@@ -10779,88 +11121,160 @@
       <c r="E35" s="2">
         <v>4749</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
+        <f>Data[[#This Row],[LoC]]-E34</f>
+        <v>18</v>
+      </c>
+      <c r="G35" s="2">
         <v>5535</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>1788</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>315</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>243</v>
       </c>
-      <c r="J35" s="2">
+      <c r="K35" s="2">
         <v>97</v>
       </c>
-      <c r="K35" s="2">
+      <c r="L35" s="2">
         <v>48</v>
       </c>
-      <c r="L35" s="2">
+      <c r="M35" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
         <v>8026</v>
       </c>
-      <c r="M35" s="2">
+      <c r="N35" s="3">
+        <f>Data[[#This Row],[Total]]-M34</f>
+        <v>-50</v>
+      </c>
+      <c r="O35" s="2">
         <v>1791</v>
       </c>
-      <c r="N35" s="2">
+      <c r="P35" s="2">
         <v>3716</v>
       </c>
-      <c r="O35" s="2">
+      <c r="Q35" s="2">
         <v>62325</v>
       </c>
-      <c r="P35" s="2">
+      <c r="R35" s="2">
         <v>43671</v>
       </c>
-      <c r="Q35" s="2">
-        <v>0</v>
-      </c>
-      <c r="R35" s="2">
-        <v>0</v>
-      </c>
       <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>0</v>
+      </c>
+      <c r="U35" s="2">
         <v>225</v>
       </c>
-      <c r="T35" s="2">
+      <c r="V35" s="2">
         <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
         <v>225</v>
       </c>
-      <c r="U35" s="2">
-        <v>0</v>
-      </c>
-      <c r="V35" s="2">
+      <c r="W35" s="2">
+        <v>0</v>
+      </c>
+      <c r="X35" s="2">
         <v>160</v>
       </c>
-      <c r="W35" s="2">
+      <c r="Y35" s="2">
         <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
         <v>160</v>
       </c>
-      <c r="X35" s="2">
+      <c r="Z35" s="2">
         <v>136</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="AA35" s="2">
         <v>140</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="AB35" s="2">
         <v>4</v>
       </c>
-      <c r="AA35" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="2">
+      <c r="AC35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="2">
         <v>322</v>
       </c>
-      <c r="AC35" s="2">
+      <c r="AE35" s="2">
         <v>618</v>
       </c>
-      <c r="AD35" s="2">
+      <c r="AF35" s="2">
         <v>7</v>
       </c>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2">
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>947</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44797</v>
+      </c>
+      <c r="B36" s="2">
+        <v>106</v>
+      </c>
+      <c r="C36" s="2">
+        <v>243</v>
+      </c>
+      <c r="D36" s="2">
+        <v>196</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4762</v>
+      </c>
+      <c r="F36" s="3">
+        <f>Data[[#This Row],[LoC]]-E35</f>
+        <v>13</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <f>Data[[#This Row],[Total]]-M35</f>
+        <v>-8026</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>0</v>
+      </c>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>0</v>
+      </c>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the documentation order
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3CB129-F2CE-044A-88A8-9E398A05E423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF91B6-C7B2-084E-B9D9-E150CA2B9B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25560" windowHeight="27100" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20600" windowHeight="24500" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -359,10 +359,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -482,16 +482,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$41</c:f>
+              <c:f>Data!$E$2:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -611,6 +614,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>4895</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4929</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,10 +656,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -773,16 +779,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$O$2:$O$41</c:f>
+              <c:f>Data!$O$2:$O$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -902,6 +911,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>1823</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1830</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -941,10 +953,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1064,16 +1076,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$41</c:f>
+              <c:f>Data!$P$2:$P$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1193,6 +1208,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>3813</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3837</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,10 +1466,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1571,16 +1589,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$41</c:f>
+              <c:f>Data!$T$2:$T$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1699,6 +1720,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1739,10 +1763,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1862,16 +1886,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$41</c:f>
+              <c:f>Data!$W$2:$W$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1990,6 +2017,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2030,10 +2060,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2153,16 +2183,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$S$2:$S$41</c:f>
+              <c:f>Data!$S$2:$S$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2281,6 +2314,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2540,10 +2576,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2663,16 +2699,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$41</c:f>
+              <c:f>Data!$V$2:$V$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -2791,6 +2830,9 @@
                   <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>228</c:v>
                 </c:pt>
               </c:numCache>
@@ -2831,10 +2873,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2954,16 +2996,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$41</c:f>
+              <c:f>Data!$Y$2:$Y$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3082,6 +3127,9 @@
                   <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>161</c:v>
                 </c:pt>
               </c:numCache>
@@ -3338,10 +3386,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3461,16 +3509,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$41</c:f>
+              <c:f>Data!$AA$2:$AA$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -3590,6 +3641,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3811,10 +3865,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3934,16 +3988,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$41</c:f>
+              <c:f>Data!$AC$2:$AC$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3996,6 +4053,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4032,10 +4092,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4155,16 +4215,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$41</c:f>
+              <c:f>Data!$AD$2:$AD$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -4218,6 +4281,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4253,10 +4319,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4376,16 +4442,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$41</c:f>
+              <c:f>Data!$AE$2:$AE$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -4439,6 +4508,9 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4474,10 +4546,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4597,16 +4669,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$41</c:f>
+              <c:f>Data!$AF$2:$AF$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -4659,6 +4734,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -4697,10 +4775,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$41</c:f>
+              <c:f>Data!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4820,16 +4898,19 @@
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$41</c:f>
+              <c:f>Data!$AG$2:$AG$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7851,7 +7932,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="172" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7906,7 +7987,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6069419"/>
+    <xdr:ext cx="9301151" cy="6066763"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8068,8 +8149,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH41" totalsRowShown="0">
-  <autoFilter ref="A1:AH41" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH42" totalsRowShown="0">
+  <autoFilter ref="A1:AH42" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="33"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="32"/>
@@ -8419,11 +8500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AH41"/>
+  <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12297,6 +12378,113 @@
         <v>1022</v>
       </c>
     </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44813</v>
+      </c>
+      <c r="B42" s="2">
+        <v>106</v>
+      </c>
+      <c r="C42" s="2">
+        <v>248</v>
+      </c>
+      <c r="D42" s="2">
+        <v>200</v>
+      </c>
+      <c r="E42" s="2">
+        <v>4929</v>
+      </c>
+      <c r="F42" s="3">
+        <f>Data[[#This Row],[LoC]]-E41</f>
+        <v>34</v>
+      </c>
+      <c r="G42" s="2">
+        <v>5743</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1830</v>
+      </c>
+      <c r="I42" s="2">
+        <v>289</v>
+      </c>
+      <c r="J42" s="2">
+        <v>259</v>
+      </c>
+      <c r="K42" s="2">
+        <v>97</v>
+      </c>
+      <c r="L42" s="2">
+        <v>51</v>
+      </c>
+      <c r="M42" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8269</v>
+      </c>
+      <c r="N42" s="3">
+        <f>Data[[#This Row],[Total]]-M41</f>
+        <v>82</v>
+      </c>
+      <c r="O42" s="2">
+        <v>1830</v>
+      </c>
+      <c r="P42" s="2">
+        <v>3837</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>63369</v>
+      </c>
+      <c r="R42" s="2">
+        <v>44256</v>
+      </c>
+      <c r="S42" s="2">
+        <v>0</v>
+      </c>
+      <c r="T42" s="2">
+        <v>0</v>
+      </c>
+      <c r="U42" s="2">
+        <v>228</v>
+      </c>
+      <c r="V42" s="2">
+        <v>228</v>
+      </c>
+      <c r="W42" s="2">
+        <v>0</v>
+      </c>
+      <c r="X42" s="2">
+        <v>161</v>
+      </c>
+      <c r="Y42" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>161</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>141</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>148</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC42" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="2">
+        <v>330</v>
+      </c>
+      <c r="AE42" s="2">
+        <v>703</v>
+      </c>
+      <c r="AF42" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1040</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the stats Do not start the tests when changing the stats
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D6A10B-D9E9-8E45-A6C1-D9BD8F314F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62347C3E-1A0E-8C4A-9490-20B2AED1C7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20600" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -359,10 +359,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -497,16 +497,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$46</c:f>
+              <c:f>Data!$E$2:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -641,6 +644,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>5159</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,10 +686,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -818,16 +824,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$O$2:$O$46</c:f>
+              <c:f>Data!$O$2:$O$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -962,6 +971,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1873</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,10 +1013,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1139,16 +1151,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$46</c:f>
+              <c:f>Data!$P$2:$P$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1283,6 +1298,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>3964</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1538,10 +1556,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1676,16 +1694,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$46</c:f>
+              <c:f>Data!$T$2:$T$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1819,6 +1840,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1859,10 +1883,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1997,16 +2021,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$46</c:f>
+              <c:f>Data!$W$2:$W$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2140,6 +2167,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2180,10 +2210,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2318,16 +2348,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$S$2:$S$46</c:f>
+              <c:f>Data!$S$2:$S$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2461,6 +2494,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2720,10 +2756,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2858,16 +2894,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$46</c:f>
+              <c:f>Data!$V$2:$V$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3002,6 +3041,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>237</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3041,10 +3083,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3179,16 +3221,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$46</c:f>
+              <c:f>Data!$Y$2:$Y$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3322,6 +3367,9 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
@@ -3578,10 +3626,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3716,16 +3764,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$46</c:f>
+              <c:f>Data!$AA$2:$AA$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -3859,6 +3910,9 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
@@ -4081,10 +4135,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4219,16 +4273,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$46</c:f>
+              <c:f>Data!$AC$2:$AC$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4296,6 +4353,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4332,10 +4392,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4470,16 +4530,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$46</c:f>
+              <c:f>Data!$AD$2:$AD$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -4547,6 +4610,9 @@
                   <c:v>338</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>341</c:v>
                 </c:pt>
               </c:numCache>
@@ -4583,10 +4649,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4721,16 +4787,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$46</c:f>
+              <c:f>Data!$AE$2:$AE$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -4799,6 +4868,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>797</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4834,10 +4906,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4972,16 +5044,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$46</c:f>
+              <c:f>Data!$AF$2:$AF$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -5049,6 +5124,9 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -5087,10 +5165,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$46</c:f>
+              <c:f>Data!$A$2:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5225,16 +5303,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$46</c:f>
+              <c:f>Data!$AG$2:$AG$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -8473,8 +8554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH46" totalsRowShown="0">
-  <autoFilter ref="A1:AH46" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH47" totalsRowShown="0">
+  <autoFilter ref="A1:AH47" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="33"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="32"/>
@@ -8824,11 +8905,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ46" sqref="AJ46"/>
+      <selection pane="bottomLeft" activeCell="AG47" sqref="AG47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13242,6 +13323,114 @@
         <v>1147</v>
       </c>
     </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44831</v>
+      </c>
+      <c r="B47" s="2">
+        <v>106</v>
+      </c>
+      <c r="C47" s="2">
+        <v>254</v>
+      </c>
+      <c r="D47" s="2">
+        <v>206</v>
+      </c>
+      <c r="E47" s="2">
+        <v>5169</v>
+      </c>
+      <c r="F47" s="3">
+        <f>Data[[#This Row],[LoC]]-E46</f>
+        <v>10</v>
+      </c>
+      <c r="G47" s="2">
+        <v>6018</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1872</v>
+      </c>
+      <c r="I47" s="2">
+        <v>289</v>
+      </c>
+      <c r="J47" s="2">
+        <v>273</v>
+      </c>
+      <c r="K47" s="2">
+        <v>98</v>
+      </c>
+      <c r="L47" s="2">
+        <v>57</v>
+      </c>
+      <c r="M47" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8607</v>
+      </c>
+      <c r="N47" s="3">
+        <f>Data[[#This Row],[Total]]-M46</f>
+        <v>13</v>
+      </c>
+      <c r="O47" s="2">
+        <v>1879</v>
+      </c>
+      <c r="P47" s="2">
+        <v>3976</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>64484</v>
+      </c>
+      <c r="R47" s="2">
+        <v>44834</v>
+      </c>
+      <c r="S47" s="2">
+        <v>0</v>
+      </c>
+      <c r="T47" s="2">
+        <v>0</v>
+      </c>
+      <c r="U47" s="2">
+        <v>237</v>
+      </c>
+      <c r="V47" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>237</v>
+      </c>
+      <c r="W47" s="2">
+        <v>0</v>
+      </c>
+      <c r="X47" s="2">
+        <v>162</v>
+      </c>
+      <c r="Y47" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>162</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>150</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>158</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="2">
+        <v>341</v>
+      </c>
+      <c r="AE47" s="2">
+        <v>815</v>
+      </c>
+      <c r="AF47" s="2">
+        <v>9</v>
+      </c>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1165</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Udated the stats (the tests should not run)
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62347C3E-1A0E-8C4A-9490-20B2AED1C7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7050273D-A45E-6F4B-9164-18D046866ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -359,10 +359,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -506,10 +506,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$47</c:f>
+              <c:f>Data!$E$2:$E$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -686,10 +686,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -833,10 +833,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$O$2:$O$47</c:f>
+              <c:f>Data!$O$2:$O$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -973,7 +973,7 @@
                   <c:v>1873</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1879</c:v>
+                  <c:v>1884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,10 +1013,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1160,10 +1160,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$P$2:$P$47</c:f>
+              <c:f>Data!$P$2:$P$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1300,7 +1300,7 @@
                   <c:v>3964</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3976</c:v>
+                  <c:v>3982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1556,10 +1556,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1703,10 +1703,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$T$2:$T$47</c:f>
+              <c:f>Data!$T$2:$T$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1883,10 +1883,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2030,10 +2030,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$47</c:f>
+              <c:f>Data!$W$2:$W$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2210,10 +2210,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2357,10 +2357,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$S$2:$S$47</c:f>
+              <c:f>Data!$S$2:$S$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2756,10 +2756,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2903,10 +2903,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$47</c:f>
+              <c:f>Data!$V$2:$V$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3083,10 +3083,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3230,10 +3230,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$47</c:f>
+              <c:f>Data!$Y$2:$Y$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3626,10 +3626,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3773,10 +3773,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$47</c:f>
+              <c:f>Data!$AA$2:$AA$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -4135,10 +4135,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4282,10 +4282,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$47</c:f>
+              <c:f>Data!$AC$2:$AC$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4392,10 +4392,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4539,10 +4539,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$47</c:f>
+              <c:f>Data!$AD$2:$AD$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -4613,7 +4613,7 @@
                   <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>341</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4649,10 +4649,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4796,10 +4796,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$47</c:f>
+              <c:f>Data!$AE$2:$AE$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -4870,7 +4870,7 @@
                   <c:v>797</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>815</c:v>
+                  <c:v>822</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4906,10 +4906,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5053,10 +5053,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$47</c:f>
+              <c:f>Data!$AF$2:$AF$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -5165,10 +5165,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$47</c:f>
+              <c:f>Data!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5312,10 +5312,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$47</c:f>
+              <c:f>Data!$AG$2:$AG$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -8908,8 +8908,8 @@
   <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG47" sqref="AG47"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF47" sqref="AF47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13350,7 +13350,7 @@
         <v>1872</v>
       </c>
       <c r="I47" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J47" s="2">
         <v>273</v>
@@ -13363,23 +13363,23 @@
       </c>
       <c r="M47" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
-        <v>8607</v>
+        <v>8609</v>
       </c>
       <c r="N47" s="3">
         <f>Data[[#This Row],[Total]]-M46</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O47" s="2">
-        <v>1879</v>
+        <v>1884</v>
       </c>
       <c r="P47" s="2">
-        <v>3976</v>
+        <v>3982</v>
       </c>
       <c r="Q47" s="2">
-        <v>64484</v>
+        <v>64492</v>
       </c>
       <c r="R47" s="2">
-        <v>44834</v>
+        <v>44840</v>
       </c>
       <c r="S47" s="2">
         <v>0</v>
@@ -13417,10 +13417,10 @@
         <v>0</v>
       </c>
       <c r="AD47" s="2">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="AE47" s="2">
-        <v>815</v>
+        <v>822</v>
       </c>
       <c r="AF47" s="2">
         <v>9</v>
@@ -13428,7 +13428,7 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
-        <v>1165</v>
+        <v>1175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the statistics after last release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/src/check_ssl_cert/varia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7050273D-A45E-6F4B-9164-18D046866ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03D2ACB-95EA-F645-84E6-D9A50A015797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24440" activeTab="1" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -501,6 +501,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -647,6 +650,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>5169</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -828,6 +834,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -974,6 +983,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>1884</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,6 +1167,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1301,6 +1316,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>3982</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,6 +1716,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1843,6 +1864,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2025,6 +2049,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2170,6 +2197,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2352,6 +2382,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2497,6 +2530,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2898,6 +2934,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3044,6 +3083,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3225,6 +3267,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3370,6 +3415,9 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
@@ -3768,6 +3816,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3914,6 +3965,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4277,6 +4331,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4356,6 +4413,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4534,6 +4594,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4614,6 +4677,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4791,6 +4857,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4871,6 +4940,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>822</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>837</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5048,6 +5120,9 @@
                 <c:pt idx="45">
                   <c:v>44831</c:v>
                 </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5127,6 +5202,9 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -5306,6 +5384,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>44831</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8337,7 +8418,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8392,7 +8473,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9301151" cy="6066763"/>
+    <xdr:ext cx="9313333" cy="6083457"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8554,8 +8635,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH47" totalsRowShown="0">
-  <autoFilter ref="A1:AH47" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AH48" totalsRowShown="0">
+  <autoFilter ref="A1:AH48" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="33"/>
     <tableColumn id="2" xr3:uid="{29461922-6B0E-7E4E-9465-94C5573BFF84}" name="Authors" dataDxfId="32"/>
@@ -8905,11 +8986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AH48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF47" sqref="AF47"/>
+    <sheetView topLeftCell="R1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI48" sqref="AI48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13431,6 +13512,114 @@
         <v>1175</v>
       </c>
     </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44840</v>
+      </c>
+      <c r="B48" s="2">
+        <v>106</v>
+      </c>
+      <c r="C48" s="2">
+        <v>255</v>
+      </c>
+      <c r="D48" s="2">
+        <v>207</v>
+      </c>
+      <c r="E48" s="2">
+        <v>5260</v>
+      </c>
+      <c r="F48" s="3">
+        <f>Data[[#This Row],[LoC]]-E47</f>
+        <v>91</v>
+      </c>
+      <c r="G48" s="2">
+        <v>6107</v>
+      </c>
+      <c r="H48" s="2">
+        <v>1875</v>
+      </c>
+      <c r="I48" s="2">
+        <v>291</v>
+      </c>
+      <c r="J48" s="2">
+        <v>425</v>
+      </c>
+      <c r="K48" s="2">
+        <v>98</v>
+      </c>
+      <c r="L48" s="2">
+        <v>57</v>
+      </c>
+      <c r="M48" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8853</v>
+      </c>
+      <c r="N48" s="3">
+        <f>Data[[#This Row],[Total]]-M47</f>
+        <v>244</v>
+      </c>
+      <c r="O48" s="2">
+        <v>1890</v>
+      </c>
+      <c r="P48" s="2">
+        <v>4001</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>64679</v>
+      </c>
+      <c r="R48" s="2">
+        <v>44879</v>
+      </c>
+      <c r="S48" s="2">
+        <v>0</v>
+      </c>
+      <c r="T48" s="2">
+        <v>0</v>
+      </c>
+      <c r="U48" s="2">
+        <v>238</v>
+      </c>
+      <c r="V48" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>238</v>
+      </c>
+      <c r="W48" s="2">
+        <v>0</v>
+      </c>
+      <c r="X48" s="2">
+        <v>162</v>
+      </c>
+      <c r="Y48" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>162</v>
+      </c>
+      <c r="Z48" s="2">
+        <v>151</v>
+      </c>
+      <c r="AA48" s="2">
+        <v>161</v>
+      </c>
+      <c r="AB48" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="2">
+        <v>345</v>
+      </c>
+      <c r="AE48" s="2">
+        <v>837</v>
+      </c>
+      <c r="AF48" s="2">
+        <v>9</v>
+      </c>
+      <c r="AG48" s="2"/>
+      <c r="AH48" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1191</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the statistics (again)
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03D2ACB-95EA-F645-84E6-D9A50A015797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620F1FCC-9680-E54F-8A1E-B5911CEE6FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24440" activeTab="1" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12180" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -652,7 +652,7 @@
                   <c:v>5169</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5260</c:v>
+                  <c:v>5265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,7 +985,7 @@
                   <c:v>1884</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1890</c:v>
+                  <c:v>1893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1318,7 +1318,7 @@
                   <c:v>3982</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4001</c:v>
+                  <c:v>4011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3967,7 +3967,7 @@
                   <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>161</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4942,7 +4942,7 @@
                   <c:v>822</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>837</c:v>
+                  <c:v>846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8418,7 +8418,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8473,7 +8473,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6083457"/>
+    <xdr:ext cx="9313333" cy="6073913"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8988,9 +8988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
   <dimension ref="A1:AH48"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI48" sqref="AI48"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF48" sqref="AF48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13520,23 +13520,23 @@
         <v>106</v>
       </c>
       <c r="C48" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D48" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E48" s="2">
-        <v>5260</v>
+        <v>5265</v>
       </c>
       <c r="F48" s="3">
         <f>Data[[#This Row],[LoC]]-E47</f>
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G48" s="2">
-        <v>6107</v>
+        <v>6117</v>
       </c>
       <c r="H48" s="2">
-        <v>1875</v>
+        <v>1877</v>
       </c>
       <c r="I48" s="2">
         <v>291</v>
@@ -13552,23 +13552,23 @@
       </c>
       <c r="M48" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
-        <v>8853</v>
+        <v>8865</v>
       </c>
       <c r="N48" s="3">
         <f>Data[[#This Row],[Total]]-M47</f>
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="O48" s="2">
-        <v>1890</v>
+        <v>1893</v>
       </c>
       <c r="P48" s="2">
-        <v>4001</v>
+        <v>4011</v>
       </c>
       <c r="Q48" s="2">
-        <v>64679</v>
+        <v>64734</v>
       </c>
       <c r="R48" s="2">
-        <v>44879</v>
+        <v>44916</v>
       </c>
       <c r="S48" s="2">
         <v>0</v>
@@ -13597,7 +13597,7 @@
         <v>151</v>
       </c>
       <c r="AA48" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AB48" s="2">
         <v>4</v>
@@ -13609,7 +13609,7 @@
         <v>345</v>
       </c>
       <c r="AE48" s="2">
-        <v>837</v>
+        <v>846</v>
       </c>
       <c r="AF48" s="2">
         <v>9</v>
@@ -13617,7 +13617,7 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
-        <v>1191</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stats after release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545AC3E-2E07-C04E-BC18-A6526AC64D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AF390C-5DD4-FA45-8C14-E83CFB346B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="64000" windowHeight="17080" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24480" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Issues &amp; PRs" sheetId="4" r:id="rId4"/>
     <sheet name="Tests" sheetId="5" r:id="rId5"/>
     <sheet name="Workflows" sheetId="6" r:id="rId6"/>
+    <sheet name="Stars &amp; Forks" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -372,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -531,16 +532,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$53</c:f>
+              <c:f>Data!$G$2:$G$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -696,6 +700,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>5443</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5447</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,10 +742,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -894,16 +901,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$53</c:f>
+              <c:f>Data!$Q$2:$Q$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1059,6 +1069,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,10 +1111,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1257,16 +1270,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$53</c:f>
+              <c:f>Data!$R$2:$R$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1422,6 +1438,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>4093</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,10 +1696,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1836,16 +1855,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$53</c:f>
+              <c:f>Data!$V$2:$V$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2000,6 +2022,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2040,10 +2065,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2199,16 +2224,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$53</c:f>
+              <c:f>Data!$Y$2:$Y$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2363,6 +2391,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2403,10 +2434,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2562,16 +2593,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$53</c:f>
+              <c:f>Data!$U$2:$U$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2726,6 +2760,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2985,10 +3022,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3144,16 +3181,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$53</c:f>
+              <c:f>Data!$X$2:$X$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3309,6 +3349,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3348,10 +3391,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3507,16 +3550,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$53</c:f>
+              <c:f>Data!$AA$2:$AA$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3671,6 +3717,9 @@
                   <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>168</c:v>
                 </c:pt>
               </c:numCache>
@@ -3927,10 +3976,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4086,16 +4135,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$53</c:f>
+              <c:f>Data!$AC$2:$AC$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -4250,6 +4302,9 @@
                   <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
@@ -4472,10 +4527,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4631,16 +4686,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$53</c:f>
+              <c:f>Data!$AE$2:$AE$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4729,6 +4787,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4765,10 +4826,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4924,16 +4985,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$53</c:f>
+              <c:f>Data!$AF$2:$AF$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -5023,6 +5087,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5058,10 +5125,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5217,16 +5284,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$53</c:f>
+              <c:f>Data!$AG$2:$AG$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -5316,6 +5386,9 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5351,10 +5424,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5510,16 +5583,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$53</c:f>
+              <c:f>Data!$AH$2:$AH$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -5608,6 +5684,9 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="51">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -5646,10 +5725,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$53</c:f>
+              <c:f>Data!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5805,16 +5884,19 @@
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$53</c:f>
+              <c:f>Data!$AI$2:$AI$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -6017,6 +6099,819 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>44574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44580</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44610</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44613</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44676</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44678</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44679</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44686</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44691</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44705</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44707</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44710</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44723</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44725</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44748</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44798</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44806</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44810</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44817</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44820</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44851</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44853</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44854</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44858</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>323</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-600F-E04F-8032-35A6577743F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Forks</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>44574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44580</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44610</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44613</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44664</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44676</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44678</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44679</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44686</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44691</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44705</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44707</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44710</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44715</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44723</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44725</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44727</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44729</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44748</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44757</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44761</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44764</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44790</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44797</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44798</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44806</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44810</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44813</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44817</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44820</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44828</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44831</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44840</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44851</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44853</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44854</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44858</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44874</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44890</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$C$2:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="47">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-600F-E04F-8032-35A6577743F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="639000495"/>
+        <c:axId val="639339903"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="639000495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639339903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="639339903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639000495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6285,6 +7180,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -8832,11 +9767,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8847,7 +10298,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{24ACA0B5-B5F6-0649-9568-624D24B93699}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8858,7 +10309,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{50B1BB8B-A1E8-FB42-B88F-023CE9967AAB}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="207" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8869,7 +10320,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B111F3D3-9A19-164A-A80F-5E41AF9CF1E4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8880,7 +10331,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{5B2EC930-5C2E-4448-96C6-E1C9EC4CF674}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="210" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3CF196A6-E282-444D-AFF0-E87110025633}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8891,7 +10353,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6073913"/>
+    <xdr:ext cx="9316565" cy="6078550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8924,7 +10386,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9316565" cy="6078550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8957,7 +10419,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304130" cy="6064710"/>
+    <xdr:ext cx="9313333" cy="6073913"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8990,7 +10452,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6077857"/>
+    <xdr:ext cx="9311298" cy="6075240"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9023,7 +10485,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6077857"/>
+    <xdr:ext cx="9311298" cy="6075240"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9052,9 +10514,42 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9311298" cy="6075240"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39D2265-965B-7D44-7ACC-AB7C49CEBA6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ53" totalsRowShown="0">
-  <autoFilter ref="A1:AJ53" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ54" totalsRowShown="0">
+  <autoFilter ref="A1:AJ54" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -9406,11 +10901,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ53"/>
+  <dimension ref="A1:AJ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ53" sqref="AJ53"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9562,6 +11057,9 @@
       <c r="A2" s="1">
         <v>44574</v>
       </c>
+      <c r="B2">
+        <v>274</v>
+      </c>
       <c r="D2" s="2">
         <v>101</v>
       </c>
@@ -9646,6 +11144,9 @@
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44578</v>
+      </c>
+      <c r="B3">
+        <v>275</v>
       </c>
       <c r="D3" s="2">
         <v>101</v>
@@ -9734,6 +11235,9 @@
       <c r="A4" s="1">
         <v>44580</v>
       </c>
+      <c r="B4">
+        <v>275</v>
+      </c>
       <c r="D4" s="2">
         <v>101</v>
       </c>
@@ -9821,6 +11325,9 @@
       <c r="A5" s="1">
         <v>44588</v>
       </c>
+      <c r="B5">
+        <v>276</v>
+      </c>
       <c r="D5" s="2">
         <v>102</v>
       </c>
@@ -9908,6 +11415,9 @@
       <c r="A6" s="1">
         <v>44593</v>
       </c>
+      <c r="B6">
+        <v>277</v>
+      </c>
       <c r="D6" s="2">
         <v>102</v>
       </c>
@@ -9995,6 +11505,9 @@
       <c r="A7" s="1">
         <v>44602</v>
       </c>
+      <c r="B7">
+        <v>280</v>
+      </c>
       <c r="D7" s="2">
         <v>102</v>
       </c>
@@ -10082,6 +11595,9 @@
       <c r="A8" s="1">
         <v>44610</v>
       </c>
+      <c r="B8">
+        <v>282</v>
+      </c>
       <c r="D8" s="2">
         <v>102</v>
       </c>
@@ -10169,6 +11685,9 @@
       <c r="A9" s="1">
         <v>44613</v>
       </c>
+      <c r="B9">
+        <v>283</v>
+      </c>
       <c r="D9" s="2">
         <v>102</v>
       </c>
@@ -10256,6 +11775,9 @@
       <c r="A10" s="1">
         <v>44636</v>
       </c>
+      <c r="B10">
+        <v>287</v>
+      </c>
       <c r="D10" s="2">
         <v>102</v>
       </c>
@@ -10343,6 +11865,9 @@
       <c r="A11" s="1">
         <v>44645</v>
       </c>
+      <c r="B11">
+        <v>290</v>
+      </c>
       <c r="D11" s="2">
         <v>102</v>
       </c>
@@ -10430,6 +11955,9 @@
       <c r="A12" s="1">
         <v>44657</v>
       </c>
+      <c r="B12">
+        <v>293</v>
+      </c>
       <c r="D12" s="2">
         <v>102</v>
       </c>
@@ -10517,6 +12045,9 @@
       <c r="A13" s="1">
         <v>44664</v>
       </c>
+      <c r="B13">
+        <v>294</v>
+      </c>
       <c r="D13" s="2">
         <v>102</v>
       </c>
@@ -10604,6 +12135,9 @@
       <c r="A14" s="1">
         <v>44676</v>
       </c>
+      <c r="B14">
+        <v>297</v>
+      </c>
       <c r="D14" s="2">
         <v>102</v>
       </c>
@@ -10691,6 +12225,9 @@
       <c r="A15" s="1">
         <v>44678</v>
       </c>
+      <c r="B15">
+        <v>297</v>
+      </c>
       <c r="D15" s="2">
         <v>102</v>
       </c>
@@ -10778,6 +12315,9 @@
       <c r="A16" s="1">
         <v>44679</v>
       </c>
+      <c r="B16">
+        <v>297</v>
+      </c>
       <c r="D16" s="2">
         <v>102</v>
       </c>
@@ -10865,6 +12405,9 @@
       <c r="A17" s="1">
         <v>44686</v>
       </c>
+      <c r="B17">
+        <v>298</v>
+      </c>
       <c r="D17" s="2">
         <v>102</v>
       </c>
@@ -10952,6 +12495,9 @@
       <c r="A18" s="1">
         <v>44691</v>
       </c>
+      <c r="B18">
+        <v>299</v>
+      </c>
       <c r="D18" s="2">
         <v>103</v>
       </c>
@@ -11039,6 +12585,9 @@
       <c r="A19" s="1">
         <v>44705</v>
       </c>
+      <c r="B19">
+        <v>300</v>
+      </c>
       <c r="D19" s="2">
         <v>103</v>
       </c>
@@ -11126,6 +12675,9 @@
       <c r="A20" s="1">
         <v>44707</v>
       </c>
+      <c r="B20">
+        <v>301</v>
+      </c>
       <c r="D20" s="2">
         <v>103</v>
       </c>
@@ -11213,6 +12765,9 @@
       <c r="A21" s="1">
         <v>44710</v>
       </c>
+      <c r="B21">
+        <v>302</v>
+      </c>
       <c r="D21" s="2">
         <v>103</v>
       </c>
@@ -11300,6 +12855,9 @@
       <c r="A22" s="1">
         <v>44713</v>
       </c>
+      <c r="B22">
+        <v>303</v>
+      </c>
       <c r="D22" s="2">
         <v>104</v>
       </c>
@@ -11387,6 +12945,9 @@
       <c r="A23" s="1">
         <v>44714</v>
       </c>
+      <c r="B23">
+        <v>303</v>
+      </c>
       <c r="D23" s="2">
         <v>104</v>
       </c>
@@ -11474,6 +13035,9 @@
       <c r="A24" s="1">
         <v>44715</v>
       </c>
+      <c r="B24">
+        <v>303</v>
+      </c>
       <c r="D24" s="2">
         <v>104</v>
       </c>
@@ -11567,6 +13131,9 @@
       <c r="A25" s="1">
         <v>44723</v>
       </c>
+      <c r="B25">
+        <v>303</v>
+      </c>
       <c r="D25" s="2">
         <v>105</v>
       </c>
@@ -11660,6 +13227,9 @@
       <c r="A26" s="1">
         <v>44725</v>
       </c>
+      <c r="B26">
+        <v>303</v>
+      </c>
       <c r="D26" s="2">
         <v>105</v>
       </c>
@@ -11753,6 +13323,9 @@
       <c r="A27" s="1">
         <v>44727</v>
       </c>
+      <c r="B27">
+        <v>303</v>
+      </c>
       <c r="D27" s="2">
         <v>105</v>
       </c>
@@ -11846,6 +13419,9 @@
       <c r="A28" s="1">
         <v>44729</v>
       </c>
+      <c r="B28">
+        <v>303</v>
+      </c>
       <c r="D28" s="2">
         <v>105</v>
       </c>
@@ -11939,6 +13515,9 @@
       <c r="A29" s="1">
         <v>44743</v>
       </c>
+      <c r="B29">
+        <v>303</v>
+      </c>
       <c r="D29" s="2">
         <v>105</v>
       </c>
@@ -12032,6 +13611,9 @@
       <c r="A30" s="1">
         <v>44748</v>
       </c>
+      <c r="B30">
+        <v>304</v>
+      </c>
       <c r="D30" s="2">
         <v>105</v>
       </c>
@@ -12125,6 +13707,9 @@
       <c r="A31" s="1">
         <v>44757</v>
       </c>
+      <c r="B31">
+        <v>305</v>
+      </c>
       <c r="D31" s="2">
         <v>105</v>
       </c>
@@ -12218,6 +13803,9 @@
       <c r="A32" s="1">
         <v>44761</v>
       </c>
+      <c r="B32">
+        <v>306</v>
+      </c>
       <c r="D32" s="2">
         <v>105</v>
       </c>
@@ -12325,6 +13913,9 @@
       <c r="A33" s="1">
         <v>44764</v>
       </c>
+      <c r="B33">
+        <v>308</v>
+      </c>
       <c r="D33" s="2">
         <v>105</v>
       </c>
@@ -12433,6 +14024,9 @@
       <c r="A34" s="1">
         <v>44768</v>
       </c>
+      <c r="B34">
+        <v>308</v>
+      </c>
       <c r="D34" s="2">
         <v>106</v>
       </c>
@@ -12541,6 +14135,9 @@
       <c r="A35" s="1">
         <v>44790</v>
       </c>
+      <c r="B35">
+        <v>310</v>
+      </c>
       <c r="D35" s="2">
         <v>106</v>
       </c>
@@ -12649,6 +14246,9 @@
       <c r="A36" s="1">
         <v>44797</v>
       </c>
+      <c r="B36">
+        <v>311</v>
+      </c>
       <c r="D36" s="2">
         <v>106</v>
       </c>
@@ -12757,6 +14357,9 @@
       <c r="A37" s="1">
         <v>44798</v>
       </c>
+      <c r="B37">
+        <v>312</v>
+      </c>
       <c r="D37" s="2">
         <v>106</v>
       </c>
@@ -12865,6 +14468,9 @@
       <c r="A38" s="1">
         <v>44805</v>
       </c>
+      <c r="B38">
+        <v>312</v>
+      </c>
       <c r="D38" s="2">
         <v>106</v>
       </c>
@@ -12973,6 +14579,9 @@
       <c r="A39" s="1">
         <v>44806</v>
       </c>
+      <c r="B39">
+        <v>312</v>
+      </c>
       <c r="D39" s="2">
         <v>106</v>
       </c>
@@ -13081,6 +14690,9 @@
       <c r="A40" s="1">
         <v>44810</v>
       </c>
+      <c r="B40">
+        <v>312</v>
+      </c>
       <c r="D40" s="2">
         <v>106</v>
       </c>
@@ -13189,6 +14801,9 @@
       <c r="A41" s="1">
         <v>44812</v>
       </c>
+      <c r="B41">
+        <v>312</v>
+      </c>
       <c r="D41" s="2">
         <v>106</v>
       </c>
@@ -13297,6 +14912,9 @@
       <c r="A42" s="1">
         <v>44813</v>
       </c>
+      <c r="B42">
+        <v>313</v>
+      </c>
       <c r="D42" s="2">
         <v>106</v>
       </c>
@@ -13405,6 +15023,9 @@
       <c r="A43" s="1">
         <v>44817</v>
       </c>
+      <c r="B43">
+        <v>313</v>
+      </c>
       <c r="D43" s="2">
         <v>106</v>
       </c>
@@ -13513,6 +15134,9 @@
       <c r="A44" s="1">
         <v>44820</v>
       </c>
+      <c r="B44">
+        <v>313</v>
+      </c>
       <c r="D44" s="2">
         <v>106</v>
       </c>
@@ -13621,6 +15245,9 @@
       <c r="A45" s="1">
         <v>44823</v>
       </c>
+      <c r="B45">
+        <v>313</v>
+      </c>
       <c r="D45" s="2">
         <v>106</v>
       </c>
@@ -13729,6 +15356,9 @@
       <c r="A46" s="1">
         <v>44828</v>
       </c>
+      <c r="B46">
+        <v>315</v>
+      </c>
       <c r="D46" s="2">
         <v>106</v>
       </c>
@@ -13837,6 +15467,9 @@
       <c r="A47" s="1">
         <v>44831</v>
       </c>
+      <c r="B47">
+        <v>315</v>
+      </c>
       <c r="D47" s="2">
         <v>106</v>
       </c>
@@ -13945,6 +15578,9 @@
       <c r="A48" s="1">
         <v>44840</v>
       </c>
+      <c r="B48">
+        <v>315</v>
+      </c>
       <c r="D48" s="2">
         <v>106</v>
       </c>
@@ -14509,10 +16145,10 @@
       <c r="A53" s="1">
         <v>44874</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53">
         <v>320</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53">
         <v>120</v>
       </c>
       <c r="D53" s="2">
@@ -14617,6 +16253,120 @@
       <c r="AJ53" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>44890</v>
+      </c>
+      <c r="B54" s="4">
+        <v>323</v>
+      </c>
+      <c r="C54" s="4">
+        <v>120</v>
+      </c>
+      <c r="D54" s="2">
+        <v>109</v>
+      </c>
+      <c r="E54" s="2">
+        <v>260</v>
+      </c>
+      <c r="F54" s="2">
+        <v>213</v>
+      </c>
+      <c r="G54" s="2">
+        <v>5447</v>
+      </c>
+      <c r="H54" s="3">
+        <f>Data[[#This Row],[LoC]]-G53</f>
+        <v>4</v>
+      </c>
+      <c r="I54" s="2">
+        <v>6285</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1898</v>
+      </c>
+      <c r="K54" s="2">
+        <v>265</v>
+      </c>
+      <c r="L54" s="2">
+        <v>279</v>
+      </c>
+      <c r="M54" s="2">
+        <v>99</v>
+      </c>
+      <c r="N54" s="2">
+        <v>57</v>
+      </c>
+      <c r="O54" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8883</v>
+      </c>
+      <c r="P54" s="3">
+        <f>Data[[#This Row],[Total]]-O53</f>
+        <v>15</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>1956</v>
+      </c>
+      <c r="R54" s="2">
+        <v>4109</v>
+      </c>
+      <c r="S54" s="2">
+        <v>65535</v>
+      </c>
+      <c r="T54" s="2">
+        <v>45441</v>
+      </c>
+      <c r="U54" s="2">
+        <v>0</v>
+      </c>
+      <c r="V54" s="2">
+        <v>0</v>
+      </c>
+      <c r="W54" s="2">
+        <v>243</v>
+      </c>
+      <c r="X54" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>243</v>
+      </c>
+      <c r="Y54" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>168</v>
+      </c>
+      <c r="AA54" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>168</v>
+      </c>
+      <c r="AB54" s="2">
+        <v>153</v>
+      </c>
+      <c r="AC54" s="2">
+        <v>164</v>
+      </c>
+      <c r="AD54" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE54" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF54" s="2">
+        <v>367</v>
+      </c>
+      <c r="AG54" s="2">
+        <v>951</v>
+      </c>
+      <c r="AH54" s="2">
+        <v>9</v>
+      </c>
+      <c r="AI54" s="2"/>
+      <c r="AJ54" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Partially filled. Temporary commit
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F335F6EC-A7F4-0849-9805-5C4891BD83CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7258EC-DAC2-994B-A5E8-753B435D7AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12240" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -373,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -538,16 +538,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$55</c:f>
+              <c:f>Data!$G$2:$G$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -709,6 +712,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>5447</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,10 +754,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -913,16 +919,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$55</c:f>
+              <c:f>Data!$Q$2:$Q$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1084,6 +1093,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,10 +1135,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1288,16 +1300,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$55</c:f>
+              <c:f>Data!$R$2:$R$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1459,6 +1474,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>4122</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,10 +1732,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1879,16 +1897,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$55</c:f>
+              <c:f>Data!$V$2:$V$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2049,6 +2070,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2089,10 +2113,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2254,16 +2278,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$55</c:f>
+              <c:f>Data!$Y$2:$Y$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2424,6 +2451,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2464,10 +2494,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2629,16 +2659,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$55</c:f>
+              <c:f>Data!$U$2:$U$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2799,6 +2832,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3058,10 +3094,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3223,16 +3259,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$55</c:f>
+              <c:f>Data!$X$2:$X$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3394,6 +3433,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3433,10 +3475,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3598,16 +3640,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$55</c:f>
+              <c:f>Data!$AA$2:$AA$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3769,6 +3814,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4024,10 +4072,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4189,16 +4237,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$55</c:f>
+              <c:f>Data!$AC$2:$AC$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -4359,6 +4410,9 @@
                   <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
@@ -4581,10 +4635,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4746,16 +4800,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$55</c:f>
+              <c:f>Data!$AE$2:$AE$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4850,6 +4907,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4886,10 +4946,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5051,16 +5111,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$55</c:f>
+              <c:f>Data!$AF$2:$AF$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -5156,6 +5219,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5191,10 +5257,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5356,16 +5422,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$55</c:f>
+              <c:f>Data!$AG$2:$AG$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -5461,6 +5530,9 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>961</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5496,10 +5568,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5661,16 +5733,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$55</c:f>
+              <c:f>Data!$AH$2:$AH$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -5765,6 +5840,9 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -5803,10 +5881,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5968,16 +6046,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$55</c:f>
+              <c:f>Data!$AI$2:$AI$56</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -6296,10 +6377,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6461,16 +6542,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$55</c:f>
+              <c:f>Data!$B$2:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -6631,6 +6715,9 @@
                   <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>325</c:v>
                 </c:pt>
               </c:numCache>
@@ -6671,10 +6758,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$55</c:f>
+              <c:f>Data!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6836,16 +6923,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>44893</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$55</c:f>
+              <c:f>Data!$C$2:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -6865,6 +6955,9 @@
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
@@ -10641,8 +10734,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ55" totalsRowShown="0">
-  <autoFilter ref="A1:AJ55" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ56" totalsRowShown="0">
+  <autoFilter ref="A1:AJ56" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -10994,11 +11087,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ55"/>
+  <dimension ref="A1:AJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI55" sqref="AI55"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG56" sqref="AG56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16576,6 +16669,120 @@
         <v>1340</v>
       </c>
     </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B56" s="4">
+        <v>325</v>
+      </c>
+      <c r="C56" s="4">
+        <v>120</v>
+      </c>
+      <c r="D56" s="2">
+        <v>110</v>
+      </c>
+      <c r="E56" s="2">
+        <v>261</v>
+      </c>
+      <c r="F56" s="2">
+        <v>214</v>
+      </c>
+      <c r="G56" s="2">
+        <v>5457</v>
+      </c>
+      <c r="H56" s="3">
+        <f>Data[[#This Row],[LoC]]-G55</f>
+        <v>10</v>
+      </c>
+      <c r="I56" s="2">
+        <v>6295</v>
+      </c>
+      <c r="J56" s="2">
+        <v>1904</v>
+      </c>
+      <c r="K56" s="2">
+        <v>265</v>
+      </c>
+      <c r="L56" s="2">
+        <v>280</v>
+      </c>
+      <c r="M56" s="2">
+        <v>106</v>
+      </c>
+      <c r="N56" s="2">
+        <v>57</v>
+      </c>
+      <c r="O56" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8907</v>
+      </c>
+      <c r="P56" s="3">
+        <f>Data[[#This Row],[Total]]-O55</f>
+        <v>16</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>1981</v>
+      </c>
+      <c r="R56" s="2">
+        <v>4152</v>
+      </c>
+      <c r="S56" s="2">
+        <v>65878</v>
+      </c>
+      <c r="T56" s="2">
+        <v>45728</v>
+      </c>
+      <c r="U56" s="2">
+        <v>0</v>
+      </c>
+      <c r="V56" s="2">
+        <v>0</v>
+      </c>
+      <c r="W56" s="2">
+        <v>244</v>
+      </c>
+      <c r="X56" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>244</v>
+      </c>
+      <c r="Y56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>169</v>
+      </c>
+      <c r="AA56" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>169</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>154</v>
+      </c>
+      <c r="AC56" s="2">
+        <v>164</v>
+      </c>
+      <c r="AD56" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF56" s="2">
+        <v>370</v>
+      </c>
+      <c r="AG56" s="2">
+        <v>977</v>
+      </c>
+      <c r="AH56" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI56" s="2"/>
+      <c r="AJ56" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1358</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removing the tests with --security-level as the result depends on the used OpenSSL version
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155E7A8D-9D3A-2943-894B-1F45B841C3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AA8018-55B4-7245-BC2E-55DF6ECCF0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24500" activeTab="6" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="13520" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -373,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -547,16 +547,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$58</c:f>
+              <c:f>Data!$G$2:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -727,6 +730,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>5460</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,10 +772,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -940,16 +946,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$58</c:f>
+              <c:f>Data!$Q$2:$Q$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1120,6 +1129,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1159,10 +1171,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1333,16 +1345,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$58</c:f>
+              <c:f>Data!$R$2:$R$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1513,6 +1528,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>4174</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,10 +1786,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1942,16 +1960,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$58</c:f>
+              <c:f>Data!$V$2:$V$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2121,6 +2142,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2161,10 +2185,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2335,16 +2359,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$58</c:f>
+              <c:f>Data!$Y$2:$Y$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2514,6 +2541,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2554,10 +2584,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2728,16 +2758,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$58</c:f>
+              <c:f>Data!$U$2:$U$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2907,6 +2940,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3166,10 +3202,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3340,16 +3376,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$58</c:f>
+              <c:f>Data!$X$2:$X$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3520,6 +3559,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>247</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3559,10 +3601,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3733,16 +3775,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$58</c:f>
+              <c:f>Data!$AA$2:$AA$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -3912,6 +3957,9 @@
                   <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>170</c:v>
                 </c:pt>
               </c:numCache>
@@ -4168,10 +4216,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4342,16 +4390,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$58</c:f>
+              <c:f>Data!$AC$2:$AC$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -4743,10 +4794,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4917,16 +4968,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$58</c:f>
+              <c:f>Data!$AE$2:$AE$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5066,10 +5120,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5240,16 +5294,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$58</c:f>
+              <c:f>Data!$AF$2:$AF$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -5389,10 +5446,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5563,16 +5620,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$58</c:f>
+              <c:f>Data!$AG$2:$AG$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -5712,10 +5772,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5886,16 +5946,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$58</c:f>
+              <c:f>Data!$AH$2:$AH$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -6037,10 +6100,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6211,16 +6274,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$58</c:f>
+              <c:f>Data!$AI$2:$AI$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -6539,10 +6605,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6713,16 +6779,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$58</c:f>
+              <c:f>Data!$B$2:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -6893,6 +6962,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6932,10 +7004,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$58</c:f>
+              <c:f>Data!$A$2:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7106,16 +7178,19 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>44912</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$58</c:f>
+              <c:f>Data!$C$2:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="57"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -7145,6 +7220,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10714,7 +10792,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3CF196A6-E282-444D-AFF0-E87110025633}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10920,8 +10998,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ58" totalsRowShown="0">
-  <autoFilter ref="A1:AJ58" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ59" totalsRowShown="0">
+  <autoFilter ref="A1:AJ59" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -11273,11 +11351,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ58"/>
+  <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ58" sqref="AJ58"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI59" sqref="AI59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17087,10 +17165,10 @@
       <c r="A58" s="1">
         <v>44912</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58">
         <v>325</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58">
         <v>121</v>
       </c>
       <c r="D58" s="2">
@@ -17195,6 +17273,108 @@
       <c r="AJ58" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1386</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>44942</v>
+      </c>
+      <c r="B59" s="4">
+        <v>326</v>
+      </c>
+      <c r="C59" s="4">
+        <v>122</v>
+      </c>
+      <c r="D59" s="2">
+        <v>110</v>
+      </c>
+      <c r="E59" s="2">
+        <v>263</v>
+      </c>
+      <c r="F59" s="2">
+        <v>216</v>
+      </c>
+      <c r="G59" s="2">
+        <v>5491</v>
+      </c>
+      <c r="H59" s="3">
+        <f>Data[[#This Row],[LoC]]-G58</f>
+        <v>31</v>
+      </c>
+      <c r="I59" s="2">
+        <v>6364</v>
+      </c>
+      <c r="J59" s="2">
+        <v>1916</v>
+      </c>
+      <c r="K59" s="2">
+        <v>265</v>
+      </c>
+      <c r="L59" s="2">
+        <v>285</v>
+      </c>
+      <c r="M59" s="2">
+        <v>106</v>
+      </c>
+      <c r="N59" s="2">
+        <v>60</v>
+      </c>
+      <c r="O59" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>8996</v>
+      </c>
+      <c r="P59" s="3">
+        <f>Data[[#This Row],[Total]]-O58</f>
+        <v>57</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>2002</v>
+      </c>
+      <c r="R59" s="2">
+        <v>4201</v>
+      </c>
+      <c r="S59" s="2">
+        <v>66282</v>
+      </c>
+      <c r="T59" s="2">
+        <v>46002</v>
+      </c>
+      <c r="U59" s="2">
+        <v>0</v>
+      </c>
+      <c r="V59" s="2">
+        <v>0</v>
+      </c>
+      <c r="W59" s="2">
+        <v>247</v>
+      </c>
+      <c r="X59" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>247</v>
+      </c>
+      <c r="Y59" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="2">
+        <v>170</v>
+      </c>
+      <c r="AA59" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>170</v>
+      </c>
+      <c r="AB59" s="2">
+        <v>156</v>
+      </c>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+      <c r="AG59" s="2"/>
+      <c r="AH59" s="2"/>
+      <c r="AI59" s="2"/>
+      <c r="AJ59" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed another incosistent test
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AA8018-55B4-7245-BC2E-55DF6ECCF0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0F9E2B-4B55-464D-97C0-416F14A4B5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="13520" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -4574,6 +4574,9 @@
                 <c:pt idx="56">
                   <c:v>165</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>166</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5086,6 +5089,9 @@
                 <c:pt idx="56">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6062,6 +6068,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -11355,7 +11364,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI59" sqref="AI59"/>
+      <selection pane="bottomLeft" activeCell="AJ59" sqref="AJ59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17365,16 +17374,24 @@
       <c r="AB59" s="2">
         <v>156</v>
       </c>
-      <c r="AC59" s="2"/>
-      <c r="AD59" s="2"/>
-      <c r="AE59" s="2"/>
+      <c r="AC59" s="2">
+        <v>166</v>
+      </c>
+      <c r="AD59" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE59" s="2">
+        <v>0</v>
+      </c>
       <c r="AF59" s="2"/>
       <c r="AG59" s="2"/>
-      <c r="AH59" s="2"/>
+      <c r="AH59" s="2">
+        <v>11</v>
+      </c>
       <c r="AI59" s="2"/>
       <c r="AJ59" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the statistics after the last release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0F9E2B-4B55-464D-97C0-416F14A4B5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540736B-BEBF-5B46-9EAC-DDB9EFB2FF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="13520" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -1131,7 +1131,7 @@
                   <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2002</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,7 +1530,7 @@
                   <c:v>4174</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4201</c:v>
+                  <c:v>4205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4575,7 +4575,7 @@
                   <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>166</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5418,6 +5418,9 @@
                 <c:pt idx="56">
                   <c:v>370</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>376</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5743,6 +5746,9 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11362,9 +11368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
   <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ59" sqref="AJ59"/>
+      <selection pane="bottomLeft" activeCell="AH59" sqref="AH59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17311,7 +17317,7 @@
         <v>31</v>
       </c>
       <c r="I59" s="2">
-        <v>6364</v>
+        <v>6354</v>
       </c>
       <c r="J59" s="2">
         <v>1916</v>
@@ -17330,23 +17336,23 @@
       </c>
       <c r="O59" s="2">
         <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
-        <v>8996</v>
+        <v>8986</v>
       </c>
       <c r="P59" s="3">
         <f>Data[[#This Row],[Total]]-O58</f>
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="Q59" s="2">
-        <v>2002</v>
+        <v>2004</v>
       </c>
       <c r="R59" s="2">
-        <v>4201</v>
+        <v>4205</v>
       </c>
       <c r="S59" s="2">
         <v>66282</v>
       </c>
       <c r="T59" s="2">
-        <v>46002</v>
+        <v>46016</v>
       </c>
       <c r="U59" s="2">
         <v>0</v>
@@ -17375,7 +17381,7 @@
         <v>156</v>
       </c>
       <c r="AC59" s="2">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AD59" s="2">
         <v>4</v>
@@ -17383,15 +17389,19 @@
       <c r="AE59" s="2">
         <v>0</v>
       </c>
-      <c r="AF59" s="2"/>
-      <c r="AG59" s="2"/>
+      <c r="AF59" s="2">
+        <v>376</v>
+      </c>
+      <c r="AG59" s="2">
+        <v>1023</v>
+      </c>
       <c r="AH59" s="2">
         <v>11</v>
       </c>
       <c r="AI59" s="2"/>
       <c r="AJ59" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
-        <v>11</v>
+        <v>1410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hot fix for version 2.59 (bug fix for ```--ignore-host-name```)
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C3AF6-EF6F-D944-A71B-BE218633FA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524DF9E4-632D-F042-AE2F-DBAE781860A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="13520" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24580" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -373,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -553,16 +553,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$60</c:f>
+              <c:f>Data!$G$2:$G$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -778,10 +781,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -958,16 +961,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$60</c:f>
+              <c:f>Data!$Q$2:$Q$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1183,10 +1189,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1363,16 +1369,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$60</c:f>
+              <c:f>Data!$R$2:$R$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1804,10 +1813,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1984,16 +1993,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$60</c:f>
+              <c:f>Data!$V$2:$V$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2209,10 +2221,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2389,16 +2401,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$60</c:f>
+              <c:f>Data!$Y$2:$Y$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2614,10 +2629,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2794,16 +2809,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$60</c:f>
+              <c:f>Data!$U$2:$U$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3238,10 +3256,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3418,16 +3436,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$60</c:f>
+              <c:f>Data!$X$2:$X$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3604,6 +3625,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3643,10 +3667,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3823,16 +3847,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$60</c:f>
+              <c:f>Data!$AA$2:$AA$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -4009,6 +4036,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4264,10 +4294,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4444,16 +4474,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$60</c:f>
+              <c:f>Data!$AC$2:$AC$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -4851,10 +4884,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5031,16 +5064,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$60</c:f>
+              <c:f>Data!$AE$2:$AE$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5186,10 +5222,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5366,16 +5402,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$60</c:f>
+              <c:f>Data!$AF$2:$AF$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -5521,10 +5560,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5701,16 +5740,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$60</c:f>
+              <c:f>Data!$AG$2:$AG$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -5856,10 +5898,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6036,16 +6078,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$60</c:f>
+              <c:f>Data!$AH$2:$AH$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -6193,10 +6238,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6373,16 +6418,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$60</c:f>
+              <c:f>Data!$AI$2:$AI$61</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -6701,10 +6749,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6881,16 +6929,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$60</c:f>
+              <c:f>Data!$B$2:$B$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -7106,10 +7157,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$60</c:f>
+              <c:f>Data!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7286,16 +7337,19 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$60</c:f>
+              <c:f>Data!$C$2:$C$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -11106,8 +11160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ60" totalsRowShown="0">
-  <autoFilter ref="A1:AJ60" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ61" totalsRowShown="0">
+  <autoFilter ref="A1:AJ61" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -11459,11 +11513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ60"/>
+  <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ60" sqref="AJ60"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17501,10 +17555,10 @@
       <c r="A60" s="1">
         <v>44953</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60">
         <v>328</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60">
         <v>124</v>
       </c>
       <c r="D60" s="2">
@@ -17609,6 +17663,64 @@
       <c r="AJ60" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1419</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44972</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="3">
+        <f>Data[[#This Row],[LoC]]-G60</f>
+        <v>-5504</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>0</v>
+      </c>
+      <c r="P61" s="3">
+        <f>Data[[#This Row],[Total]]-O60</f>
+        <v>-9003</v>
+      </c>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+      <c r="X61" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="2"/>
+      <c r="Z61" s="2"/>
+      <c r="AA61" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>0</v>
+      </c>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="2"/>
+      <c r="AE61" s="2"/>
+      <c r="AF61" s="2"/>
+      <c r="AG61" s="2"/>
+      <c r="AH61" s="2"/>
+      <c r="AI61" s="2"/>
+      <c r="AJ61" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected the number of tests
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE00BA-19A8-FE4D-A900-6CF3B8BAC9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5642F77-5C40-C244-8F05-5CBBF528CC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24580" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24500" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -4682,7 +4682,7 @@
                   <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>165</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11553,9 +11553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
   <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ61" sqref="AJ61"/>
+      <selection pane="bottomLeft" activeCell="AC62" sqref="AC62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17794,7 +17794,7 @@
         <v>156</v>
       </c>
       <c r="AC61" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AD61" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
Updated the stats (and the script)
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5642F77-5C40-C244-8F05-5CBBF528CC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE525FA-7BA8-C841-9000-3494329916D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24500" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24580" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -193,11 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,6 +557,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -743,6 +747,9 @@
                   <c:v>5504</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>5507</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>5507</c:v>
                 </c:pt>
               </c:numCache>
@@ -967,6 +974,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1155,6 +1165,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,6 +1391,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1566,6 +1582,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>4228</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2005,6 +2024,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2192,6 +2214,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2416,6 +2441,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2603,6 +2631,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2827,6 +2858,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3014,6 +3048,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3457,6 +3494,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3645,6 +3685,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3868,6 +3911,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4056,6 +4102,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4495,6 +4544,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4682,6 +4734,9 @@
                   <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>167</c:v>
                 </c:pt>
               </c:numCache>
@@ -5088,6 +5143,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5209,6 +5267,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5429,6 +5490,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5550,6 +5614,9 @@
                   <c:v>377</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>377</c:v>
                 </c:pt>
               </c:numCache>
@@ -5770,6 +5837,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5892,6 +5962,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6111,6 +6184,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -6232,6 +6308,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -6453,6 +6532,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>44972</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6965,6 +7047,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -7153,6 +7238,9 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7376,6 +7464,9 @@
                 <c:pt idx="59">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>44984</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -7422,6 +7513,9 @@
                   <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>125</c:v>
                 </c:pt>
               </c:numCache>
@@ -10937,7 +11031,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11003,7 +11097,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9311298" cy="6075240"/>
+    <xdr:ext cx="9304130" cy="6064710"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11198,8 +11292,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ61" totalsRowShown="0">
-  <autoFilter ref="A1:AJ61" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ62" totalsRowShown="0">
+  <autoFilter ref="A1:AJ62" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -11255,7 +11349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -11543,7 +11637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11551,11 +11645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ61"/>
+  <dimension ref="A1:AJ62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC62" sqref="AC62"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R68" sqref="R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17817,6 +17911,120 @@
         <v>1428</v>
       </c>
     </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44984</v>
+      </c>
+      <c r="B62" s="4">
+        <v>330</v>
+      </c>
+      <c r="C62" s="4">
+        <v>125</v>
+      </c>
+      <c r="D62" s="2">
+        <v>110</v>
+      </c>
+      <c r="E62" s="2">
+        <v>265</v>
+      </c>
+      <c r="F62" s="2">
+        <v>218</v>
+      </c>
+      <c r="G62" s="2">
+        <v>5507</v>
+      </c>
+      <c r="H62" s="3">
+        <f>Data[[#This Row],[LoC]]-G61</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="2">
+        <v>6537</v>
+      </c>
+      <c r="J62" s="2">
+        <v>1920</v>
+      </c>
+      <c r="K62" s="2">
+        <v>385</v>
+      </c>
+      <c r="L62" s="2">
+        <v>285</v>
+      </c>
+      <c r="M62" s="2">
+        <v>114</v>
+      </c>
+      <c r="N62" s="2">
+        <v>60</v>
+      </c>
+      <c r="O62" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>9301</v>
+      </c>
+      <c r="P62" s="3">
+        <f>Data[[#This Row],[Total]]-O61</f>
+        <v>292</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>2023</v>
+      </c>
+      <c r="R62" s="2">
+        <v>4244</v>
+      </c>
+      <c r="S62" s="2">
+        <v>68323</v>
+      </c>
+      <c r="T62" s="2">
+        <v>47625</v>
+      </c>
+      <c r="U62" s="2">
+        <v>0</v>
+      </c>
+      <c r="V62" s="2">
+        <v>0</v>
+      </c>
+      <c r="W62" s="2">
+        <v>251</v>
+      </c>
+      <c r="X62" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>251</v>
+      </c>
+      <c r="Y62" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="2">
+        <v>173</v>
+      </c>
+      <c r="AA62" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>173</v>
+      </c>
+      <c r="AB62" s="2">
+        <v>156</v>
+      </c>
+      <c r="AC62" s="2">
+        <v>167</v>
+      </c>
+      <c r="AD62" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE62" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="2">
+        <v>377</v>
+      </c>
+      <c r="AG62" s="2">
+        <v>1066</v>
+      </c>
+      <c r="AH62" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI62" s="2"/>
+      <c r="AJ62" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1454</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stats after the release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA3706E-8503-6E4F-96C7-C32EBCF288AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E697E8-D8D1-7A47-B1C2-079E510DB3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24580" activeTab="1" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12260" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -373,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -574,16 +574,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$67</c:f>
+              <c:f>Data!$G$2:$G$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -781,6 +784,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>5525</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,10 +826,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1021,16 +1027,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$67</c:f>
+              <c:f>Data!$Q$2:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1228,6 +1237,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,10 +1279,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1468,16 +1480,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$67</c:f>
+              <c:f>Data!$R$2:$R$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1675,6 +1690,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>4274</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1930,10 +1948,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2131,16 +2149,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$67</c:f>
+              <c:f>Data!$V$2:$V$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2337,6 +2358,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2377,10 +2401,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2578,16 +2602,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$67</c:f>
+              <c:f>Data!$Y$2:$Y$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2784,6 +2811,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2824,10 +2854,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3025,16 +3055,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$67</c:f>
+              <c:f>Data!$U$2:$U$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3231,6 +3264,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3490,10 +3526,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3691,16 +3727,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$67</c:f>
+              <c:f>Data!$X$2:$X$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -3898,6 +3937,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3937,10 +3979,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4138,16 +4180,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$67</c:f>
+              <c:f>Data!$AA$2:$AA$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -4344,6 +4389,9 @@
                   <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>173</c:v>
                 </c:pt>
               </c:numCache>
@@ -4600,10 +4648,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4801,16 +4849,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$67</c:f>
+              <c:f>Data!$AC$2:$AC$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -5008,6 +5059,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5229,10 +5283,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5430,16 +5484,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$67</c:f>
+              <c:f>Data!$AE$2:$AE$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5570,6 +5627,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5606,10 +5666,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5807,16 +5867,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$67</c:f>
+              <c:f>Data!$AF$2:$AF$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -5948,6 +6011,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>388</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5983,10 +6049,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6184,16 +6250,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$67</c:f>
+              <c:f>Data!$AG$2:$AG$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -6325,6 +6394,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6360,10 +6432,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6561,16 +6633,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$67</c:f>
+              <c:f>Data!$AH$2:$AH$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -6701,6 +6776,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -6739,10 +6817,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6940,16 +7018,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$67</c:f>
+              <c:f>Data!$AI$2:$AI$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7268,10 +7349,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7469,16 +7550,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$67</c:f>
+              <c:f>Data!$B$2:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -7676,6 +7760,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7715,10 +7802,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$67</c:f>
+              <c:f>Data!$A$2:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7916,16 +8003,19 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$67</c:f>
+              <c:f>Data!$C$2:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="67"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -7982,6 +8072,9 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11496,7 +11589,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11757,8 +11850,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ67" totalsRowShown="0">
-  <autoFilter ref="A1:AJ67" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ68" totalsRowShown="0">
+  <autoFilter ref="A1:AJ68" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -12110,11 +12203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ67"/>
+  <dimension ref="A1:AJ68"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ67" sqref="AJ67"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB71" sqref="AB71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18950,10 +19043,10 @@
       <c r="A67" s="1">
         <v>45001</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67">
         <v>329</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67">
         <v>125</v>
       </c>
       <c r="D67" s="2">
@@ -19058,6 +19151,120 @@
       <c r="AJ67" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45021</v>
+      </c>
+      <c r="B68" s="4">
+        <v>331</v>
+      </c>
+      <c r="C68" s="4">
+        <v>126</v>
+      </c>
+      <c r="D68" s="2">
+        <v>111</v>
+      </c>
+      <c r="E68" s="2">
+        <v>268</v>
+      </c>
+      <c r="F68" s="2">
+        <v>221</v>
+      </c>
+      <c r="G68" s="2">
+        <v>5566</v>
+      </c>
+      <c r="H68" s="3">
+        <f>Data[[#This Row],[LoC]]-G67</f>
+        <v>41</v>
+      </c>
+      <c r="I68" s="2">
+        <v>6587</v>
+      </c>
+      <c r="J68" s="2">
+        <v>1931</v>
+      </c>
+      <c r="K68" s="2">
+        <v>385</v>
+      </c>
+      <c r="L68" s="2">
+        <v>287</v>
+      </c>
+      <c r="M68" s="2">
+        <v>114</v>
+      </c>
+      <c r="N68" s="2">
+        <v>60</v>
+      </c>
+      <c r="O68" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>9364</v>
+      </c>
+      <c r="P68" s="3">
+        <f>Data[[#This Row],[Total]]-O67</f>
+        <v>41</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>2045</v>
+      </c>
+      <c r="R68" s="2">
+        <v>4296</v>
+      </c>
+      <c r="S68" s="2">
+        <v>68527</v>
+      </c>
+      <c r="T68" s="2">
+        <v>47701</v>
+      </c>
+      <c r="U68" s="2">
+        <v>0</v>
+      </c>
+      <c r="V68" s="2">
+        <v>0</v>
+      </c>
+      <c r="W68" s="2">
+        <v>257</v>
+      </c>
+      <c r="X68" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>257</v>
+      </c>
+      <c r="Y68" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="2">
+        <v>173</v>
+      </c>
+      <c r="AA68" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>173</v>
+      </c>
+      <c r="AB68" s="2">
+        <v>157</v>
+      </c>
+      <c r="AC68" s="2">
+        <v>166</v>
+      </c>
+      <c r="AD68" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE68" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="2">
+        <v>388</v>
+      </c>
+      <c r="AG68" s="2">
+        <v>1143</v>
+      </c>
+      <c r="AH68" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI68" s="2"/>
+      <c r="AJ68" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the statistics after release
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A392C24F-5998-714D-93CD-47C9AA130AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA7F3F9-6156-004C-9BED-BDCEB52E22D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12260" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -193,11 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -585,16 +586,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$71</c:f>
+              <c:f>Data!$G$2:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -804,6 +808,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>5576</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5618</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,10 +850,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1056,16 +1063,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$71</c:f>
+              <c:f>Data!$Q$2:$Q$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1275,6 +1285,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,10 +1327,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1527,16 +1540,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$71</c:f>
+              <c:f>Data!$R$2:$R$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1746,6 +1762,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>4333</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,10 +2020,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2214,16 +2233,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$71</c:f>
+              <c:f>Data!$V$2:$V$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2432,6 +2454,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2472,10 +2497,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2685,16 +2710,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$71</c:f>
+              <c:f>Data!$Y$2:$Y$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2903,6 +2931,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2943,10 +2974,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3156,16 +3187,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$71</c:f>
+              <c:f>Data!$U$2:$U$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3374,6 +3408,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3633,10 +3670,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3846,16 +3883,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$71</c:f>
+              <c:f>Data!$X$2:$X$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -4065,6 +4105,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4104,10 +4147,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4317,16 +4360,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$71</c:f>
+              <c:f>Data!$AA$2:$AA$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -4535,6 +4581,9 @@
                   <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>174</c:v>
                 </c:pt>
               </c:numCache>
@@ -4791,10 +4840,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5004,16 +5053,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$71</c:f>
+              <c:f>Data!$AC$2:$AC$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -5222,6 +5274,9 @@
                   <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
@@ -5444,10 +5499,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5657,16 +5712,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$71</c:f>
+              <c:f>Data!$AE$2:$AE$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5809,6 +5867,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5845,10 +5906,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6058,16 +6119,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$71</c:f>
+              <c:f>Data!$AF$2:$AF$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -6211,6 +6275,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6246,10 +6313,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6459,16 +6526,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$71</c:f>
+              <c:f>Data!$AG$2:$AG$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -6612,6 +6682,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>1184</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6647,10 +6720,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6860,16 +6933,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$71</c:f>
+              <c:f>Data!$AH$2:$AH$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -7012,6 +7088,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -7050,10 +7129,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7263,16 +7342,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$71</c:f>
+              <c:f>Data!$AI$2:$AI$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7591,10 +7673,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7804,16 +7886,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$71</c:f>
+              <c:f>Data!$B$2:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -8023,6 +8108,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8062,10 +8150,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$71</c:f>
+              <c:f>Data!$A$2:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -8275,16 +8363,19 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$71</c:f>
+              <c:f>Data!$C$2:$C$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="70"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -8353,6 +8444,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12128,8 +12222,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ71" totalsRowShown="0">
-  <autoFilter ref="A1:AJ71" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ72" totalsRowShown="0">
+  <autoFilter ref="A1:AJ72" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -12481,11 +12575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ71"/>
+  <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI71" sqref="AI71"/>
+      <selection pane="bottomLeft" activeCell="AI72" sqref="AI72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19887,6 +19981,120 @@
         <v>1592</v>
       </c>
     </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B72" s="4">
+        <v>333</v>
+      </c>
+      <c r="C72" s="4">
+        <v>128</v>
+      </c>
+      <c r="D72" s="2">
+        <v>112</v>
+      </c>
+      <c r="E72" s="2">
+        <v>273</v>
+      </c>
+      <c r="F72" s="2">
+        <v>224</v>
+      </c>
+      <c r="G72" s="2">
+        <v>5618</v>
+      </c>
+      <c r="H72" s="3">
+        <f>Data[[#This Row],[LoC]]-G71</f>
+        <v>42</v>
+      </c>
+      <c r="I72" s="2">
+        <v>6646</v>
+      </c>
+      <c r="J72" s="2">
+        <v>1945</v>
+      </c>
+      <c r="K72" s="2">
+        <v>385</v>
+      </c>
+      <c r="L72" s="2">
+        <v>287</v>
+      </c>
+      <c r="M72" s="2">
+        <v>114</v>
+      </c>
+      <c r="N72" s="2">
+        <v>60</v>
+      </c>
+      <c r="O72" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>9437</v>
+      </c>
+      <c r="P72" s="3">
+        <f>Data[[#This Row],[Total]]-O71</f>
+        <v>48</v>
+      </c>
+      <c r="Q72" s="2">
+        <v>2066</v>
+      </c>
+      <c r="R72" s="2">
+        <v>4357</v>
+      </c>
+      <c r="S72" s="2">
+        <v>68813</v>
+      </c>
+      <c r="T72" s="2">
+        <v>47851</v>
+      </c>
+      <c r="U72" s="2">
+        <v>0</v>
+      </c>
+      <c r="V72" s="2">
+        <v>0</v>
+      </c>
+      <c r="W72" s="2">
+        <v>261</v>
+      </c>
+      <c r="X72" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>261</v>
+      </c>
+      <c r="Y72" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="2">
+        <v>174</v>
+      </c>
+      <c r="AA72" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>174</v>
+      </c>
+      <c r="AB72" s="2">
+        <v>157</v>
+      </c>
+      <c r="AC72" s="2">
+        <v>164</v>
+      </c>
+      <c r="AD72" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE72" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="2">
+        <v>407</v>
+      </c>
+      <c r="AG72" s="2">
+        <v>1207</v>
+      </c>
+      <c r="AH72" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI72" s="2"/>
+      <c r="AJ72" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1625</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed the stats script and updated the statistics
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A25CB27-E22D-F342-9A4A-5BD1FFAFD87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF703DC-8D00-0A4B-89CC-D7E3C449DDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="12260" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
@@ -373,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -592,16 +592,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$73</c:f>
+              <c:f>Data!$G$2:$G$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -816,6 +819,9 @@
                   <c:v>5618</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>5682</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>5682</c:v>
                 </c:pt>
               </c:numCache>
@@ -856,10 +862,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1075,16 +1081,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$73</c:f>
+              <c:f>Data!$Q$2:$Q$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1300,6 +1309,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1339,10 +1351,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1558,16 +1570,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$73</c:f>
+              <c:f>Data!$R$2:$R$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1783,6 +1798,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>4379</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2038,10 +2056,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2257,16 +2275,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$73</c:f>
+              <c:f>Data!$V$2:$V$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2481,6 +2502,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2521,10 +2545,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2740,16 +2764,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$73</c:f>
+              <c:f>Data!$Y$2:$Y$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2964,6 +2991,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3004,10 +3034,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3223,16 +3253,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$U$2:$U$73</c:f>
+              <c:f>Data!$U$2:$U$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3447,6 +3480,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3706,10 +3742,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3925,16 +3961,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$2:$X$73</c:f>
+              <c:f>Data!$X$2:$X$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -4149,6 +4188,9 @@
                   <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>262</c:v>
                 </c:pt>
               </c:numCache>
@@ -4189,10 +4231,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4408,16 +4450,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$73</c:f>
+              <c:f>Data!$AA$2:$AA$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -4633,6 +4678,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4888,10 +4936,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5107,16 +5155,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$73</c:f>
+              <c:f>Data!$AC$2:$AC$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -5331,6 +5382,9 @@
                   <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
@@ -5553,10 +5607,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5772,16 +5826,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$73</c:f>
+              <c:f>Data!$AE$2:$AE$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5930,6 +5987,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5966,10 +6026,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6185,16 +6245,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$73</c:f>
+              <c:f>Data!$AF$2:$AF$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -6344,6 +6407,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6379,10 +6445,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6598,16 +6664,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$73</c:f>
+              <c:f>Data!$AG$2:$AG$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -6757,6 +6826,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>1228</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1245</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6792,10 +6864,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7011,16 +7083,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$73</c:f>
+              <c:f>Data!$AH$2:$AH$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -7169,6 +7244,9 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="71">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="72">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -7207,10 +7285,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7426,16 +7504,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$73</c:f>
+              <c:f>Data!$AI$2:$AI$74</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -7754,10 +7835,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7973,16 +8054,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$73</c:f>
+              <c:f>Data!$B$2:$B$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -8198,6 +8282,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8237,10 +8324,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$73</c:f>
+              <c:f>Data!$A$2:$A$74</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -8456,16 +8543,19 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>45058</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$73</c:f>
+              <c:f>Data!$C$2:$C$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="73"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -8540,6 +8630,9 @@
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12315,8 +12408,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ73" totalsRowShown="0">
-  <autoFilter ref="A1:AJ73" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AJ74" totalsRowShown="0">
+  <autoFilter ref="A1:AJ74" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="35"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="34"/>
@@ -12668,11 +12761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AJ73"/>
+  <dimension ref="A1:AJ74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI71" sqref="AI71"/>
+      <selection pane="bottomLeft" activeCell="AJ74" sqref="AJ74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20192,10 +20285,10 @@
       <c r="A73" s="1">
         <v>45058</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73">
         <v>335</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73">
         <v>128</v>
       </c>
       <c r="D73" s="2">
@@ -20300,6 +20393,120 @@
       <c r="AJ73" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1654</v>
+      </c>
+    </row>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>45061</v>
+      </c>
+      <c r="B74" s="4">
+        <v>336</v>
+      </c>
+      <c r="C74" s="4">
+        <v>129</v>
+      </c>
+      <c r="D74" s="2">
+        <v>113</v>
+      </c>
+      <c r="E74" s="2">
+        <v>274</v>
+      </c>
+      <c r="F74" s="2">
+        <v>225</v>
+      </c>
+      <c r="G74" s="2">
+        <v>5682</v>
+      </c>
+      <c r="H74" s="3">
+        <f>Data[[#This Row],[LoC]]-G73</f>
+        <v>0</v>
+      </c>
+      <c r="I74" s="2">
+        <v>6728</v>
+      </c>
+      <c r="J74" s="2">
+        <v>1952</v>
+      </c>
+      <c r="K74" s="2">
+        <v>385</v>
+      </c>
+      <c r="L74" s="2">
+        <v>290</v>
+      </c>
+      <c r="M74" s="2">
+        <v>114</v>
+      </c>
+      <c r="N74" s="2">
+        <v>60</v>
+      </c>
+      <c r="O74" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>9529</v>
+      </c>
+      <c r="P74" s="3">
+        <f>Data[[#This Row],[Total]]-O73</f>
+        <v>16</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>2079</v>
+      </c>
+      <c r="R74" s="2">
+        <v>4391</v>
+      </c>
+      <c r="S74" s="2">
+        <v>70047</v>
+      </c>
+      <c r="T74" s="2">
+        <v>48194</v>
+      </c>
+      <c r="U74" s="2">
+        <v>0</v>
+      </c>
+      <c r="V74" s="2">
+        <v>0</v>
+      </c>
+      <c r="W74" s="2">
+        <v>262</v>
+      </c>
+      <c r="X74" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>262</v>
+      </c>
+      <c r="Y74" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="2">
+        <v>175</v>
+      </c>
+      <c r="AA74" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>175</v>
+      </c>
+      <c r="AB74" s="2">
+        <v>159</v>
+      </c>
+      <c r="AC74" s="2">
+        <v>164</v>
+      </c>
+      <c r="AD74" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE74" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="2">
+        <v>416</v>
+      </c>
+      <c r="AG74" s="2">
+        <v>1245</v>
+      </c>
+      <c r="AH74" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI74" s="2"/>
+      <c r="AJ74" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ShellCheck fix (unused variable)
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808D41F6-83F8-B14D-8D43-FA74151E9056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA535AF-9A2F-4640-BD8A-09C2BC75A0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20520" windowHeight="24480" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="20600" yWindow="880" windowWidth="20520" windowHeight="24480" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -379,10 +379,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -625,16 +625,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$82</c:f>
+              <c:f>Data!$G$2:$G$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -877,6 +880,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>5743</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5754</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -916,10 +922,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1162,16 +1168,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$82</c:f>
+              <c:f>Data!$R$2:$R$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1414,6 +1423,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>2152</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,10 +1465,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1699,16 +1711,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$S$2:$S$82</c:f>
+              <c:f>Data!$S$2:$S$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -1951,6 +1966,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>4569</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,10 +2224,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2452,16 +2470,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$82</c:f>
+              <c:f>Data!$W$2:$W$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2704,6 +2725,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2743,10 +2767,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2989,16 +3013,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Z$2:$Z$82</c:f>
+              <c:f>Data!$Z$2:$Z$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3240,6 +3267,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3280,10 +3310,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3526,16 +3556,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$82</c:f>
+              <c:f>Data!$V$2:$V$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3778,6 +3811,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4036,10 +4072,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4282,16 +4318,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$82</c:f>
+              <c:f>Data!$Y$2:$Y$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -4534,6 +4573,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4573,10 +4615,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4819,16 +4861,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$82</c:f>
+              <c:f>Data!$AB$2:$AB$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -5070,6 +5115,9 @@
                   <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="80">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>178</c:v>
                 </c:pt>
               </c:numCache>
@@ -5326,10 +5374,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5572,16 +5620,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$82</c:f>
+              <c:f>Data!$AD$2:$AD$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -5824,6 +5875,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6045,10 +6099,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6291,16 +6345,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$82</c:f>
+              <c:f>Data!$AF$2:$AF$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6512,10 +6569,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6758,16 +6815,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$82</c:f>
+              <c:f>Data!$AG$2:$AG$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -6979,10 +7039,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7225,16 +7285,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$82</c:f>
+              <c:f>Data!$AH$2:$AH$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -7446,10 +7509,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7692,16 +7755,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$82</c:f>
+              <c:f>Data!$AI$2:$AI$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -7915,10 +7981,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -8161,16 +8227,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AJ$2:$AJ$82</c:f>
+              <c:f>Data!$AJ$2:$AJ$83</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -8489,10 +8558,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -8735,16 +8804,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$82</c:f>
+              <c:f>Data!$B$2:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -8987,6 +9059,9 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9026,10 +9101,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$82</c:f>
+              <c:f>Data!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -9272,16 +9347,19 @@
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$82</c:f>
+              <c:f>Data!$C$2:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -9382,6 +9460,9 @@
                   <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="80">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
@@ -13158,8 +13239,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AK82" totalsRowShown="0">
-  <autoFilter ref="A1:AK82" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AK83" totalsRowShown="0">
+  <autoFilter ref="A1:AK83" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="36"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="35"/>
@@ -13512,11 +13593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AK82"/>
+  <dimension ref="A1:AK83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK82" sqref="AK82"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB76" sqref="AB76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13531,7 +13612,8 @@
     <col min="9" max="9" width="7.5" customWidth="1"/>
     <col min="10" max="12" width="6.5" customWidth="1"/>
     <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="6.5" customWidth="1"/>
+    <col min="14" max="15" width="6.5" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
@@ -22152,10 +22234,10 @@
       <c r="A82" s="1">
         <v>45253</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82">
         <v>346</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82">
         <v>129</v>
       </c>
       <c r="D82" s="2">
@@ -22263,6 +22345,115 @@
       <c r="AK82" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1052</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B83" s="4">
+        <v>347</v>
+      </c>
+      <c r="C83" s="4">
+        <v>129</v>
+      </c>
+      <c r="D83" s="2">
+        <v>114</v>
+      </c>
+      <c r="E83" s="2">
+        <v>282</v>
+      </c>
+      <c r="F83" s="2">
+        <v>233</v>
+      </c>
+      <c r="G83" s="2">
+        <v>5754</v>
+      </c>
+      <c r="H83" s="3">
+        <f>Data[[#This Row],[LoC]]-G82</f>
+        <v>11</v>
+      </c>
+      <c r="I83" s="2">
+        <v>6920</v>
+      </c>
+      <c r="J83" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K83" s="2">
+        <v>563</v>
+      </c>
+      <c r="L83" s="2">
+        <v>417</v>
+      </c>
+      <c r="M83" s="2">
+        <v>134</v>
+      </c>
+      <c r="N83" s="2">
+        <v>60</v>
+      </c>
+      <c r="O83" s="2">
+        <v>16</v>
+      </c>
+      <c r="P83" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>10065</v>
+      </c>
+      <c r="Q83" s="3">
+        <f>Data[[#This Row],[Total]]-P82</f>
+        <v>144</v>
+      </c>
+      <c r="R83" s="2">
+        <v>2160</v>
+      </c>
+      <c r="S83" s="2">
+        <v>4583</v>
+      </c>
+      <c r="T83" s="2">
+        <v>71467</v>
+      </c>
+      <c r="U83" s="2">
+        <v>48982</v>
+      </c>
+      <c r="V83" s="2">
+        <v>2</v>
+      </c>
+      <c r="W83" s="2">
+        <v>1</v>
+      </c>
+      <c r="X83" s="2">
+        <v>285</v>
+      </c>
+      <c r="Y83" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>287</v>
+      </c>
+      <c r="Z83" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="2">
+        <v>178</v>
+      </c>
+      <c r="AB83" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>178</v>
+      </c>
+      <c r="AC83" s="2">
+        <v>159</v>
+      </c>
+      <c r="AD83" s="2">
+        <v>166</v>
+      </c>
+      <c r="AE83" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF83" s="2"/>
+      <c r="AG83" s="2"/>
+      <c r="AH83" s="2"/>
+      <c r="AI83" s="2"/>
+      <c r="AJ83" s="2"/>
+      <c r="AK83" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the stats after the last commit
</commit_message>
<xml_diff>
--- a/varia/check_ssl_cert_stats.xlsx
+++ b/varia/check_ssl_cert_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corti/git/check_ssl_cert/varia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F3AFC8-4112-F64C-9C16-F93BD26815BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529A6C0-A941-EE46-A930-7E90DE6464D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27100" activeTab="1" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24460" xr2:uid="{EF8E2D16-8F1A-D743-ABFE-CD06731F2ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -379,10 +379,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -637,16 +637,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$86</c:f>
+              <c:f>Data!$G$2:$G$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>4368</c:v>
                 </c:pt>
@@ -901,6 +904,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>5979</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -940,10 +946,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1198,16 +1204,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$R$2:$R$86</c:f>
+              <c:f>Data!$R$2:$R$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>1523</c:v>
                 </c:pt>
@@ -1462,6 +1471,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>2266</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,10 +1513,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -1759,16 +1771,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$S$2:$S$86</c:f>
+              <c:f>Data!$S$2:$S$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>3195</c:v>
                 </c:pt>
@@ -2023,6 +2038,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>4858</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2233,7 +2251,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2278,10 +2296,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -2536,16 +2554,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$2:$W$86</c:f>
+              <c:f>Data!$W$2:$W$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2799,6 +2820,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2839,10 +2863,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3097,16 +3121,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Z$2:$Z$86</c:f>
+              <c:f>Data!$Z$2:$Z$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3360,6 +3387,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3400,10 +3430,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -3658,16 +3688,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$V$2:$V$86</c:f>
+              <c:f>Data!$V$2:$V$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3922,6 +3955,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4135,7 +4171,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4180,10 +4216,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4438,16 +4474,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$86</c:f>
+              <c:f>Data!$Y$2:$Y$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>204</c:v>
                 </c:pt>
@@ -4702,6 +4741,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>315</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4741,10 +4783,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -4999,16 +5041,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$86</c:f>
+              <c:f>Data!$AB$2:$AB$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>135</c:v>
                 </c:pt>
@@ -5262,6 +5307,9 @@
                   <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>184</c:v>
                 </c:pt>
               </c:numCache>
@@ -5473,7 +5521,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5518,10 +5566,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -5776,16 +5824,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$86</c:f>
+              <c:f>Data!$AD$2:$AD$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>122</c:v>
                 </c:pt>
@@ -6039,6 +6090,9 @@
                   <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>136</c:v>
                 </c:pt>
               </c:numCache>
@@ -6219,7 +6273,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6261,10 +6315,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -6519,16 +6573,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$86</c:f>
+              <c:f>Data!$AF$2:$AF$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6716,6 +6773,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6752,10 +6812,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7010,16 +7070,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$86</c:f>
+              <c:f>Data!$AG$2:$AG$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="22">
                   <c:v>302</c:v>
                 </c:pt>
@@ -7208,6 +7271,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7243,10 +7309,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7501,16 +7567,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AH$2:$AH$86</c:f>
+              <c:f>Data!$AH$2:$AH$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="22">
                   <c:v>488</c:v>
                 </c:pt>
@@ -7699,6 +7768,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>1202</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7734,10 +7806,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -7992,16 +8064,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$86</c:f>
+              <c:f>Data!$AI$2:$AI$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="22">
                   <c:v>7</c:v>
                 </c:pt>
@@ -8190,6 +8265,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8227,10 +8305,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -8485,16 +8563,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$AJ$2:$AJ$86</c:f>
+              <c:f>Data!$AJ$2:$AJ$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>541</c:v>
                 </c:pt>
@@ -8768,7 +8849,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8813,10 +8894,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -9071,16 +9152,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$86</c:f>
+              <c:f>Data!$B$2:$B$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>274</c:v>
                 </c:pt>
@@ -9335,6 +9419,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9374,10 +9461,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$86</c:f>
+              <c:f>Data!$A$2:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="0">
                   <c:v>44574</c:v>
                 </c:pt>
@@ -9632,16 +9719,19 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$86</c:f>
+              <c:f>Data!$C$2:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="85"/>
+                <c:ptCount val="86"/>
                 <c:pt idx="47">
                   <c:v>118</c:v>
                 </c:pt>
@@ -9754,6 +9844,9 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="84">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="85">
                   <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
@@ -13269,7 +13362,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79BFC0E2-E15C-9645-95CF-EABB927DA6C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="234" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="207" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13335,7 +13428,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6073205"/>
+    <xdr:ext cx="9311298" cy="6075240"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -13530,8 +13623,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AK86" totalsRowShown="0">
-  <autoFilter ref="A1:AK86" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}" name="Data" displayName="Data" ref="A1:AK87" totalsRowShown="0">
+  <autoFilter ref="A1:AK87" xr:uid="{93166B95-8F57-7249-BAD0-F6F6DB81EEDA}"/>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{20F9E231-C300-0444-AC18-9BA75DF43CD7}" name="Date" dataDxfId="36"/>
     <tableColumn id="35" xr3:uid="{6D5DE1BF-18D0-144B-BD3F-DACE38879478}" name="Stars" dataDxfId="35"/>
@@ -13884,11 +13977,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25124EE0-0CAD-CD49-A20F-54498FB40B76}">
-  <dimension ref="A1:AK86"/>
+  <dimension ref="A1:AK87"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK78" sqref="AK78"/>
+      <selection pane="bottomLeft" activeCell="AJ87" sqref="AJ87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22993,10 +23086,10 @@
       <c r="A86" s="1">
         <v>45664</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B86">
         <v>374</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86">
         <v>132</v>
       </c>
       <c r="D86" s="2">
@@ -23104,6 +23197,123 @@
       <c r="AK86" s="2">
         <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
         <v>1572</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>45712</v>
+      </c>
+      <c r="B87" s="4">
+        <v>383</v>
+      </c>
+      <c r="C87" s="4">
+        <v>132</v>
+      </c>
+      <c r="D87" s="2">
+        <v>118</v>
+      </c>
+      <c r="E87" s="2">
+        <v>300</v>
+      </c>
+      <c r="F87" s="2">
+        <v>249</v>
+      </c>
+      <c r="G87" s="2">
+        <v>5985</v>
+      </c>
+      <c r="H87" s="3">
+        <f>Data[[#This Row],[LoC]]-G86</f>
+        <v>6</v>
+      </c>
+      <c r="I87" s="2">
+        <v>7428</v>
+      </c>
+      <c r="J87" s="2">
+        <v>2034</v>
+      </c>
+      <c r="K87" s="2">
+        <v>567</v>
+      </c>
+      <c r="L87" s="2">
+        <v>326</v>
+      </c>
+      <c r="M87" s="2">
+        <v>153</v>
+      </c>
+      <c r="N87" s="2">
+        <v>60</v>
+      </c>
+      <c r="O87" s="2">
+        <v>15</v>
+      </c>
+      <c r="P87" s="2">
+        <f>SUM(Data[[#This Row],[Shell]:[Bash]])</f>
+        <v>10568</v>
+      </c>
+      <c r="Q87" s="3">
+        <f>Data[[#This Row],[Total]]-P86</f>
+        <v>2</v>
+      </c>
+      <c r="R87" s="2">
+        <v>2276</v>
+      </c>
+      <c r="S87" s="2">
+        <v>4887</v>
+      </c>
+      <c r="T87" s="2">
+        <v>74099</v>
+      </c>
+      <c r="U87" s="2">
+        <v>50700</v>
+      </c>
+      <c r="V87" s="2">
+        <v>10</v>
+      </c>
+      <c r="W87" s="2">
+        <v>6</v>
+      </c>
+      <c r="X87" s="2">
+        <v>305</v>
+      </c>
+      <c r="Y87" s="2">
+        <f>Data[[#This Row],[Open issues]]+Data[[#This Row],[Closed issues]]</f>
+        <v>315</v>
+      </c>
+      <c r="Z87" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA87" s="2">
+        <v>184</v>
+      </c>
+      <c r="AB87" s="2">
+        <f>Data[[#This Row],[Open pull requests]]+Data[[#This Row],[Closed pull requests]]</f>
+        <v>184</v>
+      </c>
+      <c r="AC87" s="2">
+        <v>164</v>
+      </c>
+      <c r="AD87" s="2">
+        <v>136</v>
+      </c>
+      <c r="AE87" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF87" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG87" s="2">
+        <v>295</v>
+      </c>
+      <c r="AH87" s="2">
+        <v>1022</v>
+      </c>
+      <c r="AI87" s="2">
+        <v>7</v>
+      </c>
+      <c r="AJ87" s="2"/>
+      <c r="AK87" s="2">
+        <f>SUM(Data[[#This Row],[Running]:[GH runs]])</f>
+        <v>1324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>